<commit_message>
Boat Enabled - TBS News
Boat Enabled - TBS News
ShieldW Enabled
</commit_message>
<xml_diff>
--- a/System_2.1.3.xlsx
+++ b/System_2.1.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C85CE7-EB1D-45BE-A89B-CA1573BD264B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C3B729-CB65-494E-89AD-39B493A0ED53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="592">
   <si>
     <t>Zone</t>
   </si>
@@ -1812,6 +1812,9 @@
   </si>
   <si>
     <t>ViolationRCA</t>
+  </si>
+  <si>
+    <t>FishW</t>
   </si>
 </sst>
 </file>
@@ -4640,7 +4643,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4658,6 +4660,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5228,7 +5233,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5523,7 +5528,7 @@
   <dimension ref="B1:U28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5691,7 +5696,7 @@
         <v>228</v>
       </c>
       <c r="Q5" s="19">
-        <v>5100</v>
+        <v>5280</v>
       </c>
       <c r="S5" s="539"/>
     </row>
@@ -5849,7 +5854,7 @@
         <v>227</v>
       </c>
       <c r="Q10" s="64">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="S10" s="539"/>
     </row>
@@ -6377,10 +6382,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
-  <dimension ref="A1:X30"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M11" workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+    <sheetView topLeftCell="M11" workbookViewId="0">
+      <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6448,7 +6453,7 @@
     <row r="2" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="559">
         <f ca="1">TODAY()</f>
-        <v>45276</v>
+        <v>45277</v>
       </c>
       <c r="B2" s="561" t="s">
         <v>389</v>
@@ -6498,7 +6503,7 @@
       <c r="Q2" s="547"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S18</f>
@@ -6522,7 +6527,7 @@
       <c r="N3" s="80" t="s">
         <v>282</v>
       </c>
-      <c r="Q3" s="529">
+      <c r="Q3" s="528">
         <f>SUM(X24:X30)</f>
         <v>5</v>
       </c>
@@ -6538,7 +6543,7 @@
         <v>178</v>
       </c>
       <c r="I4" s="554"/>
-      <c r="R4" s="529" t="s">
+      <c r="R4" s="528" t="s">
         <v>585</v>
       </c>
       <c r="T4" s="20">
@@ -6587,14 +6592,14 @@
       <c r="N5" s="80" t="s">
         <v>317</v>
       </c>
-      <c r="S5" s="529" t="s">
+      <c r="S5" s="528" t="s">
         <v>585</v>
       </c>
       <c r="T5" s="20">
         <f>IF((S7-SUM(X2:X10))&lt;0,S7-SUM(X2:X10),0)</f>
         <v>0</v>
       </c>
-      <c r="V5" s="525"/>
+      <c r="V5" s="524"/>
       <c r="W5" s="6"/>
       <c r="X5" s="232">
         <v>0</v>
@@ -6654,7 +6659,7 @@
       <c r="U7" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="V7" s="526">
+      <c r="V7" s="525">
         <v>1</v>
       </c>
       <c r="W7" s="6" t="s">
@@ -6679,7 +6684,7 @@
       <c r="U8" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="V8" s="527">
+      <c r="V8" s="526">
         <v>1</v>
       </c>
       <c r="W8" s="6"/>
@@ -6708,7 +6713,7 @@
       <c r="U9" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="V9" s="527">
+      <c r="V9" s="526">
         <v>1</v>
       </c>
       <c r="X9" s="109"/>
@@ -6724,7 +6729,7 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!S8</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" s="532"/>
       <c r="I10" s="554"/>
@@ -6902,11 +6907,11 @@
       <c r="M15" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="R15" s="529" t="s">
+      <c r="R15" s="528" t="s">
         <v>585</v>
       </c>
       <c r="T15" s="20">
-        <f>IF((R18-SUM(V18:V22))&lt;0,R18-SUM(V18:V22),0)</f>
+        <f>IF((R18-SUM(V18:V23))&lt;0,R18-SUM(V18:V23),0)</f>
         <v>0</v>
       </c>
       <c r="U15" s="6"/>
@@ -6925,7 +6930,7 @@
         <v>44</v>
       </c>
       <c r="L16" s="6"/>
-      <c r="S16" s="529" t="s">
+      <c r="S16" s="528" t="s">
         <v>585</v>
       </c>
       <c r="T16" s="20">
@@ -6935,7 +6940,7 @@
       <c r="U16" s="6"/>
       <c r="V16" s="112"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="244" t="s">
         <v>525</v>
       </c>
@@ -6964,7 +6969,7 @@
       <c r="U17" s="6"/>
       <c r="V17" s="112"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
       <c r="I18" s="554"/>
       <c r="L18" s="16"/>
@@ -6978,7 +6983,7 @@
       </c>
       <c r="R18" s="24">
         <f>5-R26</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S18" s="24">
         <f>5-S26</f>
@@ -6987,7 +6992,7 @@
       <c r="U18" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="V18" s="526">
+      <c r="V18" s="525">
         <v>1</v>
       </c>
       <c r="W18" s="6" t="s">
@@ -6997,7 +7002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I19" s="554"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
@@ -7011,7 +7016,7 @@
       <c r="W19" s="6"/>
       <c r="X19" s="109"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="244" t="s">
         <v>566</v>
       </c>
@@ -7048,8 +7053,9 @@
       </c>
       <c r="W20" s="6"/>
       <c r="X20" s="109"/>
-    </row>
-    <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z20" s="6"/>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I21" s="554"/>
       <c r="M21" s="227" t="s">
         <v>422</v>
@@ -7065,7 +7071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="244" t="s">
         <v>503</v>
       </c>
@@ -7088,7 +7094,7 @@
       <c r="U22" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="V22" s="525">
+      <c r="V22" s="524">
         <v>1</v>
       </c>
       <c r="W22" s="6" t="s">
@@ -7098,7 +7104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
         <v>579</v>
       </c>
@@ -7109,13 +7115,18 @@
         <v>44</v>
       </c>
       <c r="I23" s="554"/>
-      <c r="V23" s="112"/>
+      <c r="U23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="V23" s="24">
+        <v>1</v>
+      </c>
       <c r="W23" s="6"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I24" s="554"/>
       <c r="U24" s="379"/>
-      <c r="V24" s="528">
+      <c r="V24" s="527">
         <v>0</v>
       </c>
       <c r="W24" s="19" t="s">
@@ -7125,7 +7136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="174" t="s">
         <v>142</v>
       </c>
@@ -7156,9 +7167,11 @@
       </c>
       <c r="U25" s="35"/>
       <c r="W25" s="19"/>
-      <c r="X25" s="523"/>
-    </row>
-    <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X25" s="721" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="244" t="s">
         <v>582</v>
       </c>
@@ -7194,7 +7207,7 @@
         <v>44</v>
       </c>
       <c r="R26" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S26" s="24">
         <v>2</v>
@@ -7213,7 +7226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I27" s="554"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
@@ -7234,7 +7247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="176" t="s">
         <v>178</v>
       </c>
@@ -7256,7 +7269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="241" t="s">
         <v>136</v>
       </c>
@@ -7285,23 +7298,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="246" t="s">
         <v>388</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="U30" s="530" t="s">
+      <c r="U30" s="529" t="s">
         <v>587</v>
       </c>
-      <c r="V30" s="721">
+      <c r="V30" s="530">
         <v>0</v>
       </c>
       <c r="W30" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="X30" s="524">
+      <c r="X30" s="523">
         <v>1</v>
       </c>
     </row>
@@ -7470,7 +7483,7 @@
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="626">
         <f ca="1">TODAY()</f>
-        <v>45276</v>
+        <v>45277</v>
       </c>
       <c r="B2" s="628" t="s">
         <v>379</v>
@@ -8008,7 +8021,7 @@
       <c r="D10" s="142"/>
       <c r="E10" s="250">
         <f>Boat!S8</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="584"/>
       <c r="N10" s="470" t="s">
@@ -9069,8 +9082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AN8" sqref="AN8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9152,7 +9165,7 @@
       </c>
       <c r="P1" s="151">
         <f ca="1">TODAY()</f>
-        <v>45276</v>
+        <v>45277</v>
       </c>
       <c r="Q1" s="142"/>
       <c r="R1" s="142"/>
@@ -9209,11 +9222,11 @@
       </c>
       <c r="K2" s="660">
         <f>SUM(K4:K29)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L2" s="662">
         <f>SUM(L4:L29)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M2" s="599">
         <f>SUM(K30:K37)* (-1)</f>
@@ -9255,7 +9268,7 @@
         <v>457</v>
       </c>
       <c r="AA2" s="323" t="s">
-        <v>260</v>
+        <v>591</v>
       </c>
       <c r="AB2" s="72" t="s">
         <v>455</v>
@@ -9315,7 +9328,7 @@
       </c>
       <c r="R3" s="159">
         <f>SUM(R4:R29)</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S3" s="665"/>
       <c r="T3" s="572"/>
@@ -9329,7 +9342,7 @@
       </c>
       <c r="W3" s="187">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9337,15 +9350,15 @@
       </c>
       <c r="Y3" s="66">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" ref="AB3:AK3" si="1">SUM(AB4:AB29)</f>
@@ -9353,7 +9366,7 @@
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" si="1"/>
@@ -9365,7 +9378,7 @@
       </c>
       <c r="AF3" s="66">
         <f>SUM(AF4:AF29)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AG3" s="412">
         <f t="shared" si="1"/>
@@ -9377,15 +9390,15 @@
       </c>
       <c r="AI3" s="100">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AJ3" s="329">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AK3" s="330">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AN3" s="112"/>
     </row>
@@ -9802,7 +9815,7 @@
       </c>
       <c r="S8" s="340">
         <f>R3</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T8" s="17"/>
       <c r="U8" s="348"/>
@@ -9962,11 +9975,11 @@
       </c>
       <c r="J10" s="363"/>
       <c r="K10" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="311">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="667"/>
       <c r="N10" s="20"/>
@@ -9980,7 +9993,7 @@
         <v>1</v>
       </c>
       <c r="R10" s="157">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S10" s="338">
         <v>-2</v>
@@ -9990,46 +10003,46 @@
       <c r="V10" s="346"/>
       <c r="W10" s="190">
         <f>SUM(J10:K10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10" s="314"/>
       <c r="Y10" s="117">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10" s="308">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA10" s="308">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10" s="308">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC10" s="312">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10" s="318"/>
       <c r="AE10" s="314"/>
       <c r="AF10" s="314">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10" s="373"/>
       <c r="AH10" s="158"/>
       <c r="AI10" s="326">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10" s="327">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK10" s="328">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL10" s="6"/>
       <c r="AM10" s="231"/>
@@ -12728,7 +12741,7 @@
       <c r="P1" s="38"/>
       <c r="S1" s="58">
         <f ca="1">TODAY()</f>
-        <v>45276</v>
+        <v>45277</v>
       </c>
       <c r="V1" s="536" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Token Enabled - France 24 F
Token Enabled - France 24 F
Africa 15 - G 639
</commit_message>
<xml_diff>
--- a/System_2.1.3.xlsx
+++ b/System_2.1.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C3B729-CB65-494E-89AD-39B493A0ED53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F42D1CD-DECC-4A17-9D54-B5586F9507AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="593">
   <si>
     <t>Zone</t>
   </si>
@@ -1815,6 +1815,9 @@
   </si>
   <si>
     <t>FishW</t>
+  </si>
+  <si>
+    <t>Africa 15 - G 639</t>
   </si>
 </sst>
 </file>
@@ -3401,7 +3404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="722">
+  <cellXfs count="724">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4643,7 +4646,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4663,6 +4665,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4708,6 +4716,63 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4738,62 +4803,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4819,12 +4989,6 @@
     <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4846,161 +5010,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5044,39 +5085,6 @@
     <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5095,25 +5103,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5191,51 +5220,31 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5581,10 +5590,10 @@
       <c r="I2" s="443" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="534" t="s">
+      <c r="J2" s="535" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="535"/>
+      <c r="K2" s="536"/>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5594,13 +5603,13 @@
       <c r="N2" s="386" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="536" t="s">
+      <c r="O2" s="537" t="s">
         <v>385</v>
       </c>
-      <c r="P2" s="537"/>
-      <c r="Q2" s="537"/>
-      <c r="R2" s="537"/>
-      <c r="S2" s="538" t="s">
+      <c r="P2" s="538"/>
+      <c r="Q2" s="538"/>
+      <c r="R2" s="538"/>
+      <c r="S2" s="539" t="s">
         <v>386</v>
       </c>
       <c r="U2" s="2" t="s">
@@ -5614,7 +5623,7 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="531"/>
+      <c r="D3" s="532"/>
       <c r="E3" s="374"/>
       <c r="F3" s="281" t="s">
         <v>69</v>
@@ -5639,7 +5648,7 @@
       </c>
       <c r="O3" s="6"/>
       <c r="R3" s="6"/>
-      <c r="S3" s="539"/>
+      <c r="S3" s="540"/>
     </row>
     <row r="4" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -5648,7 +5657,7 @@
       <c r="C4" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="D4" s="532"/>
+      <c r="D4" s="533"/>
       <c r="E4" s="61"/>
       <c r="F4" s="396" t="s">
         <v>42</v>
@@ -5665,7 +5674,7 @@
       </c>
       <c r="O4" s="6"/>
       <c r="R4" s="6"/>
-      <c r="S4" s="539"/>
+      <c r="S4" s="540"/>
     </row>
     <row r="5" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -5674,7 +5683,7 @@
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="533"/>
+      <c r="D5" s="534"/>
       <c r="F5" s="401" t="s">
         <v>42</v>
       </c>
@@ -5698,7 +5707,7 @@
       <c r="Q5" s="19">
         <v>5280</v>
       </c>
-      <c r="S5" s="539"/>
+      <c r="S5" s="540"/>
     </row>
     <row r="6" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -5730,7 +5739,7 @@
       </c>
       <c r="P6" s="16"/>
       <c r="Q6" s="6"/>
-      <c r="S6" s="539"/>
+      <c r="S6" s="540"/>
     </row>
     <row r="7" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="219" t="s">
@@ -5760,7 +5769,7 @@
       </c>
       <c r="P7" s="16"/>
       <c r="Q7" s="6"/>
-      <c r="S7" s="539"/>
+      <c r="S7" s="540"/>
     </row>
     <row r="8" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -5788,7 +5797,7 @@
       </c>
       <c r="P8" s="16"/>
       <c r="Q8" s="6"/>
-      <c r="S8" s="539"/>
+      <c r="S8" s="540"/>
     </row>
     <row r="9" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -5821,7 +5830,7 @@
       <c r="O9" s="256" t="s">
         <v>44</v>
       </c>
-      <c r="S9" s="539"/>
+      <c r="S9" s="540"/>
     </row>
     <row r="10" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -5856,7 +5865,7 @@
       <c r="Q10" s="64">
         <v>88</v>
       </c>
-      <c r="S10" s="539"/>
+      <c r="S10" s="540"/>
     </row>
     <row r="11" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -5890,7 +5899,7 @@
       </c>
       <c r="P11" s="16"/>
       <c r="Q11" s="142"/>
-      <c r="S11" s="539"/>
+      <c r="S11" s="540"/>
       <c r="T11" s="23"/>
     </row>
     <row r="12" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5917,7 +5926,7 @@
       </c>
       <c r="P12" s="16"/>
       <c r="Q12" s="142"/>
-      <c r="S12" s="539"/>
+      <c r="S12" s="540"/>
     </row>
     <row r="13" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="271" t="s">
@@ -5951,10 +5960,10 @@
       <c r="N13" s="404" t="s">
         <v>522</v>
       </c>
-      <c r="S13" s="539"/>
+      <c r="S13" s="540"/>
     </row>
     <row r="14" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S14" s="539"/>
+      <c r="S14" s="540"/>
     </row>
     <row r="15" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -5980,17 +5989,17 @@
       <c r="L15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="543">
+      <c r="M15" s="544">
         <v>45275</v>
       </c>
-      <c r="N15" s="531" t="s">
+      <c r="N15" s="532" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="256" t="s">
         <v>44</v>
       </c>
       <c r="R15" s="6"/>
-      <c r="S15" s="539"/>
+      <c r="S15" s="540"/>
     </row>
     <row r="16" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="514" t="s">
@@ -6016,9 +6025,9 @@
       <c r="L16" s="204" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="544"/>
-      <c r="N16" s="532"/>
-      <c r="S16" s="539"/>
+      <c r="M16" s="545"/>
+      <c r="N16" s="533"/>
+      <c r="S16" s="540"/>
     </row>
     <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -6046,15 +6055,15 @@
       <c r="L17" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="545"/>
-      <c r="N17" s="533"/>
+      <c r="M17" s="546"/>
+      <c r="N17" s="534"/>
       <c r="O17" s="256" t="s">
         <v>44</v>
       </c>
-      <c r="S17" s="539"/>
+      <c r="S17" s="540"/>
     </row>
     <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S18" s="539"/>
+      <c r="S18" s="540"/>
     </row>
     <row r="19" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -6082,13 +6091,13 @@
       <c r="L19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="543">
+      <c r="M19" s="544">
         <v>45275</v>
       </c>
       <c r="N19" s="442" t="s">
         <v>522</v>
       </c>
-      <c r="S19" s="539"/>
+      <c r="S19" s="540"/>
     </row>
     <row r="20" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="254" t="s">
@@ -6114,11 +6123,11 @@
       <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="544"/>
+      <c r="M20" s="545"/>
       <c r="N20" s="431" t="s">
         <v>26</v>
       </c>
-      <c r="S20" s="539"/>
+      <c r="S20" s="540"/>
     </row>
     <row r="21" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="254" t="s">
@@ -6144,15 +6153,15 @@
       <c r="L21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="544"/>
+      <c r="M21" s="545"/>
       <c r="N21" s="431" t="s">
         <v>18</v>
       </c>
-      <c r="P21" s="541" t="s">
+      <c r="P21" s="542" t="s">
         <v>226</v>
       </c>
-      <c r="Q21" s="542"/>
-      <c r="S21" s="539"/>
+      <c r="Q21" s="543"/>
+      <c r="S21" s="540"/>
     </row>
     <row r="22" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="288" t="s">
@@ -6178,11 +6187,11 @@
       <c r="L22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="544"/>
+      <c r="M22" s="545"/>
       <c r="N22" s="410" t="s">
         <v>26</v>
       </c>
-      <c r="S22" s="539"/>
+      <c r="S22" s="540"/>
     </row>
     <row r="23" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -6208,11 +6217,11 @@
       <c r="L23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="544"/>
+      <c r="M23" s="545"/>
       <c r="N23" s="61" t="s">
         <v>523</v>
       </c>
-      <c r="S23" s="539"/>
+      <c r="S23" s="540"/>
     </row>
     <row r="24" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
@@ -6238,7 +6247,7 @@
       <c r="L24" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="544"/>
+      <c r="M24" s="545"/>
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
@@ -6246,7 +6255,7 @@
         <v>44</v>
       </c>
       <c r="R24" s="16"/>
-      <c r="S24" s="539"/>
+      <c r="S24" s="540"/>
     </row>
     <row r="25" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
@@ -6272,11 +6281,11 @@
       <c r="L25" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="544"/>
+      <c r="M25" s="545"/>
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="S25" s="539"/>
+      <c r="S25" s="540"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
@@ -6302,11 +6311,11 @@
       <c r="L26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="544"/>
+      <c r="M26" s="545"/>
       <c r="N26" s="61" t="s">
         <v>524</v>
       </c>
-      <c r="S26" s="539"/>
+      <c r="S26" s="540"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="271" t="s">
@@ -6328,9 +6337,9 @@
       <c r="J27" s="439"/>
       <c r="K27" s="440"/>
       <c r="L27" s="441"/>
-      <c r="M27" s="544"/>
+      <c r="M27" s="545"/>
       <c r="N27" s="61"/>
-      <c r="S27" s="539"/>
+      <c r="S27" s="540"/>
     </row>
     <row r="28" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="271" t="s">
@@ -6358,12 +6367,12 @@
       <c r="L28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="545"/>
+      <c r="M28" s="546"/>
       <c r="N28" s="61" t="s">
         <v>524</v>
       </c>
       <c r="R28" s="16"/>
-      <c r="S28" s="540"/>
+      <c r="S28" s="541"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6385,7 +6394,7 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView topLeftCell="M11" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+      <selection activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6412,7 +6421,7 @@
     <col min="20" max="20" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="3.7109375" style="20" customWidth="1"/>
     <col min="23" max="23" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3.85546875" customWidth="1"/>
+    <col min="24" max="24" width="3.85546875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6440,7 +6449,7 @@
       <c r="P1" s="450" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="546" t="s">
+      <c r="Q1" s="566" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6451,32 +6460,32 @@
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="559">
+      <c r="A2" s="550">
         <f ca="1">TODAY()</f>
         <v>45277</v>
       </c>
-      <c r="B2" s="561" t="s">
+      <c r="B2" s="552" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="573" t="s">
+      <c r="C2" s="564" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="563" t="s">
+      <c r="D2" s="554" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="565" t="s">
+      <c r="E2" s="556" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="201" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="571" t="s">
+      <c r="G2" s="562" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="553" t="s">
+      <c r="I2" s="573" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="448" t="s">
@@ -6500,7 +6509,7 @@
       <c r="P2" s="451">
         <v>40</v>
       </c>
-      <c r="Q2" s="547"/>
+      <c r="Q2" s="567"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>8</v>
@@ -6510,40 +6519,40 @@
         <v>4</v>
       </c>
       <c r="V2" s="520"/>
-      <c r="X2" s="56"/>
+      <c r="X2" s="524"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="560"/>
-      <c r="B3" s="562"/>
-      <c r="C3" s="574"/>
-      <c r="D3" s="564"/>
-      <c r="E3" s="566"/>
-      <c r="G3" s="572"/>
+      <c r="A3" s="551"/>
+      <c r="B3" s="553"/>
+      <c r="C3" s="565"/>
+      <c r="D3" s="555"/>
+      <c r="E3" s="557"/>
+      <c r="G3" s="563"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="554"/>
+      <c r="I3" s="574"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
       <c r="N3" s="80" t="s">
         <v>282</v>
       </c>
-      <c r="Q3" s="528">
+      <c r="Q3" s="527">
         <f>SUM(X24:X30)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V3" s="521"/>
-      <c r="X3" s="231"/>
+      <c r="X3" s="525"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="249" t="s">
         <v>390</v>
       </c>
       <c r="B4" s="257"/>
-      <c r="C4" s="567" t="s">
+      <c r="C4" s="558" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="554"/>
-      <c r="R4" s="528" t="s">
+      <c r="I4" s="574"/>
+      <c r="R4" s="527" t="s">
         <v>585</v>
       </c>
       <c r="T4" s="20">
@@ -6551,7 +6560,7 @@
         <v>0</v>
       </c>
       <c r="V4" s="521"/>
-      <c r="X4" s="231"/>
+      <c r="X4" s="525"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="234" t="s">
@@ -6560,7 +6569,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="568"/>
+      <c r="C5" s="559"/>
       <c r="D5" s="235" t="s">
         <v>103</v>
       </c>
@@ -6570,13 +6579,13 @@
       <c r="F5" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="531" t="s">
+      <c r="G5" s="532" t="s">
         <v>276</v>
       </c>
       <c r="H5" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="554"/>
+      <c r="I5" s="574"/>
       <c r="J5" s="449" t="s">
         <v>273</v>
       </c>
@@ -6592,36 +6601,36 @@
       <c r="N5" s="80" t="s">
         <v>317</v>
       </c>
-      <c r="S5" s="528" t="s">
+      <c r="S5" s="527" t="s">
         <v>585</v>
       </c>
       <c r="T5" s="20">
         <f>IF((S7-SUM(X2:X10))&lt;0,S7-SUM(X2:X10),0)</f>
         <v>0</v>
       </c>
-      <c r="V5" s="524"/>
+      <c r="V5" s="523"/>
       <c r="W5" s="6"/>
-      <c r="X5" s="232">
+      <c r="X5" s="523">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="556" t="s">
+      <c r="A6" s="547" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="569"/>
-      <c r="D6" s="570"/>
+      <c r="C6" s="560"/>
+      <c r="D6" s="561"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
-      <c r="G6" s="532"/>
-      <c r="I6" s="554"/>
+      <c r="G6" s="533"/>
+      <c r="I6" s="574"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="557"/>
+      <c r="A7" s="548"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6631,8 +6640,8 @@
       <c r="D7" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="532"/>
-      <c r="I7" s="554"/>
+      <c r="G7" s="533"/>
+      <c r="I7" s="574"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6659,18 +6668,18 @@
       <c r="U7" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="V7" s="525">
+      <c r="V7" s="524">
         <v>1</v>
       </c>
       <c r="W7" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="X7" s="56">
+      <c r="X7" s="524">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="558"/>
+      <c r="A8" s="549"/>
       <c r="B8" s="222" t="s">
         <v>28</v>
       </c>
@@ -6678,17 +6687,17 @@
       <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="532"/>
-      <c r="I8" s="554"/>
+      <c r="G8" s="533"/>
+      <c r="I8" s="574"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="V8" s="526">
+      <c r="V8" s="525">
         <v>1</v>
       </c>
       <c r="W8" s="6"/>
-      <c r="X8" s="109"/>
+      <c r="X8" s="521"/>
     </row>
     <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="244" t="s">
@@ -6703,9 +6712,9 @@
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="532"/>
+      <c r="G9" s="533"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="554"/>
+      <c r="I9" s="574"/>
       <c r="M9" s="19" t="s">
         <v>548</v>
       </c>
@@ -6713,10 +6722,10 @@
       <c r="U9" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="V9" s="526">
-        <v>1</v>
-      </c>
-      <c r="X9" s="109"/>
+      <c r="V9" s="525">
+        <v>1</v>
+      </c>
+      <c r="X9" s="521"/>
     </row>
     <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="245" t="s">
@@ -6731,8 +6740,8 @@
         <f>Boat!S8</f>
         <v>43</v>
       </c>
-      <c r="G10" s="532"/>
-      <c r="I10" s="554"/>
+      <c r="G10" s="533"/>
+      <c r="I10" s="574"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6744,13 +6753,13 @@
       </c>
       <c r="N10" s="80"/>
       <c r="V10" s="521"/>
-      <c r="X10" s="109"/>
+      <c r="X10" s="521"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="531" t="s">
+      <c r="B11" s="532" t="s">
         <v>392</v>
       </c>
       <c r="C11" s="176" t="s">
@@ -6759,8 +6768,8 @@
       <c r="D11" s="229" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="532"/>
-      <c r="I11" s="554"/>
+      <c r="G11" s="533"/>
+      <c r="I11" s="574"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -6786,23 +6795,23 @@
       <c r="S11" s="24">
         <v>2</v>
       </c>
-      <c r="U11" s="548" t="s">
+      <c r="U11" s="568" t="s">
         <v>588</v>
       </c>
-      <c r="V11" s="549"/>
-      <c r="W11" s="549"/>
-      <c r="X11" s="550"/>
+      <c r="V11" s="569"/>
+      <c r="W11" s="569"/>
+      <c r="X11" s="570"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="240" t="s">
         <v>393</v>
       </c>
-      <c r="B12" s="533"/>
+      <c r="B12" s="534"/>
       <c r="E12" s="242">
         <v>3</v>
       </c>
-      <c r="G12" s="532"/>
-      <c r="I12" s="554"/>
+      <c r="G12" s="533"/>
+      <c r="I12" s="574"/>
       <c r="J12" s="24" t="s">
         <v>539</v>
       </c>
@@ -6830,12 +6839,12 @@
       <c r="B13" s="227" t="s">
         <v>330</v>
       </c>
-      <c r="C13" s="531" t="s">
+      <c r="C13" s="532" t="s">
         <v>195</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="G13" s="532"/>
-      <c r="I13" s="554"/>
+      <c r="G13" s="533"/>
+      <c r="I13" s="574"/>
       <c r="J13" s="108" t="s">
         <v>577</v>
       </c>
@@ -6862,7 +6871,7 @@
       <c r="B14" s="178" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="533"/>
+      <c r="C14" s="534"/>
       <c r="D14" s="214" t="s">
         <v>154</v>
       </c>
@@ -6872,11 +6881,11 @@
       <c r="F14" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="G14" s="533"/>
+      <c r="G14" s="534"/>
       <c r="H14" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="554"/>
+      <c r="I14" s="574"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -6894,7 +6903,7 @@
       <c r="H15" s="289">
         <v>0</v>
       </c>
-      <c r="I15" s="554"/>
+      <c r="I15" s="574"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -6907,10 +6916,10 @@
       <c r="M15" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="R15" s="528" t="s">
+      <c r="R15" s="527" t="s">
         <v>585</v>
       </c>
-      <c r="T15" s="20">
+      <c r="T15" s="24">
         <f>IF((R18-SUM(V18:V23))&lt;0,R18-SUM(V18:V23),0)</f>
         <v>0</v>
       </c>
@@ -6925,15 +6934,15 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="554"/>
+      <c r="I16" s="574"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
       <c r="L16" s="6"/>
-      <c r="S16" s="528" t="s">
+      <c r="S16" s="527" t="s">
         <v>585</v>
       </c>
-      <c r="T16" s="20">
+      <c r="T16" s="24">
         <f>IF((S18-SUM(X18:X22))&lt;0,S18-SUM(X18:X22),0)</f>
         <v>0</v>
       </c>
@@ -6959,7 +6968,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="554"/>
+      <c r="I17" s="574"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -6971,13 +6980,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="554"/>
+      <c r="I18" s="574"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="551" t="s">
+      <c r="O18" s="571" t="s">
         <v>540</v>
       </c>
-      <c r="P18" s="552"/>
+      <c r="P18" s="572"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -6992,18 +7001,18 @@
       <c r="U18" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="V18" s="525">
+      <c r="V18" s="524">
         <v>1</v>
       </c>
       <c r="W18" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="X18" s="132">
+      <c r="X18" s="520">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="554"/>
+      <c r="I19" s="574"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7014,7 +7023,7 @@
         <v>1</v>
       </c>
       <c r="W19" s="6"/>
-      <c r="X19" s="109"/>
+      <c r="X19" s="521"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="244" t="s">
@@ -7035,7 +7044,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="554"/>
+      <c r="I20" s="574"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7051,12 +7060,16 @@
       <c r="V20" s="24">
         <v>1</v>
       </c>
-      <c r="W20" s="6"/>
-      <c r="X20" s="109"/>
+      <c r="W20" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="X20" s="521">
+        <v>1</v>
+      </c>
       <c r="Z20" s="6"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="554"/>
+      <c r="I21" s="574"/>
       <c r="M21" s="227" t="s">
         <v>422</v>
       </c>
@@ -7067,9 +7080,7 @@
       <c r="W21" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="X21" s="109">
-        <v>1</v>
-      </c>
+      <c r="X21" s="521"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="244" t="s">
@@ -7090,17 +7101,17 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="554"/>
+      <c r="I22" s="574"/>
       <c r="U22" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="V22" s="524">
+      <c r="V22" s="523">
         <v>1</v>
       </c>
       <c r="W22" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="X22" s="110">
+      <c r="X22" s="530">
         <v>1</v>
       </c>
     </row>
@@ -7114,7 +7125,7 @@
       <c r="E23" s="301" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="554"/>
+      <c r="I23" s="574"/>
       <c r="U23" s="6" t="s">
         <v>74</v>
       </c>
@@ -7124,16 +7135,16 @@
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="554"/>
+      <c r="I24" s="574"/>
       <c r="U24" s="379"/>
-      <c r="V24" s="527">
-        <v>0</v>
+      <c r="V24" s="526">
+        <v>-1</v>
       </c>
       <c r="W24" s="19" t="s">
         <v>513</v>
       </c>
-      <c r="X24" s="19">
-        <v>2</v>
+      <c r="X24" s="24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7152,7 +7163,7 @@
       <c r="H25" s="201" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="554"/>
+      <c r="I25" s="574"/>
       <c r="J25" s="449" t="s">
         <v>274</v>
       </c>
@@ -7167,7 +7178,7 @@
       </c>
       <c r="U25" s="35"/>
       <c r="W25" s="19"/>
-      <c r="X25" s="721" t="s">
+      <c r="X25" s="531" t="s">
         <v>44</v>
       </c>
     </row>
@@ -7192,7 +7203,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="554"/>
+      <c r="I26" s="574"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7222,12 +7233,12 @@
       <c r="W26" s="19" t="s">
         <v>541</v>
       </c>
-      <c r="X26" s="19">
+      <c r="X26" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="554"/>
+      <c r="I27" s="574"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7243,7 +7254,7 @@
       <c r="W27" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="X27" s="19">
+      <c r="X27" s="24">
         <v>0</v>
       </c>
     </row>
@@ -7254,7 +7265,7 @@
       <c r="E28" s="226">
         <v>2</v>
       </c>
-      <c r="I28" s="554"/>
+      <c r="I28" s="574"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7265,7 +7276,7 @@
       <c r="W28" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="X28" s="19">
+      <c r="X28" s="24">
         <v>1</v>
       </c>
     </row>
@@ -7276,7 +7287,7 @@
       <c r="H29" s="201" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="555"/>
+      <c r="I29" s="575"/>
       <c r="J29" s="358"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7289,13 +7300,13 @@
       <c r="T29" s="80"/>
       <c r="U29" s="35"/>
       <c r="V29" s="112">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="W29" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="X29" s="23">
-        <v>1</v>
+      <c r="X29" s="177">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7305,21 +7316,26 @@
       <c r="B30" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="U30" s="529" t="s">
+      <c r="U30" s="528" t="s">
         <v>587</v>
       </c>
-      <c r="V30" s="530">
+      <c r="V30" s="529">
         <v>0</v>
       </c>
       <c r="W30" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="X30" s="523">
+      <c r="X30" s="722">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7331,11 +7347,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7411,7 +7422,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="571" t="s">
+      <c r="I1" s="562" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7447,7 +7458,7 @@
       <c r="X1" s="482" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="617" t="s">
+      <c r="Y1" s="618" t="s">
         <v>555</v>
       </c>
       <c r="Z1" s="458">
@@ -7472,7 +7483,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="454"/>
-      <c r="AN1" s="602"/>
+      <c r="AN1" s="600"/>
       <c r="AO1" s="375" t="s">
         <v>487</v>
       </c>
@@ -7481,23 +7492,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="626">
+      <c r="A2" s="582">
         <f ca="1">TODAY()</f>
         <v>45277</v>
       </c>
-      <c r="B2" s="628" t="s">
+      <c r="B2" s="584" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="573" t="s">
+      <c r="C2" s="564" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="630" t="s">
+      <c r="D2" s="586" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="575" t="s">
+      <c r="E2" s="630" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="583" t="s">
+      <c r="F2" s="605" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="445" t="s">
@@ -7506,15 +7517,15 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="572"/>
+      <c r="I2" s="563"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="577" t="s">
+      <c r="K2" s="632" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="578"/>
-      <c r="M2" s="583" t="s">
+      <c r="L2" s="633"/>
+      <c r="M2" s="605" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
@@ -7526,11 +7537,11 @@
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="573" t="s">
+      <c r="Q2" s="564" t="s">
         <v>144</v>
       </c>
-      <c r="R2" s="531"/>
-      <c r="S2" s="596" t="s">
+      <c r="R2" s="532"/>
+      <c r="S2" s="622" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7540,7 +7551,7 @@
       <c r="X2" s="483" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="618"/>
+      <c r="Y2" s="619"/>
       <c r="Z2" s="459">
         <v>1</v>
       </c>
@@ -7563,15 +7574,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="480"/>
-      <c r="AN2" s="603"/>
+      <c r="AN2" s="601"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="627"/>
-      <c r="B3" s="629"/>
-      <c r="C3" s="574"/>
-      <c r="D3" s="631"/>
-      <c r="E3" s="576"/>
-      <c r="F3" s="584"/>
+      <c r="A3" s="583"/>
+      <c r="B3" s="585"/>
+      <c r="C3" s="565"/>
+      <c r="D3" s="587"/>
+      <c r="E3" s="631"/>
+      <c r="F3" s="606"/>
       <c r="G3" s="446" t="s">
         <v>28</v>
       </c>
@@ -7590,7 +7601,7 @@
       <c r="L3" s="211" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="584"/>
+      <c r="M3" s="606"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
@@ -7598,9 +7609,9 @@
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="574"/>
-      <c r="R3" s="533"/>
-      <c r="S3" s="598"/>
+      <c r="Q3" s="565"/>
+      <c r="R3" s="534"/>
+      <c r="S3" s="623"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7608,7 +7619,7 @@
       <c r="X3" s="483" t="s">
         <v>158</v>
       </c>
-      <c r="Y3" s="618"/>
+      <c r="Y3" s="619"/>
       <c r="Z3" s="460">
         <v>1</v>
       </c>
@@ -7617,7 +7628,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="593" t="s">
+      <c r="AD3" s="621" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="272"/>
@@ -7629,16 +7640,16 @@
       <c r="AK3" s="272"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="480"/>
-      <c r="AN3" s="603"/>
+      <c r="AN3" s="601"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="251" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="642" t="s">
+      <c r="B4" s="598" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="573" t="s">
+      <c r="C4" s="564" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="384" t="s">
@@ -7647,7 +7658,7 @@
       <c r="E4" s="422">
         <v>1</v>
       </c>
-      <c r="F4" s="584"/>
+      <c r="F4" s="606"/>
       <c r="G4" s="427" t="s">
         <v>203</v>
       </c>
@@ -7664,7 +7675,7 @@
         <v>151</v>
       </c>
       <c r="L4" s="214"/>
-      <c r="M4" s="584"/>
+      <c r="M4" s="606"/>
       <c r="N4" s="179" t="s">
         <v>70</v>
       </c>
@@ -7690,12 +7701,12 @@
       <c r="X4" s="483" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="618"/>
+      <c r="Y4" s="619"/>
       <c r="Z4" s="461"/>
       <c r="AA4" s="325"/>
       <c r="AB4" s="219"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="593"/>
+      <c r="AD4" s="621"/>
       <c r="AE4" s="272"/>
       <c r="AF4" s="272"/>
       <c r="AG4" s="16"/>
@@ -7705,33 +7716,33 @@
       <c r="AK4" s="272"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="480"/>
-      <c r="AN4" s="603"/>
+      <c r="AN4" s="601"/>
       <c r="AO4" s="375" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="571" t="s">
+      <c r="A5" s="562" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="643"/>
-      <c r="C5" s="574"/>
+      <c r="B5" s="599"/>
+      <c r="C5" s="565"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="423">
         <v>1</v>
       </c>
-      <c r="F5" s="584"/>
-      <c r="G5" s="634" t="s">
+      <c r="F5" s="606"/>
+      <c r="G5" s="590" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="634"/>
-      <c r="I5" s="634"/>
-      <c r="J5" s="634"/>
-      <c r="K5" s="634"/>
-      <c r="L5" s="635"/>
-      <c r="M5" s="584"/>
+      <c r="H5" s="590"/>
+      <c r="I5" s="590"/>
+      <c r="J5" s="590"/>
+      <c r="K5" s="590"/>
+      <c r="L5" s="591"/>
+      <c r="M5" s="606"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
@@ -7743,7 +7754,7 @@
       <c r="X5" s="483" t="s">
         <v>160</v>
       </c>
-      <c r="Y5" s="618"/>
+      <c r="Y5" s="619"/>
       <c r="Z5" s="461">
         <v>1</v>
       </c>
@@ -7766,23 +7777,23 @@
       <c r="AK5" s="272"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="480"/>
-      <c r="AN5" s="603"/>
+      <c r="AN5" s="601"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="572"/>
-      <c r="B6" s="640" t="s">
+      <c r="A6" s="563"/>
+      <c r="B6" s="596" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="569"/>
-      <c r="D6" s="570"/>
-      <c r="F6" s="584"/>
-      <c r="G6" s="636"/>
-      <c r="H6" s="636"/>
-      <c r="I6" s="636"/>
-      <c r="J6" s="636"/>
-      <c r="K6" s="636"/>
-      <c r="L6" s="637"/>
-      <c r="M6" s="584"/>
+      <c r="C6" s="560"/>
+      <c r="D6" s="561"/>
+      <c r="F6" s="606"/>
+      <c r="G6" s="592"/>
+      <c r="H6" s="592"/>
+      <c r="I6" s="592"/>
+      <c r="J6" s="592"/>
+      <c r="K6" s="592"/>
+      <c r="L6" s="593"/>
+      <c r="M6" s="606"/>
       <c r="O6" s="610"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
@@ -7793,7 +7804,7 @@
       <c r="X6" s="483" t="s">
         <v>161</v>
       </c>
-      <c r="Y6" s="618"/>
+      <c r="Y6" s="619"/>
       <c r="Z6" s="459">
         <v>1</v>
       </c>
@@ -7807,16 +7818,16 @@
       <c r="AF6" s="272"/>
       <c r="AG6" s="272"/>
       <c r="AH6" s="272"/>
-      <c r="AI6" s="592"/>
+      <c r="AI6" s="615"/>
       <c r="AJ6" s="493" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="592" t="s">
+      <c r="AK6" s="615" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="272"/>
       <c r="AM6" s="480"/>
-      <c r="AN6" s="603"/>
+      <c r="AN6" s="601"/>
       <c r="AO6" s="375" t="s">
         <v>488</v>
       </c>
@@ -7825,7 +7836,7 @@
       <c r="A7" s="245" t="s">
         <v>552</v>
       </c>
-      <c r="B7" s="641"/>
+      <c r="B7" s="597"/>
       <c r="C7" s="212" t="s">
         <v>383</v>
       </c>
@@ -7835,7 +7846,7 @@
       <c r="E7" s="281">
         <v>3</v>
       </c>
-      <c r="F7" s="584"/>
+      <c r="F7" s="606"/>
       <c r="G7" s="447">
         <v>0</v>
       </c>
@@ -7848,13 +7859,13 @@
       <c r="J7" s="30">
         <v>0</v>
       </c>
-      <c r="K7" s="531">
+      <c r="K7" s="532">
         <v>1</v>
       </c>
       <c r="L7" s="222">
         <v>0</v>
       </c>
-      <c r="M7" s="584"/>
+      <c r="M7" s="606"/>
       <c r="O7" s="610"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
@@ -7869,7 +7880,7 @@
       <c r="X7" s="483" t="s">
         <v>162</v>
       </c>
-      <c r="Y7" s="618"/>
+      <c r="Y7" s="619"/>
       <c r="Z7" s="459">
         <v>1</v>
       </c>
@@ -7879,18 +7890,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="272"/>
       <c r="AF7" s="272"/>
-      <c r="AG7" s="593" t="s">
+      <c r="AG7" s="621" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="272"/>
-      <c r="AI7" s="592"/>
+      <c r="AI7" s="615"/>
       <c r="AJ7" s="272"/>
-      <c r="AK7" s="592"/>
+      <c r="AK7" s="615"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="480"/>
-      <c r="AN7" s="603"/>
+      <c r="AN7" s="601"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -7907,21 +7918,21 @@
         <f>SUM(G7:N9)</f>
         <v>16</v>
       </c>
-      <c r="F8" s="584"/>
-      <c r="G8" s="635">
-        <v>0</v>
-      </c>
-      <c r="H8" s="632" t="s">
+      <c r="F8" s="606"/>
+      <c r="G8" s="591">
+        <v>0</v>
+      </c>
+      <c r="H8" s="588" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="531"/>
-      <c r="J8" s="632" t="s">
+      <c r="I8" s="532"/>
+      <c r="J8" s="588" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="638"/>
-      <c r="L8" s="594"/>
+      <c r="K8" s="594"/>
+      <c r="L8" s="624"/>
       <c r="M8" s="607"/>
-      <c r="N8" s="599">
+      <c r="N8" s="627">
         <f>N5+N11</f>
         <v>15</v>
       </c>
@@ -7935,7 +7946,7 @@
       <c r="X8" s="483" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="618"/>
+      <c r="Y8" s="619"/>
       <c r="Z8" s="461"/>
       <c r="AA8" s="325"/>
       <c r="AB8" s="219"/>
@@ -7943,14 +7954,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="272"/>
       <c r="AF8" s="272"/>
-      <c r="AG8" s="593"/>
+      <c r="AG8" s="621"/>
       <c r="AH8" s="272"/>
-      <c r="AI8" s="592"/>
+      <c r="AI8" s="615"/>
       <c r="AJ8" s="272"/>
       <c r="AK8" s="272"/>
       <c r="AL8" s="272"/>
       <c r="AM8" s="480"/>
-      <c r="AN8" s="603"/>
+      <c r="AN8" s="601"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="245" t="s">
@@ -7965,17 +7976,17 @@
       <c r="D9" s="385" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="584"/>
-      <c r="G9" s="637"/>
-      <c r="H9" s="633"/>
-      <c r="I9" s="533"/>
-      <c r="J9" s="633"/>
-      <c r="K9" s="639"/>
-      <c r="L9" s="595"/>
+      <c r="F9" s="606"/>
+      <c r="G9" s="593"/>
+      <c r="H9" s="589"/>
+      <c r="I9" s="534"/>
+      <c r="J9" s="589"/>
+      <c r="K9" s="595"/>
+      <c r="L9" s="625"/>
       <c r="M9" s="608"/>
-      <c r="N9" s="600"/>
+      <c r="N9" s="628"/>
       <c r="O9" s="611"/>
-      <c r="S9" s="596" t="s">
+      <c r="S9" s="622" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -7987,7 +7998,7 @@
       <c r="X9" s="483" t="s">
         <v>164</v>
       </c>
-      <c r="Y9" s="618"/>
+      <c r="Y9" s="619"/>
       <c r="Z9" s="462"/>
       <c r="AA9" s="325"/>
       <c r="AB9" s="219"/>
@@ -7997,16 +8008,16 @@
       </c>
       <c r="AE9" s="272"/>
       <c r="AF9" s="272"/>
-      <c r="AG9" s="593"/>
+      <c r="AG9" s="621"/>
       <c r="AH9" s="272"/>
-      <c r="AI9" s="592"/>
+      <c r="AI9" s="615"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="592" t="s">
+      <c r="AK9" s="615" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="272"/>
       <c r="AM9" s="480"/>
-      <c r="AN9" s="603"/>
+      <c r="AN9" s="601"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8023,11 +8034,11 @@
         <f>Boat!S8</f>
         <v>43</v>
       </c>
-      <c r="F10" s="584"/>
+      <c r="F10" s="606"/>
       <c r="N10" s="470" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="586" t="s">
+      <c r="O10" s="639" t="s">
         <v>103</v>
       </c>
       <c r="P10" s="612" t="s">
@@ -8036,7 +8047,7 @@
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="597"/>
+      <c r="S10" s="626"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8048,7 +8059,7 @@
       <c r="X10" s="483" t="s">
         <v>165</v>
       </c>
-      <c r="Y10" s="618"/>
+      <c r="Y10" s="619"/>
       <c r="Z10" s="461">
         <v>0</v>
       </c>
@@ -8066,16 +8077,16 @@
       <c r="AF10" s="251" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="593"/>
+      <c r="AG10" s="621"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="592"/>
+      <c r="AI10" s="615"/>
       <c r="AJ10" s="272"/>
-      <c r="AK10" s="592"/>
+      <c r="AK10" s="615"/>
       <c r="AL10" s="272"/>
       <c r="AM10" s="494" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="603"/>
+      <c r="AN10" s="601"/>
       <c r="AO10" s="214" t="s">
         <v>95</v>
       </c>
@@ -8084,7 +8095,7 @@
       <c r="A11" s="236" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="531" t="s">
+      <c r="B11" s="532" t="s">
         <v>288</v>
       </c>
       <c r="C11" s="509" t="s">
@@ -8093,18 +8104,18 @@
       <c r="D11" s="175" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="584"/>
+      <c r="F11" s="606"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="587"/>
+      <c r="O11" s="640"/>
       <c r="P11" s="613"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="597"/>
+      <c r="S11" s="626"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8114,7 +8125,7 @@
       <c r="X11" s="483" t="s">
         <v>166</v>
       </c>
-      <c r="Y11" s="618"/>
+      <c r="Y11" s="619"/>
       <c r="Z11" s="461"/>
       <c r="AA11" s="325">
         <v>1</v>
@@ -8128,14 +8139,14 @@
       <c r="AF11" s="272" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="593"/>
+      <c r="AG11" s="621"/>
       <c r="AH11" s="272"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="272"/>
       <c r="AK11" s="272"/>
       <c r="AL11" s="272"/>
       <c r="AM11" s="480"/>
-      <c r="AN11" s="603"/>
+      <c r="AN11" s="601"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8144,7 +8155,7 @@
       <c r="A12" s="240" t="s">
         <v>393</v>
       </c>
-      <c r="B12" s="533"/>
+      <c r="B12" s="534"/>
       <c r="C12" s="510" t="s">
         <v>394</v>
       </c>
@@ -8154,25 +8165,25 @@
       <c r="E12" s="237">
         <v>3</v>
       </c>
-      <c r="F12" s="584"/>
+      <c r="F12" s="606"/>
       <c r="G12" s="374" t="s">
         <v>411</v>
       </c>
-      <c r="H12" s="536" t="s">
+      <c r="H12" s="537" t="s">
         <v>447</v>
       </c>
-      <c r="I12" s="537"/>
-      <c r="J12" s="537"/>
-      <c r="K12" s="591"/>
+      <c r="I12" s="538"/>
+      <c r="J12" s="538"/>
+      <c r="K12" s="644"/>
       <c r="L12" s="213"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
-      <c r="O12" s="587"/>
+      <c r="O12" s="640"/>
       <c r="P12" s="613"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="598"/>
+      <c r="S12" s="623"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8182,7 +8193,7 @@
       <c r="X12" s="483" t="s">
         <v>167</v>
       </c>
-      <c r="Y12" s="618"/>
+      <c r="Y12" s="619"/>
       <c r="Z12" s="459">
         <v>1</v>
       </c>
@@ -8193,16 +8204,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="601" t="s">
+      <c r="AD12" s="629" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="493" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="593" t="s">
+      <c r="AF12" s="621" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="593"/>
+      <c r="AG12" s="621"/>
       <c r="AH12" s="251" t="s">
         <v>264</v>
       </c>
@@ -8212,10 +8223,10 @@
       <c r="AJ12" s="272"/>
       <c r="AK12" s="272"/>
       <c r="AL12" s="272"/>
-      <c r="AM12" s="615" t="s">
+      <c r="AM12" s="616" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="603"/>
+      <c r="AN12" s="601"/>
       <c r="AO12" s="375" t="s">
         <v>97</v>
       </c>
@@ -8227,16 +8238,16 @@
       <c r="E13" s="500">
         <v>-3</v>
       </c>
-      <c r="F13" s="584"/>
-      <c r="G13" s="537" t="s">
+      <c r="F13" s="606"/>
+      <c r="G13" s="538" t="s">
         <v>448</v>
       </c>
-      <c r="H13" s="537"/>
-      <c r="I13" s="537"/>
-      <c r="J13" s="591"/>
+      <c r="H13" s="538"/>
+      <c r="I13" s="538"/>
+      <c r="J13" s="644"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="587"/>
+      <c r="O13" s="640"/>
       <c r="P13" s="614"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
@@ -8247,7 +8258,7 @@
       <c r="X13" s="483" t="s">
         <v>168</v>
       </c>
-      <c r="Y13" s="618"/>
+      <c r="Y13" s="619"/>
       <c r="Z13" s="459">
         <v>1</v>
       </c>
@@ -8258,8 +8269,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="601"/>
-      <c r="AF13" s="593"/>
+      <c r="AD13" s="629"/>
+      <c r="AF13" s="621"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="251" t="s">
         <v>314</v>
@@ -8270,8 +8281,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="272"/>
       <c r="AL13" s="272"/>
-      <c r="AM13" s="615"/>
-      <c r="AN13" s="603"/>
+      <c r="AM13" s="616"/>
+      <c r="AN13" s="601"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="502"/>
@@ -8279,18 +8290,18 @@
       <c r="C14" s="511"/>
       <c r="D14" s="504"/>
       <c r="E14" s="505"/>
-      <c r="F14" s="584"/>
-      <c r="G14" s="537" t="s">
+      <c r="F14" s="606"/>
+      <c r="G14" s="538" t="s">
         <v>447</v>
       </c>
-      <c r="H14" s="537"/>
-      <c r="I14" s="537"/>
-      <c r="J14" s="591"/>
+      <c r="H14" s="538"/>
+      <c r="I14" s="538"/>
+      <c r="J14" s="644"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="587"/>
+      <c r="O14" s="640"/>
       <c r="Q14" s="61" t="s">
         <v>559</v>
       </c>
@@ -8304,34 +8315,34 @@
       <c r="X14" s="483" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="618"/>
+      <c r="Y14" s="619"/>
       <c r="Z14" s="459">
         <v>1</v>
       </c>
       <c r="AA14" s="325"/>
       <c r="AB14" s="219"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="601"/>
+      <c r="AD14" s="629"/>
       <c r="AE14" s="272"/>
-      <c r="AF14" s="593"/>
+      <c r="AF14" s="621"/>
       <c r="AG14" s="272"/>
       <c r="AH14" s="272"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="272"/>
       <c r="AK14" s="272"/>
       <c r="AL14" s="272"/>
-      <c r="AM14" s="615"/>
-      <c r="AN14" s="603"/>
+      <c r="AM14" s="616"/>
+      <c r="AN14" s="601"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="501" t="s">
         <v>525</v>
       </c>
-      <c r="C15" s="531" t="s">
+      <c r="C15" s="532" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="584"/>
-      <c r="O15" s="587"/>
+      <c r="F15" s="606"/>
+      <c r="O15" s="640"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8344,7 +8355,7 @@
       <c r="X15" s="483" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="618"/>
+      <c r="Y15" s="619"/>
       <c r="Z15" s="461">
         <v>1</v>
       </c>
@@ -8353,8 +8364,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="601"/>
-      <c r="AF15" s="593"/>
+      <c r="AD15" s="629"/>
+      <c r="AF15" s="621"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="251" t="s">
         <v>466</v>
@@ -8367,8 +8378,8 @@
       </c>
       <c r="AK15" s="272"/>
       <c r="AL15" s="272"/>
-      <c r="AM15" s="615"/>
-      <c r="AN15" s="603"/>
+      <c r="AM15" s="616"/>
+      <c r="AN15" s="601"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8383,20 +8394,20 @@
       <c r="B16" s="21" t="s">
         <v>417</v>
       </c>
-      <c r="C16" s="533"/>
+      <c r="C16" s="534"/>
       <c r="D16" s="61" t="s">
         <v>511</v>
       </c>
       <c r="E16" s="237">
         <v>1</v>
       </c>
-      <c r="F16" s="584"/>
+      <c r="F16" s="606"/>
       <c r="G16" s="374" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="587"/>
+      <c r="O16" s="640"/>
       <c r="R16" s="487" t="s">
         <v>185</v>
       </c>
@@ -8407,7 +8418,7 @@
       <c r="X16" s="483" t="s">
         <v>171</v>
       </c>
-      <c r="Y16" s="618"/>
+      <c r="Y16" s="619"/>
       <c r="Z16" s="459">
         <v>1</v>
       </c>
@@ -8428,18 +8439,18 @@
       <c r="AM16" s="480" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="603"/>
+      <c r="AN16" s="601"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="584"/>
+      <c r="F17" s="606"/>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="587"/>
+      <c r="O17" s="640"/>
       <c r="Q17" s="21" t="s">
         <v>557</v>
       </c>
@@ -8459,7 +8470,7 @@
       <c r="X17" s="483" t="s">
         <v>172</v>
       </c>
-      <c r="Y17" s="618"/>
+      <c r="Y17" s="619"/>
       <c r="Z17" s="461"/>
       <c r="AA17" s="325"/>
       <c r="AB17" s="219"/>
@@ -8484,7 +8495,7 @@
       <c r="AK17" s="272"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="480"/>
-      <c r="AN17" s="603"/>
+      <c r="AN17" s="601"/>
       <c r="AO17" s="214" t="s">
         <v>516</v>
       </c>
@@ -8508,21 +8519,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="584"/>
+      <c r="F18" s="606"/>
       <c r="G18" s="374" t="s">
         <v>554</v>
       </c>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="587"/>
+      <c r="O18" s="640"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="579" t="s">
+      <c r="R18" s="634" t="s">
         <v>562</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="623" t="s">
+      <c r="U18" s="579" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8532,7 +8543,7 @@
       <c r="X18" s="483" t="s">
         <v>173</v>
       </c>
-      <c r="Y18" s="618"/>
+      <c r="Y18" s="619"/>
       <c r="Z18" s="461">
         <v>1</v>
       </c>
@@ -8543,37 +8554,37 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="272"/>
-      <c r="AF18" s="592" t="s">
+      <c r="AF18" s="615" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="272"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="616" t="s">
+      <c r="AJ18" s="617" t="s">
         <v>322</v>
       </c>
       <c r="AK18" s="272"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="480"/>
-      <c r="AN18" s="603"/>
+      <c r="AN18" s="601"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="584"/>
-      <c r="O19" s="587"/>
-      <c r="R19" s="580"/>
+      <c r="F19" s="606"/>
+      <c r="O19" s="640"/>
+      <c r="R19" s="635"/>
       <c r="S19" s="30" t="s">
         <v>560</v>
       </c>
-      <c r="U19" s="624"/>
+      <c r="U19" s="580"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="483" t="s">
         <v>174</v>
       </c>
-      <c r="Y19" s="618"/>
+      <c r="Y19" s="619"/>
       <c r="Z19" s="459">
         <v>1</v>
       </c>
@@ -8582,17 +8593,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="272"/>
-      <c r="AF19" s="592"/>
+      <c r="AF19" s="615"/>
       <c r="AG19" s="272"/>
       <c r="AH19" s="272"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="616"/>
+      <c r="AJ19" s="617"/>
       <c r="AK19" s="512" t="s">
         <v>256</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="480"/>
-      <c r="AN19" s="603"/>
+      <c r="AN19" s="601"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8613,23 +8624,23 @@
       <c r="E20" s="489">
         <v>-1</v>
       </c>
-      <c r="F20" s="584"/>
+      <c r="F20" s="606"/>
       <c r="G20" s="374" t="s">
         <v>509</v>
       </c>
-      <c r="O20" s="587"/>
-      <c r="Q20" s="589" t="s">
+      <c r="O20" s="640"/>
+      <c r="Q20" s="642" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="456" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="625"/>
+      <c r="U20" s="581"/>
       <c r="W20" s="457"/>
       <c r="X20" s="484" t="s">
         <v>175</v>
       </c>
-      <c r="Y20" s="618"/>
+      <c r="Y20" s="619"/>
       <c r="Z20" s="463">
         <v>1</v>
       </c>
@@ -8654,7 +8665,7 @@
       <c r="AM20" s="427" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="603"/>
+      <c r="AN20" s="601"/>
       <c r="AO20" s="375" t="s">
         <v>478</v>
       </c>
@@ -8678,19 +8689,19 @@
       <c r="E21" s="281">
         <v>1</v>
       </c>
-      <c r="F21" s="584"/>
-      <c r="O21" s="587"/>
-      <c r="Q21" s="590"/>
+      <c r="F21" s="606"/>
+      <c r="O21" s="640"/>
+      <c r="Q21" s="643"/>
       <c r="T21" s="474"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="620"/>
+      <c r="V21" s="576"/>
       <c r="W21" s="478" t="s">
         <v>176</v>
       </c>
       <c r="X21" s="481" t="s">
         <v>187</v>
       </c>
-      <c r="Y21" s="618"/>
+      <c r="Y21" s="619"/>
       <c r="Z21" s="497">
         <v>3</v>
       </c>
@@ -8721,14 +8732,14 @@
       <c r="AM21" s="480" t="s">
         <v>572</v>
       </c>
-      <c r="AN21" s="603"/>
+      <c r="AN21" s="601"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="584"/>
+      <c r="F22" s="606"/>
       <c r="G22" s="374" t="s">
         <v>507</v>
       </c>
-      <c r="O22" s="587"/>
+      <c r="O22" s="640"/>
       <c r="R22" s="486" t="s">
         <v>44</v>
       </c>
@@ -8736,14 +8747,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="621"/>
+      <c r="V22" s="577"/>
       <c r="W22" s="478" t="s">
         <v>176</v>
       </c>
       <c r="X22" s="481" t="s">
         <v>188</v>
       </c>
-      <c r="Y22" s="618"/>
+      <c r="Y22" s="619"/>
       <c r="Z22" s="467"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="467"/>
@@ -8754,7 +8765,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="592" t="s">
+      <c r="AJ22" s="615" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="272"/>
@@ -8762,7 +8773,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="318"/>
-      <c r="AN22" s="603"/>
+      <c r="AN22" s="601"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="244" t="s">
@@ -8780,21 +8791,21 @@
       <c r="E23" s="238">
         <v>1</v>
       </c>
-      <c r="F23" s="584"/>
-      <c r="O23" s="587"/>
-      <c r="Q23" s="589" t="s">
+      <c r="F23" s="606"/>
+      <c r="O23" s="640"/>
+      <c r="Q23" s="642" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="472" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="621"/>
+      <c r="V23" s="577"/>
       <c r="W23" s="148"/>
       <c r="X23" s="481" t="s">
         <v>189</v>
       </c>
-      <c r="Y23" s="618"/>
+      <c r="Y23" s="619"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="467"/>
@@ -8805,13 +8816,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="592"/>
+      <c r="AJ23" s="615"/>
       <c r="AK23" s="272"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="318"/>
-      <c r="AN23" s="603"/>
+      <c r="AN23" s="601"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="492" t="s">
@@ -8829,22 +8840,22 @@
       <c r="E24" s="488">
         <v>1</v>
       </c>
-      <c r="F24" s="584"/>
+      <c r="F24" s="606"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
-      <c r="O24" s="587"/>
-      <c r="Q24" s="590"/>
+      <c r="O24" s="640"/>
+      <c r="Q24" s="643"/>
       <c r="T24" s="17"/>
       <c r="U24" s="240" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="621"/>
+      <c r="V24" s="577"/>
       <c r="W24" s="148"/>
       <c r="X24" s="481" t="s">
         <v>186</v>
       </c>
-      <c r="Y24" s="618"/>
+      <c r="Y24" s="619"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="467"/>
@@ -8863,11 +8874,11 @@
         <v>481</v>
       </c>
       <c r="AM24" s="318"/>
-      <c r="AN24" s="603"/>
+      <c r="AN24" s="601"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="584"/>
-      <c r="O25" s="587"/>
+      <c r="F25" s="606"/>
+      <c r="O25" s="640"/>
       <c r="P25" s="214" t="s">
         <v>285</v>
       </c>
@@ -8880,12 +8891,12 @@
       <c r="U25" s="452" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="622"/>
+      <c r="V25" s="578"/>
       <c r="W25" s="148"/>
       <c r="X25" s="481" t="s">
         <v>190</v>
       </c>
-      <c r="Y25" s="618"/>
+      <c r="Y25" s="619"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="467"/>
@@ -8902,7 +8913,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="318"/>
-      <c r="AN25" s="603"/>
+      <c r="AN25" s="601"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="244" t="s">
@@ -8920,16 +8931,16 @@
       <c r="E26" s="424">
         <v>1</v>
       </c>
-      <c r="F26" s="584"/>
+      <c r="F26" s="606"/>
       <c r="G26" s="374" t="s">
         <v>505</v>
       </c>
-      <c r="O26" s="587"/>
-      <c r="P26" s="605" t="s">
+      <c r="O26" s="640"/>
+      <c r="P26" s="603" t="s">
         <v>549</v>
       </c>
-      <c r="Q26" s="606"/>
-      <c r="R26" s="581" t="s">
+      <c r="Q26" s="604"/>
+      <c r="R26" s="636" t="s">
         <v>561</v>
       </c>
       <c r="T26" s="183"/>
@@ -8941,7 +8952,7 @@
       <c r="X26" s="481" t="s">
         <v>182</v>
       </c>
-      <c r="Y26" s="618"/>
+      <c r="Y26" s="619"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="467"/>
@@ -8968,7 +8979,7 @@
       <c r="AM26" s="494" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="603"/>
+      <c r="AN26" s="601"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8980,12 +8991,12 @@
       <c r="E27" s="281" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="585"/>
+      <c r="F27" s="638"/>
       <c r="G27" s="61" t="s">
         <v>571</v>
       </c>
-      <c r="O27" s="588"/>
-      <c r="R27" s="582"/>
+      <c r="O27" s="641"/>
+      <c r="R27" s="637"/>
       <c r="S27" s="473" t="s">
         <v>54</v>
       </c>
@@ -8998,7 +9009,7 @@
       <c r="X27" s="481" t="s">
         <v>556</v>
       </c>
-      <c r="Y27" s="619"/>
+      <c r="Y27" s="620"/>
       <c r="Z27" s="163"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="468"/>
@@ -9015,10 +9026,48 @@
       <c r="AM27" s="427" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="604"/>
+      <c r="AN27" s="602"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9035,44 +9084,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9082,8 +9093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView tabSelected="1" topLeftCell="P9" workbookViewId="0">
+      <selection activeCell="AM14" sqref="AM14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9119,7 +9130,7 @@
     <col min="36" max="36" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9170,16 +9181,16 @@
       <c r="Q1" s="142"/>
       <c r="R1" s="142"/>
       <c r="S1" s="6"/>
-      <c r="T1" s="571" t="s">
+      <c r="T1" s="562" t="s">
         <v>236</v>
       </c>
-      <c r="U1" s="648" t="s">
+      <c r="U1" s="660" t="s">
         <v>237</v>
       </c>
-      <c r="V1" s="650" t="s">
+      <c r="V1" s="662" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="651"/>
+      <c r="W1" s="663"/>
       <c r="X1" s="324">
         <f>68-(S8+W3+V3+Q3)</f>
         <v>0</v>
@@ -9195,40 +9206,40 @@
       <c r="AB1" s="320" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="652" t="s">
+      <c r="AC1" s="664" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="653"/>
-      <c r="AE1" s="654"/>
-      <c r="AF1" s="655" t="s">
+      <c r="AD1" s="665"/>
+      <c r="AE1" s="666"/>
+      <c r="AF1" s="667" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="656"/>
-      <c r="AH1" s="657"/>
-      <c r="AI1" s="644" t="s">
+      <c r="AG1" s="668"/>
+      <c r="AH1" s="669"/>
+      <c r="AI1" s="656" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="645"/>
-      <c r="AK1" s="646"/>
+      <c r="AJ1" s="657"/>
+      <c r="AK1" s="658"/>
       <c r="AN1" s="112"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="658">
+      <c r="J2" s="648">
         <f>SUM(J5:J30)</f>
         <v>2</v>
       </c>
-      <c r="K2" s="660">
+      <c r="K2" s="650">
         <f>SUM(K4:K29)</f>
         <v>4</v>
       </c>
-      <c r="L2" s="662">
+      <c r="L2" s="652">
         <f>SUM(L4:L29)</f>
         <v>7</v>
       </c>
-      <c r="M2" s="599">
+      <c r="M2" s="627">
         <f>SUM(K30:K37)* (-1)</f>
         <v>3</v>
       </c>
@@ -9247,11 +9258,11 @@
       <c r="R2" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="S2" s="664" t="s">
+      <c r="S2" s="654" t="s">
         <v>239</v>
       </c>
-      <c r="T2" s="647"/>
-      <c r="U2" s="649"/>
+      <c r="T2" s="659"/>
+      <c r="U2" s="661"/>
       <c r="V2" s="61" t="s">
         <v>456</v>
       </c>
@@ -9311,10 +9322,10 @@
       </c>
     </row>
     <row r="3" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J3" s="659"/>
-      <c r="K3" s="661"/>
-      <c r="L3" s="663"/>
-      <c r="M3" s="600"/>
+      <c r="J3" s="649"/>
+      <c r="K3" s="651"/>
+      <c r="L3" s="653"/>
+      <c r="M3" s="628"/>
       <c r="N3" s="177">
         <f>(J2+K2)-W3</f>
         <v>0</v>
@@ -9330,8 +9341,8 @@
         <f>SUM(R4:R29)</f>
         <v>43</v>
       </c>
-      <c r="S3" s="665"/>
-      <c r="T3" s="572"/>
+      <c r="S3" s="655"/>
+      <c r="T3" s="563"/>
       <c r="U3" s="331">
         <f>R3+V3+W3+Q3</f>
         <v>68</v>
@@ -9432,7 +9443,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="666" t="s">
+      <c r="M4" s="645" t="s">
         <v>200</v>
       </c>
       <c r="N4" s="20"/>
@@ -9515,7 +9526,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="667"/>
+      <c r="M5" s="646"/>
       <c r="N5" s="20"/>
       <c r="O5" s="2" t="s">
         <v>347</v>
@@ -9603,7 +9614,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="667"/>
+      <c r="M6" s="646"/>
       <c r="N6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9693,7 +9704,7 @@
         <f t="shared" ref="L7:L37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="M7" s="667"/>
+      <c r="M7" s="646"/>
       <c r="N7" s="20"/>
       <c r="O7" s="2" t="s">
         <v>342</v>
@@ -9797,7 +9808,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M8" s="667"/>
+      <c r="M8" s="646"/>
       <c r="N8" s="21" t="s">
         <v>238</v>
       </c>
@@ -9883,7 +9894,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M9" s="667"/>
+      <c r="M9" s="646"/>
       <c r="N9" s="21" t="s">
         <v>342</v>
       </c>
@@ -9981,7 +9992,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M10" s="667"/>
+      <c r="M10" s="646"/>
       <c r="N10" s="20"/>
       <c r="O10" s="2" t="s">
         <v>347</v>
@@ -10060,7 +10071,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M11" s="667"/>
+      <c r="M11" s="646"/>
       <c r="N11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10122,7 +10133,7 @@
       <c r="AN11" s="112"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="635" t="s">
+      <c r="A12" s="591" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10131,7 +10142,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="589" t="s">
+      <c r="E12" s="642" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="277">
@@ -10151,7 +10162,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M12" s="667"/>
+      <c r="M12" s="646"/>
       <c r="N12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10225,14 +10236,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="637"/>
+      <c r="A13" s="593"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="590"/>
+      <c r="E13" s="643"/>
       <c r="F13" s="177">
         <v>0</v>
       </c>
@@ -10253,7 +10264,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M13" s="667"/>
+      <c r="M13" s="646"/>
       <c r="N13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10328,7 +10339,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M14" s="667"/>
+      <c r="M14" s="646"/>
       <c r="N14" s="20"/>
       <c r="O14" s="210" t="s">
         <v>346</v>
@@ -10396,7 +10407,9 @@
       <c r="AL14" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="AM14" s="19"/>
+      <c r="AM14" s="723" t="s">
+        <v>592</v>
+      </c>
       <c r="AN14" s="112" t="s">
         <v>516</v>
       </c>
@@ -10423,7 +10436,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M15" s="667"/>
+      <c r="M15" s="646"/>
       <c r="N15" s="20"/>
       <c r="O15" s="210" t="s">
         <v>346</v>
@@ -10508,7 +10521,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M16" s="667"/>
+      <c r="M16" s="646"/>
       <c r="N16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10604,7 +10617,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M17" s="667"/>
+      <c r="M17" s="646"/>
       <c r="N17" s="20"/>
       <c r="O17" s="2" t="s">
         <v>348</v>
@@ -10687,7 +10700,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M18" s="667"/>
+      <c r="M18" s="646"/>
       <c r="N18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10772,7 +10785,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M19" s="667"/>
+      <c r="M19" s="646"/>
       <c r="N19" s="20"/>
       <c r="O19" s="2" t="s">
         <v>341</v>
@@ -10867,11 +10880,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M20" s="668"/>
-      <c r="N20" s="536" t="s">
+      <c r="M20" s="647"/>
+      <c r="N20" s="537" t="s">
         <v>342</v>
       </c>
-      <c r="O20" s="591"/>
+      <c r="O20" s="644"/>
       <c r="P20" s="334" t="s">
         <v>86</v>
       </c>
@@ -11116,7 +11129,7 @@
       <c r="AN22" s="112"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="642" t="s">
+      <c r="E23" s="598" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="185">
@@ -11202,7 +11215,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="643"/>
+      <c r="E24" s="599"/>
       <c r="F24" s="177"/>
       <c r="I24" s="430" t="s">
         <v>301</v>
@@ -11217,10 +11230,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="N24" s="536" t="s">
+      <c r="N24" s="537" t="s">
         <v>342</v>
       </c>
-      <c r="O24" s="591"/>
+      <c r="O24" s="644"/>
       <c r="P24" s="334" t="s">
         <v>254</v>
       </c>
@@ -12297,23 +12310,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="S2:S3"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="N20:O20"/>
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="N24:O24"/>
     <mergeCell ref="M4:M20"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12347,15 +12360,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="536" t="s">
+      <c r="B1" s="537" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="591"/>
+      <c r="C1" s="644"/>
       <c r="D1" s="214"/>
-      <c r="J1" s="536" t="s">
+      <c r="J1" s="537" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="591"/>
+      <c r="K1" s="644"/>
       <c r="L1" s="205" t="s">
         <v>337</v>
       </c>
@@ -12393,13 +12406,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="206"/>
-      <c r="M2" s="669"/>
+      <c r="M2" s="670"/>
       <c r="N2" s="154">
         <v>2</v>
       </c>
       <c r="O2" s="155"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="672" t="s">
+      <c r="Q2" s="673" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="19">
@@ -12422,13 +12435,13 @@
       <c r="K3" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="M3" s="670"/>
+      <c r="M3" s="671"/>
       <c r="N3" s="17">
         <v>1</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="673"/>
+      <c r="Q3" s="674"/>
       <c r="R3" s="231"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12447,13 +12460,13 @@
       <c r="K4" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="M4" s="670"/>
+      <c r="M4" s="671"/>
       <c r="N4" s="17"/>
       <c r="O4" s="15">
         <v>1</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="673"/>
+      <c r="Q4" s="674"/>
       <c r="R4" s="231"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12473,13 +12486,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="206"/>
-      <c r="M5" s="670"/>
+      <c r="M5" s="671"/>
       <c r="N5" s="17">
         <v>1</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="673"/>
+      <c r="Q5" s="674"/>
       <c r="R5" s="19">
         <v>-1</v>
       </c>
@@ -12500,13 +12513,13 @@
       <c r="K6" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="M6" s="670"/>
+      <c r="M6" s="671"/>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="673"/>
+      <c r="Q6" s="674"/>
       <c r="R6" s="231"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12526,13 +12539,13 @@
         <v>334</v>
       </c>
       <c r="L7" s="208"/>
-      <c r="M7" s="670"/>
+      <c r="M7" s="671"/>
       <c r="N7" s="17">
         <v>1</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="673"/>
+      <c r="Q7" s="674"/>
       <c r="R7" s="19">
         <v>-1</v>
       </c>
@@ -12553,13 +12566,13 @@
       <c r="K8" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="M8" s="670"/>
+      <c r="M8" s="671"/>
       <c r="N8" s="17">
         <v>1</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="673"/>
+      <c r="Q8" s="674"/>
       <c r="R8" s="231"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12579,13 +12592,13 @@
         <v>336</v>
       </c>
       <c r="L9" s="186"/>
-      <c r="M9" s="671"/>
+      <c r="M9" s="672"/>
       <c r="N9" s="163"/>
       <c r="O9" s="18"/>
       <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="674"/>
+      <c r="Q9" s="675"/>
       <c r="R9" s="232"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -12743,10 +12756,10 @@
         <f ca="1">TODAY()</f>
         <v>45277</v>
       </c>
-      <c r="V1" s="536" t="s">
+      <c r="V1" s="537" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="591"/>
+      <c r="W1" s="644"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12765,7 +12778,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="682" t="s">
+      <c r="AD1" s="690" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12782,10 +12795,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="681" t="s">
+      <c r="F2" s="721" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="709" t="s">
+      <c r="G2" s="678" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -12813,10 +12826,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="650" t="s">
+      <c r="V2" s="662" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="651"/>
+      <c r="W2" s="663"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -12835,7 +12848,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="683"/>
+      <c r="AD2" s="691"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -12854,8 +12867,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="639"/>
-      <c r="G3" s="710"/>
+      <c r="F3" s="595"/>
+      <c r="G3" s="679"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -12866,13 +12879,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="719" t="s">
+      <c r="O3" s="688" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="701" t="s">
+      <c r="P3" s="709" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="702"/>
+      <c r="Q3" s="710"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -12882,15 +12895,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="683"/>
+      <c r="AD3" s="691"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="710"/>
+      <c r="G4" s="679"/>
       <c r="H4" s="6"/>
-      <c r="L4" s="672" t="s">
+      <c r="L4" s="673" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="720"/>
+      <c r="O4" s="689"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -12900,12 +12913,12 @@
       <c r="X4" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="536" t="s">
+      <c r="Y4" s="537" t="s">
         <v>195</v>
       </c>
-      <c r="Z4" s="537"/>
-      <c r="AA4" s="591"/>
-      <c r="AD4" s="683"/>
+      <c r="Z4" s="538"/>
+      <c r="AA4" s="644"/>
+      <c r="AD4" s="691"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -12920,21 +12933,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="710"/>
+      <c r="G5" s="679"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="688" t="s">
+      <c r="K5" s="696" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="703"/>
+      <c r="L5" s="711"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="720"/>
+      <c r="O5" s="689"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -12950,11 +12963,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="691" t="s">
+      <c r="Y5" s="699" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="692"/>
-      <c r="AD5" s="683"/>
+      <c r="Z5" s="700"/>
+      <c r="AD5" s="691"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -12964,16 +12977,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="710"/>
+      <c r="G6" s="679"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="689"/>
-      <c r="L6" s="703"/>
-      <c r="O6" s="720"/>
+      <c r="K6" s="697"/>
+      <c r="L6" s="711"/>
+      <c r="O6" s="689"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -12983,20 +12996,20 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="683"/>
+      <c r="AD6" s="691"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="710"/>
+      <c r="G7" s="679"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="689"/>
-      <c r="L7" s="703"/>
+      <c r="K7" s="697"/>
+      <c r="L7" s="711"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="720"/>
+      <c r="O7" s="689"/>
       <c r="P7" s="73"/>
-      <c r="AD7" s="683"/>
+      <c r="AD7" s="691"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13009,7 +13022,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="710"/>
+      <c r="G8" s="679"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13019,41 +13032,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="689"/>
-      <c r="L8" s="703"/>
-      <c r="O8" s="720"/>
+      <c r="K8" s="697"/>
+      <c r="L8" s="711"/>
+      <c r="O8" s="689"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="685" t="s">
+      <c r="S8" s="693" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="686"/>
-      <c r="U8" s="686"/>
-      <c r="V8" s="686"/>
-      <c r="W8" s="686"/>
-      <c r="X8" s="686"/>
-      <c r="Y8" s="686"/>
-      <c r="Z8" s="686"/>
-      <c r="AA8" s="686"/>
-      <c r="AB8" s="686"/>
-      <c r="AC8" s="687"/>
-      <c r="AD8" s="683"/>
+      <c r="T8" s="694"/>
+      <c r="U8" s="694"/>
+      <c r="V8" s="694"/>
+      <c r="W8" s="694"/>
+      <c r="X8" s="694"/>
+      <c r="Y8" s="694"/>
+      <c r="Z8" s="694"/>
+      <c r="AA8" s="694"/>
+      <c r="AB8" s="694"/>
+      <c r="AC8" s="695"/>
+      <c r="AD8" s="691"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="675"/>
-      <c r="G9" s="710"/>
+      <c r="C9" s="715"/>
+      <c r="G9" s="679"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="689"/>
-      <c r="L9" s="713" t="s">
+      <c r="K9" s="697"/>
+      <c r="L9" s="682" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="714"/>
-      <c r="N9" s="715"/>
-      <c r="O9" s="720"/>
+      <c r="M9" s="683"/>
+      <c r="N9" s="684"/>
+      <c r="O9" s="689"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="683"/>
+      <c r="AD9" s="691"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="676"/>
+      <c r="C10" s="716"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13061,7 +13074,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="710"/>
+      <c r="G10" s="679"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13069,33 +13082,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="689"/>
-      <c r="M10" s="678" t="s">
+      <c r="K10" s="697"/>
+      <c r="M10" s="718" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="679"/>
-      <c r="O10" s="679"/>
-      <c r="P10" s="679"/>
-      <c r="Q10" s="679"/>
-      <c r="R10" s="679"/>
-      <c r="S10" s="679"/>
-      <c r="T10" s="679"/>
-      <c r="U10" s="679"/>
-      <c r="V10" s="679"/>
-      <c r="W10" s="679"/>
-      <c r="X10" s="679"/>
-      <c r="Y10" s="679"/>
-      <c r="Z10" s="679"/>
-      <c r="AA10" s="679"/>
-      <c r="AB10" s="679"/>
-      <c r="AC10" s="680"/>
-      <c r="AD10" s="683"/>
+      <c r="N10" s="719"/>
+      <c r="O10" s="719"/>
+      <c r="P10" s="719"/>
+      <c r="Q10" s="719"/>
+      <c r="R10" s="719"/>
+      <c r="S10" s="719"/>
+      <c r="T10" s="719"/>
+      <c r="U10" s="719"/>
+      <c r="V10" s="719"/>
+      <c r="W10" s="719"/>
+      <c r="X10" s="719"/>
+      <c r="Y10" s="719"/>
+      <c r="Z10" s="719"/>
+      <c r="AA10" s="719"/>
+      <c r="AB10" s="719"/>
+      <c r="AC10" s="720"/>
+      <c r="AD10" s="691"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="677"/>
-      <c r="G11" s="710"/>
+      <c r="C11" s="717"/>
+      <c r="G11" s="679"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="689"/>
+      <c r="K11" s="697"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13106,17 +13119,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="699" t="s">
+      <c r="Z11" s="707" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="700"/>
+      <c r="AA11" s="708"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="683"/>
+      <c r="AD11" s="691"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13129,7 +13142,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="710"/>
+      <c r="G12" s="679"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13137,8 +13150,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="689"/>
-      <c r="L12" s="704" t="s">
+      <c r="K12" s="697"/>
+      <c r="L12" s="712" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13153,7 +13166,7 @@
       <c r="Q12" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="531" t="s">
+      <c r="S12" s="532" t="s">
         <v>107</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -13169,26 +13182,26 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="693" t="s">
+      <c r="AA12" s="701" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="694"/>
+      <c r="AB12" s="702"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="683"/>
+      <c r="AD12" s="691"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="675"/>
-      <c r="G13" s="710"/>
-      <c r="K13" s="689"/>
-      <c r="L13" s="705"/>
+      <c r="C13" s="715"/>
+      <c r="G13" s="679"/>
+      <c r="K13" s="697"/>
+      <c r="L13" s="713"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="712" t="s">
+      <c r="Q13" s="681" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="606"/>
-      <c r="S13" s="532"/>
+      <c r="R13" s="604"/>
+      <c r="S13" s="533"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
         <v>132</v>
@@ -13196,17 +13209,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="695"/>
-      <c r="AB13" s="696"/>
-      <c r="AD13" s="683"/>
+      <c r="AA13" s="703"/>
+      <c r="AB13" s="704"/>
+      <c r="AD13" s="691"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="677"/>
+      <c r="C14" s="717"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="710"/>
+      <c r="G14" s="679"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13214,8 +13227,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="689"/>
-      <c r="L14" s="705"/>
+      <c r="K14" s="697"/>
+      <c r="L14" s="713"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13225,7 +13238,7 @@
       <c r="R14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="532"/>
+      <c r="S14" s="533"/>
       <c r="T14" s="77" t="s">
         <v>130</v>
       </c>
@@ -13236,9 +13249,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="695"/>
-      <c r="AB14" s="696"/>
-      <c r="AD14" s="683"/>
+      <c r="AA14" s="703"/>
+      <c r="AB14" s="704"/>
+      <c r="AD14" s="691"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13253,20 +13266,20 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="710"/>
+      <c r="G15" s="679"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="689"/>
-      <c r="L15" s="706"/>
-      <c r="Q15" s="712" t="s">
+      <c r="K15" s="697"/>
+      <c r="L15" s="714"/>
+      <c r="Q15" s="681" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="606"/>
-      <c r="S15" s="532"/>
+      <c r="R15" s="604"/>
+      <c r="S15" s="533"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
         <v>44</v>
@@ -13274,14 +13287,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="695"/>
-      <c r="AB15" s="696"/>
-      <c r="AD15" s="683"/>
+      <c r="AA15" s="703"/>
+      <c r="AB15" s="704"/>
+      <c r="AD15" s="691"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="710"/>
-      <c r="K16" s="689"/>
+      <c r="G16" s="679"/>
+      <c r="K16" s="697"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13289,7 +13302,7 @@
       <c r="R16" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="532"/>
+      <c r="S16" s="533"/>
       <c r="T16" s="76" t="s">
         <v>129</v>
       </c>
@@ -13300,34 +13313,34 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="695"/>
-      <c r="AB16" s="696"/>
-      <c r="AD16" s="683"/>
+      <c r="AA16" s="703"/>
+      <c r="AB16" s="704"/>
+      <c r="AD16" s="691"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="707" t="s">
+      <c r="F17" s="676" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="710"/>
+      <c r="G17" s="679"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="689"/>
-      <c r="S17" s="532"/>
+      <c r="K17" s="697"/>
+      <c r="S17" s="533"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="695"/>
-      <c r="AB17" s="696"/>
-      <c r="AD17" s="683"/>
+      <c r="AA17" s="703"/>
+      <c r="AB17" s="704"/>
+      <c r="AD17" s="691"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13337,61 +13350,58 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="708"/>
-      <c r="G18" s="710"/>
+      <c r="F18" s="677"/>
+      <c r="G18" s="679"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="689"/>
+      <c r="K18" s="697"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="S18" s="532"/>
+      <c r="S18" s="533"/>
       <c r="U18" s="76" t="s">
         <v>133</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="697"/>
-      <c r="AB18" s="698"/>
-      <c r="AD18" s="683"/>
+      <c r="AA18" s="705"/>
+      <c r="AB18" s="706"/>
+      <c r="AD18" s="691"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="711"/>
-      <c r="K19" s="690"/>
+      <c r="G19" s="680"/>
+      <c r="K19" s="698"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="716" t="s">
+      <c r="R19" s="685" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="717"/>
-      <c r="T19" s="718"/>
+      <c r="S19" s="686"/>
+      <c r="T19" s="687"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="684"/>
+      <c r="AD19" s="692"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13403,11 +13413,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Enabled - Al Jazeera E , CNA
Boat_X_Token - Flag

MatriX_TF_V - 4

Boat Node - CNA
Isarel - Gaza - Al Jazeera E
</commit_message>
<xml_diff>
--- a/System_2.1.3.xlsx
+++ b/System_2.1.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F42D1CD-DECC-4A17-9D54-B5586F9507AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3D366D-3E67-47A3-ADBC-C8F9DD032A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="595">
   <si>
     <t>Zone</t>
   </si>
@@ -1818,6 +1818,12 @@
   </si>
   <si>
     <t>Africa 15 - G 639</t>
+  </si>
+  <si>
+    <t>Boat_X_Token</t>
+  </si>
+  <si>
+    <t>Boat Node</t>
   </si>
 </sst>
 </file>
@@ -3404,7 +3410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="724">
+  <cellXfs count="723">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4665,12 +4671,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4716,6 +4720,36 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="40" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4773,34 +4807,139 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4875,140 +5014,71 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -5019,130 +5089,43 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5220,31 +5203,51 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6393,8 +6396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView topLeftCell="M11" workbookViewId="0">
-      <selection activeCell="Z24" sqref="Z24"/>
+    <sheetView topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6449,7 +6452,7 @@
       <c r="P1" s="450" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="566" t="s">
+      <c r="Q1" s="547" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6460,32 +6463,32 @@
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="550">
+      <c r="A2" s="560">
         <f ca="1">TODAY()</f>
         <v>45277</v>
       </c>
-      <c r="B2" s="552" t="s">
+      <c r="B2" s="562" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="564" t="s">
+      <c r="C2" s="574" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="554" t="s">
+      <c r="D2" s="564" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="556" t="s">
+      <c r="E2" s="566" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="201" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="562" t="s">
+      <c r="G2" s="572" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="573" t="s">
+      <c r="I2" s="554" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="448" t="s">
@@ -6509,27 +6512,27 @@
       <c r="P2" s="451">
         <v>40</v>
       </c>
-      <c r="Q2" s="567"/>
+      <c r="Q2" s="548"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>8</v>
       </c>
       <c r="S2" s="21">
         <f>S7+S18</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V2" s="520"/>
       <c r="X2" s="524"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="551"/>
-      <c r="B3" s="553"/>
-      <c r="C3" s="565"/>
-      <c r="D3" s="555"/>
-      <c r="E3" s="557"/>
-      <c r="G3" s="563"/>
+      <c r="A3" s="561"/>
+      <c r="B3" s="563"/>
+      <c r="C3" s="575"/>
+      <c r="D3" s="565"/>
+      <c r="E3" s="567"/>
+      <c r="G3" s="573"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="574"/>
+      <c r="I3" s="555"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6538,7 +6541,7 @@
       </c>
       <c r="Q3" s="527">
         <f>SUM(X24:X30)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V3" s="521"/>
       <c r="X3" s="525"/>
@@ -6548,10 +6551,10 @@
         <v>390</v>
       </c>
       <c r="B4" s="257"/>
-      <c r="C4" s="558" t="s">
+      <c r="C4" s="568" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="574"/>
+      <c r="I4" s="555"/>
       <c r="R4" s="527" t="s">
         <v>585</v>
       </c>
@@ -6569,7 +6572,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="559"/>
+      <c r="C5" s="569"/>
       <c r="D5" s="235" t="s">
         <v>103</v>
       </c>
@@ -6585,7 +6588,7 @@
       <c r="H5" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="574"/>
+      <c r="I5" s="555"/>
       <c r="J5" s="449" t="s">
         <v>273</v>
       </c>
@@ -6615,22 +6618,22 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="547" t="s">
+      <c r="A6" s="557" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="560"/>
-      <c r="D6" s="561"/>
+      <c r="C6" s="570"/>
+      <c r="D6" s="571"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="533"/>
-      <c r="I6" s="574"/>
+      <c r="I6" s="555"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="548"/>
+      <c r="A7" s="558"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6641,7 +6644,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="533"/>
-      <c r="I7" s="574"/>
+      <c r="I7" s="555"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6679,7 +6682,7 @@
       </c>
     </row>
     <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="549"/>
+      <c r="A8" s="559"/>
       <c r="B8" s="222" t="s">
         <v>28</v>
       </c>
@@ -6688,7 +6691,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="533"/>
-      <c r="I8" s="574"/>
+      <c r="I8" s="555"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
@@ -6714,7 +6717,7 @@
       </c>
       <c r="G9" s="533"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="574"/>
+      <c r="I9" s="555"/>
       <c r="M9" s="19" t="s">
         <v>548</v>
       </c>
@@ -6738,10 +6741,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!S8</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" s="533"/>
-      <c r="I10" s="574"/>
+      <c r="I10" s="555"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6769,7 +6772,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="533"/>
-      <c r="I11" s="574"/>
+      <c r="I11" s="555"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -6795,12 +6798,12 @@
       <c r="S11" s="24">
         <v>2</v>
       </c>
-      <c r="U11" s="568" t="s">
+      <c r="U11" s="549" t="s">
         <v>588</v>
       </c>
-      <c r="V11" s="569"/>
-      <c r="W11" s="569"/>
-      <c r="X11" s="570"/>
+      <c r="V11" s="550"/>
+      <c r="W11" s="550"/>
+      <c r="X11" s="551"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="240" t="s">
@@ -6811,7 +6814,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="533"/>
-      <c r="I12" s="574"/>
+      <c r="I12" s="555"/>
       <c r="J12" s="24" t="s">
         <v>539</v>
       </c>
@@ -6844,7 +6847,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="533"/>
-      <c r="I13" s="574"/>
+      <c r="I13" s="555"/>
       <c r="J13" s="108" t="s">
         <v>577</v>
       </c>
@@ -6885,7 +6888,7 @@
       <c r="H14" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="574"/>
+      <c r="I14" s="555"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -6903,7 +6906,7 @@
       <c r="H15" s="289">
         <v>0</v>
       </c>
-      <c r="I15" s="574"/>
+      <c r="I15" s="555"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -6934,7 +6937,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="574"/>
+      <c r="I16" s="555"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -6968,7 +6971,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="574"/>
+      <c r="I17" s="555"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -6980,13 +6983,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="574"/>
+      <c r="I18" s="555"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="571" t="s">
+      <c r="O18" s="552" t="s">
         <v>540</v>
       </c>
-      <c r="P18" s="572"/>
+      <c r="P18" s="553"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -6996,7 +6999,7 @@
       </c>
       <c r="S18" s="24">
         <f>5-S26</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U18" s="6" t="s">
         <v>479</v>
@@ -7007,12 +7010,12 @@
       <c r="W18" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="X18" s="520">
+      <c r="X18" s="524">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="574"/>
+      <c r="I19" s="555"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7023,7 +7026,7 @@
         <v>1</v>
       </c>
       <c r="W19" s="6"/>
-      <c r="X19" s="521"/>
+      <c r="X19" s="525"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="244" t="s">
@@ -7044,7 +7047,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="574"/>
+      <c r="I20" s="555"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7063,13 +7066,13 @@
       <c r="W20" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="X20" s="521">
+      <c r="X20" s="525">
         <v>1</v>
       </c>
       <c r="Z20" s="6"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="574"/>
+      <c r="I21" s="555"/>
       <c r="M21" s="227" t="s">
         <v>422</v>
       </c>
@@ -7080,7 +7083,9 @@
       <c r="W21" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="X21" s="521"/>
+      <c r="X21" s="525">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="244" t="s">
@@ -7101,7 +7106,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="574"/>
+      <c r="I22" s="555"/>
       <c r="U22" s="6" t="s">
         <v>589</v>
       </c>
@@ -7111,7 +7116,7 @@
       <c r="W22" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="X22" s="530">
+      <c r="X22" s="523">
         <v>1</v>
       </c>
     </row>
@@ -7125,7 +7130,7 @@
       <c r="E23" s="301" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="574"/>
+      <c r="I23" s="555"/>
       <c r="U23" s="6" t="s">
         <v>74</v>
       </c>
@@ -7135,7 +7140,7 @@
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="574"/>
+      <c r="I24" s="555"/>
       <c r="U24" s="379"/>
       <c r="V24" s="526">
         <v>-1</v>
@@ -7163,7 +7168,7 @@
       <c r="H25" s="201" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="574"/>
+      <c r="I25" s="555"/>
       <c r="J25" s="449" t="s">
         <v>274</v>
       </c>
@@ -7178,7 +7183,7 @@
       </c>
       <c r="U25" s="35"/>
       <c r="W25" s="19"/>
-      <c r="X25" s="531" t="s">
+      <c r="X25" s="530" t="s">
         <v>44</v>
       </c>
     </row>
@@ -7203,7 +7208,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="574"/>
+      <c r="I26" s="555"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7221,7 +7226,7 @@
         <v>0</v>
       </c>
       <c r="S26" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T26" s="61" t="s">
         <v>586</v>
@@ -7238,7 +7243,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="574"/>
+      <c r="I27" s="555"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7265,7 +7270,7 @@
       <c r="E28" s="226">
         <v>2</v>
       </c>
-      <c r="I28" s="574"/>
+      <c r="I28" s="555"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7287,7 +7292,7 @@
       <c r="H29" s="201" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="575"/>
+      <c r="I29" s="556"/>
       <c r="J29" s="358"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7305,8 +7310,8 @@
       <c r="W29" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="X29" s="177">
-        <v>0</v>
+      <c r="X29" s="24">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7331,11 +7336,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7347,6 +7347,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7356,8 +7361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CFE6D2-5300-4D31-9A66-EC93F2A54B69}">
   <dimension ref="A1:AQ27"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AQ15" sqref="AQ15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7422,7 +7427,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="562" t="s">
+      <c r="I1" s="572" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7483,7 +7488,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="454"/>
-      <c r="AN1" s="600"/>
+      <c r="AN1" s="603"/>
       <c r="AO1" s="375" t="s">
         <v>487</v>
       </c>
@@ -7492,23 +7497,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="582">
+      <c r="A2" s="627">
         <f ca="1">TODAY()</f>
         <v>45277</v>
       </c>
-      <c r="B2" s="584" t="s">
+      <c r="B2" s="629" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="564" t="s">
+      <c r="C2" s="574" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="586" t="s">
+      <c r="D2" s="631" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="630" t="s">
+      <c r="E2" s="576" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="605" t="s">
+      <c r="F2" s="584" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="445" t="s">
@@ -7517,31 +7522,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="563"/>
+      <c r="I2" s="573"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="632" t="s">
+      <c r="K2" s="578" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="633"/>
-      <c r="M2" s="605" t="s">
+      <c r="L2" s="579"/>
+      <c r="M2" s="584" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="609" t="s">
+      <c r="O2" s="610" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="564" t="s">
+      <c r="Q2" s="574" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="532"/>
-      <c r="S2" s="622" t="s">
+      <c r="S2" s="597" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7574,15 +7579,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="480"/>
-      <c r="AN2" s="601"/>
+      <c r="AN2" s="604"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="583"/>
-      <c r="B3" s="585"/>
-      <c r="C3" s="565"/>
-      <c r="D3" s="587"/>
-      <c r="E3" s="631"/>
-      <c r="F3" s="606"/>
+      <c r="A3" s="628"/>
+      <c r="B3" s="630"/>
+      <c r="C3" s="575"/>
+      <c r="D3" s="632"/>
+      <c r="E3" s="577"/>
+      <c r="F3" s="585"/>
       <c r="G3" s="446" t="s">
         <v>28</v>
       </c>
@@ -7601,17 +7606,17 @@
       <c r="L3" s="211" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="606"/>
+      <c r="M3" s="585"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="610"/>
+      <c r="O3" s="611"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="565"/>
+      <c r="Q3" s="575"/>
       <c r="R3" s="534"/>
-      <c r="S3" s="623"/>
+      <c r="S3" s="599"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7628,7 +7633,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="621" t="s">
+      <c r="AD3" s="594" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="272"/>
@@ -7640,16 +7645,16 @@
       <c r="AK3" s="272"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="480"/>
-      <c r="AN3" s="601"/>
+      <c r="AN3" s="604"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="251" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="598" t="s">
+      <c r="B4" s="643" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="564" t="s">
+      <c r="C4" s="574" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="384" t="s">
@@ -7658,7 +7663,7 @@
       <c r="E4" s="422">
         <v>1</v>
       </c>
-      <c r="F4" s="606"/>
+      <c r="F4" s="585"/>
       <c r="G4" s="427" t="s">
         <v>203</v>
       </c>
@@ -7675,11 +7680,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="214"/>
-      <c r="M4" s="606"/>
+      <c r="M4" s="585"/>
       <c r="N4" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="610"/>
+      <c r="O4" s="611"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7706,7 +7711,7 @@
       <c r="AA4" s="325"/>
       <c r="AB4" s="219"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="621"/>
+      <c r="AD4" s="594"/>
       <c r="AE4" s="272"/>
       <c r="AF4" s="272"/>
       <c r="AG4" s="16"/>
@@ -7716,37 +7721,37 @@
       <c r="AK4" s="272"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="480"/>
-      <c r="AN4" s="601"/>
+      <c r="AN4" s="604"/>
       <c r="AO4" s="375" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="562" t="s">
+      <c r="A5" s="572" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="599"/>
-      <c r="C5" s="565"/>
+      <c r="B5" s="644"/>
+      <c r="C5" s="575"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="423">
         <v>1</v>
       </c>
-      <c r="F5" s="606"/>
-      <c r="G5" s="590" t="s">
+      <c r="F5" s="585"/>
+      <c r="G5" s="635" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="590"/>
-      <c r="I5" s="590"/>
-      <c r="J5" s="590"/>
-      <c r="K5" s="590"/>
-      <c r="L5" s="591"/>
-      <c r="M5" s="606"/>
+      <c r="H5" s="635"/>
+      <c r="I5" s="635"/>
+      <c r="J5" s="635"/>
+      <c r="K5" s="635"/>
+      <c r="L5" s="636"/>
+      <c r="M5" s="585"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="610"/>
+      <c r="O5" s="611"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7777,24 +7782,24 @@
       <c r="AK5" s="272"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="480"/>
-      <c r="AN5" s="601"/>
+      <c r="AN5" s="604"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="563"/>
-      <c r="B6" s="596" t="s">
+      <c r="A6" s="573"/>
+      <c r="B6" s="641" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="560"/>
-      <c r="D6" s="561"/>
-      <c r="F6" s="606"/>
-      <c r="G6" s="592"/>
-      <c r="H6" s="592"/>
-      <c r="I6" s="592"/>
-      <c r="J6" s="592"/>
-      <c r="K6" s="592"/>
-      <c r="L6" s="593"/>
-      <c r="M6" s="606"/>
-      <c r="O6" s="610"/>
+      <c r="C6" s="570"/>
+      <c r="D6" s="571"/>
+      <c r="F6" s="585"/>
+      <c r="G6" s="637"/>
+      <c r="H6" s="637"/>
+      <c r="I6" s="637"/>
+      <c r="J6" s="637"/>
+      <c r="K6" s="637"/>
+      <c r="L6" s="638"/>
+      <c r="M6" s="585"/>
+      <c r="O6" s="611"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7818,16 +7823,16 @@
       <c r="AF6" s="272"/>
       <c r="AG6" s="272"/>
       <c r="AH6" s="272"/>
-      <c r="AI6" s="615"/>
+      <c r="AI6" s="593"/>
       <c r="AJ6" s="493" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="615" t="s">
+      <c r="AK6" s="593" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="272"/>
       <c r="AM6" s="480"/>
-      <c r="AN6" s="601"/>
+      <c r="AN6" s="604"/>
       <c r="AO6" s="375" t="s">
         <v>488</v>
       </c>
@@ -7836,7 +7841,7 @@
       <c r="A7" s="245" t="s">
         <v>552</v>
       </c>
-      <c r="B7" s="597"/>
+      <c r="B7" s="642"/>
       <c r="C7" s="212" t="s">
         <v>383</v>
       </c>
@@ -7846,7 +7851,7 @@
       <c r="E7" s="281">
         <v>3</v>
       </c>
-      <c r="F7" s="606"/>
+      <c r="F7" s="585"/>
       <c r="G7" s="447">
         <v>0</v>
       </c>
@@ -7865,8 +7870,8 @@
       <c r="L7" s="222">
         <v>0</v>
       </c>
-      <c r="M7" s="606"/>
-      <c r="O7" s="610"/>
+      <c r="M7" s="585"/>
+      <c r="O7" s="611"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7890,18 +7895,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="272"/>
       <c r="AF7" s="272"/>
-      <c r="AG7" s="621" t="s">
+      <c r="AG7" s="594" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="272"/>
-      <c r="AI7" s="615"/>
+      <c r="AI7" s="593"/>
       <c r="AJ7" s="272"/>
-      <c r="AK7" s="615"/>
+      <c r="AK7" s="593"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="480"/>
-      <c r="AN7" s="601"/>
+      <c r="AN7" s="604"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -7918,25 +7923,27 @@
         <f>SUM(G7:N9)</f>
         <v>16</v>
       </c>
-      <c r="F8" s="606"/>
-      <c r="G8" s="591">
-        <v>0</v>
-      </c>
-      <c r="H8" s="588" t="s">
+      <c r="F8" s="585"/>
+      <c r="G8" s="636">
+        <v>0</v>
+      </c>
+      <c r="H8" s="633" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="532"/>
-      <c r="J8" s="588" t="s">
+      <c r="I8" s="532">
+        <v>0</v>
+      </c>
+      <c r="J8" s="633" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="594"/>
-      <c r="L8" s="624"/>
-      <c r="M8" s="607"/>
-      <c r="N8" s="627">
+      <c r="K8" s="639"/>
+      <c r="L8" s="595"/>
+      <c r="M8" s="608"/>
+      <c r="N8" s="600">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="610"/>
+      <c r="O8" s="611"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7954,14 +7961,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="272"/>
       <c r="AF8" s="272"/>
-      <c r="AG8" s="621"/>
+      <c r="AG8" s="594"/>
       <c r="AH8" s="272"/>
-      <c r="AI8" s="615"/>
+      <c r="AI8" s="593"/>
       <c r="AJ8" s="272"/>
       <c r="AK8" s="272"/>
       <c r="AL8" s="272"/>
       <c r="AM8" s="480"/>
-      <c r="AN8" s="601"/>
+      <c r="AN8" s="604"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="245" t="s">
@@ -7976,17 +7983,17 @@
       <c r="D9" s="385" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="606"/>
-      <c r="G9" s="593"/>
-      <c r="H9" s="589"/>
+      <c r="F9" s="585"/>
+      <c r="G9" s="638"/>
+      <c r="H9" s="634"/>
       <c r="I9" s="534"/>
-      <c r="J9" s="589"/>
-      <c r="K9" s="595"/>
-      <c r="L9" s="625"/>
-      <c r="M9" s="608"/>
-      <c r="N9" s="628"/>
-      <c r="O9" s="611"/>
-      <c r="S9" s="622" t="s">
+      <c r="J9" s="634"/>
+      <c r="K9" s="640"/>
+      <c r="L9" s="596"/>
+      <c r="M9" s="609"/>
+      <c r="N9" s="601"/>
+      <c r="O9" s="612"/>
+      <c r="S9" s="597" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8008,16 +8015,16 @@
       </c>
       <c r="AE9" s="272"/>
       <c r="AF9" s="272"/>
-      <c r="AG9" s="621"/>
+      <c r="AG9" s="594"/>
       <c r="AH9" s="272"/>
-      <c r="AI9" s="615"/>
+      <c r="AI9" s="593"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="615" t="s">
+      <c r="AK9" s="593" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="272"/>
       <c r="AM9" s="480"/>
-      <c r="AN9" s="601"/>
+      <c r="AN9" s="604"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8032,22 +8039,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="250">
         <f>Boat!S8</f>
-        <v>43</v>
-      </c>
-      <c r="F10" s="606"/>
+        <v>42</v>
+      </c>
+      <c r="F10" s="585"/>
       <c r="N10" s="470" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="639" t="s">
+      <c r="O10" s="587" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="612" t="s">
+      <c r="P10" s="613" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="626"/>
+      <c r="S10" s="598"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8077,16 +8084,16 @@
       <c r="AF10" s="251" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="621"/>
+      <c r="AG10" s="594"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="615"/>
+      <c r="AI10" s="593"/>
       <c r="AJ10" s="272"/>
-      <c r="AK10" s="615"/>
+      <c r="AK10" s="593"/>
       <c r="AL10" s="272"/>
       <c r="AM10" s="494" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="601"/>
+      <c r="AN10" s="604"/>
       <c r="AO10" s="214" t="s">
         <v>95</v>
       </c>
@@ -8104,18 +8111,18 @@
       <c r="D11" s="175" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="606"/>
+      <c r="F11" s="585"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="640"/>
-      <c r="P11" s="613"/>
+      <c r="O11" s="588"/>
+      <c r="P11" s="614"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="626"/>
+      <c r="S11" s="598"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8139,14 +8146,14 @@
       <c r="AF11" s="272" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="621"/>
+      <c r="AG11" s="594"/>
       <c r="AH11" s="272"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="272"/>
       <c r="AK11" s="272"/>
       <c r="AL11" s="272"/>
       <c r="AM11" s="480"/>
-      <c r="AN11" s="601"/>
+      <c r="AN11" s="604"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8165,7 +8172,7 @@
       <c r="E12" s="237">
         <v>3</v>
       </c>
-      <c r="F12" s="606"/>
+      <c r="F12" s="585"/>
       <c r="G12" s="374" t="s">
         <v>411</v>
       </c>
@@ -8174,16 +8181,16 @@
       </c>
       <c r="I12" s="538"/>
       <c r="J12" s="538"/>
-      <c r="K12" s="644"/>
+      <c r="K12" s="592"/>
       <c r="L12" s="213"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
-      <c r="O12" s="640"/>
-      <c r="P12" s="613"/>
+      <c r="O12" s="588"/>
+      <c r="P12" s="614"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="623"/>
+      <c r="S12" s="599"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8204,16 +8211,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="629" t="s">
+      <c r="AD12" s="602" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="493" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="621" t="s">
+      <c r="AF12" s="594" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="621"/>
+      <c r="AG12" s="594"/>
       <c r="AH12" s="251" t="s">
         <v>264</v>
       </c>
@@ -8226,7 +8233,7 @@
       <c r="AM12" s="616" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="601"/>
+      <c r="AN12" s="604"/>
       <c r="AO12" s="375" t="s">
         <v>97</v>
       </c>
@@ -8238,17 +8245,17 @@
       <c r="E13" s="500">
         <v>-3</v>
       </c>
-      <c r="F13" s="606"/>
+      <c r="F13" s="585"/>
       <c r="G13" s="538" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="538"/>
       <c r="I13" s="538"/>
-      <c r="J13" s="644"/>
+      <c r="J13" s="592"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="640"/>
-      <c r="P13" s="614"/>
+      <c r="O13" s="588"/>
+      <c r="P13" s="615"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8269,8 +8276,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="629"/>
-      <c r="AF13" s="621"/>
+      <c r="AD13" s="602"/>
+      <c r="AF13" s="594"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="251" t="s">
         <v>314</v>
@@ -8282,7 +8289,7 @@
       <c r="AK13" s="272"/>
       <c r="AL13" s="272"/>
       <c r="AM13" s="616"/>
-      <c r="AN13" s="601"/>
+      <c r="AN13" s="604"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="502"/>
@@ -8290,18 +8297,18 @@
       <c r="C14" s="511"/>
       <c r="D14" s="504"/>
       <c r="E14" s="505"/>
-      <c r="F14" s="606"/>
+      <c r="F14" s="585"/>
       <c r="G14" s="538" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="538"/>
       <c r="I14" s="538"/>
-      <c r="J14" s="644"/>
+      <c r="J14" s="592"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="640"/>
+      <c r="O14" s="588"/>
       <c r="Q14" s="61" t="s">
         <v>559</v>
       </c>
@@ -8322,9 +8329,9 @@
       <c r="AA14" s="325"/>
       <c r="AB14" s="219"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="629"/>
+      <c r="AD14" s="602"/>
       <c r="AE14" s="272"/>
-      <c r="AF14" s="621"/>
+      <c r="AF14" s="594"/>
       <c r="AG14" s="272"/>
       <c r="AH14" s="272"/>
       <c r="AI14" s="70"/>
@@ -8332,7 +8339,7 @@
       <c r="AK14" s="272"/>
       <c r="AL14" s="272"/>
       <c r="AM14" s="616"/>
-      <c r="AN14" s="601"/>
+      <c r="AN14" s="604"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="501" t="s">
@@ -8341,8 +8348,8 @@
       <c r="C15" s="532" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="606"/>
-      <c r="O15" s="640"/>
+      <c r="F15" s="585"/>
+      <c r="O15" s="588"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8364,8 +8371,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="629"/>
-      <c r="AF15" s="621"/>
+      <c r="AD15" s="602"/>
+      <c r="AF15" s="594"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="251" t="s">
         <v>466</v>
@@ -8379,7 +8386,7 @@
       <c r="AK15" s="272"/>
       <c r="AL15" s="272"/>
       <c r="AM15" s="616"/>
-      <c r="AN15" s="601"/>
+      <c r="AN15" s="604"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8401,13 +8408,13 @@
       <c r="E16" s="237">
         <v>1</v>
       </c>
-      <c r="F16" s="606"/>
+      <c r="F16" s="585"/>
       <c r="G16" s="374" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="640"/>
+      <c r="O16" s="588"/>
       <c r="R16" s="487" t="s">
         <v>185</v>
       </c>
@@ -8439,18 +8446,18 @@
       <c r="AM16" s="480" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="601"/>
+      <c r="AN16" s="604"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="606"/>
+      <c r="F17" s="585"/>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="640"/>
+      <c r="O17" s="588"/>
       <c r="Q17" s="21" t="s">
         <v>557</v>
       </c>
@@ -8495,7 +8502,7 @@
       <c r="AK17" s="272"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="480"/>
-      <c r="AN17" s="601"/>
+      <c r="AN17" s="604"/>
       <c r="AO17" s="214" t="s">
         <v>516</v>
       </c>
@@ -8519,21 +8526,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="606"/>
+      <c r="F18" s="585"/>
       <c r="G18" s="374" t="s">
         <v>554</v>
       </c>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="640"/>
+      <c r="O18" s="588"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="634" t="s">
+      <c r="R18" s="580" t="s">
         <v>562</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="579" t="s">
+      <c r="U18" s="624" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8554,7 +8561,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="272"/>
-      <c r="AF18" s="615" t="s">
+      <c r="AF18" s="593" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="272"/>
@@ -8566,19 +8573,19 @@
       <c r="AK18" s="272"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="480"/>
-      <c r="AN18" s="601"/>
+      <c r="AN18" s="604"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="606"/>
-      <c r="O19" s="640"/>
-      <c r="R19" s="635"/>
+      <c r="F19" s="585"/>
+      <c r="O19" s="588"/>
+      <c r="R19" s="581"/>
       <c r="S19" s="30" t="s">
         <v>560</v>
       </c>
-      <c r="U19" s="580"/>
+      <c r="U19" s="625"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="483" t="s">
@@ -8593,7 +8600,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="272"/>
-      <c r="AF19" s="615"/>
+      <c r="AF19" s="593"/>
       <c r="AG19" s="272"/>
       <c r="AH19" s="272"/>
       <c r="AI19" s="70"/>
@@ -8603,7 +8610,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="480"/>
-      <c r="AN19" s="601"/>
+      <c r="AN19" s="604"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8624,18 +8631,18 @@
       <c r="E20" s="489">
         <v>-1</v>
       </c>
-      <c r="F20" s="606"/>
+      <c r="F20" s="585"/>
       <c r="G20" s="374" t="s">
         <v>509</v>
       </c>
-      <c r="O20" s="640"/>
-      <c r="Q20" s="642" t="s">
+      <c r="O20" s="588"/>
+      <c r="Q20" s="590" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="456" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="581"/>
+      <c r="U20" s="626"/>
       <c r="W20" s="457"/>
       <c r="X20" s="484" t="s">
         <v>175</v>
@@ -8665,7 +8672,7 @@
       <c r="AM20" s="427" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="601"/>
+      <c r="AN20" s="604"/>
       <c r="AO20" s="375" t="s">
         <v>478</v>
       </c>
@@ -8689,12 +8696,12 @@
       <c r="E21" s="281">
         <v>1</v>
       </c>
-      <c r="F21" s="606"/>
-      <c r="O21" s="640"/>
-      <c r="Q21" s="643"/>
+      <c r="F21" s="585"/>
+      <c r="O21" s="588"/>
+      <c r="Q21" s="591"/>
       <c r="T21" s="474"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="576"/>
+      <c r="V21" s="621"/>
       <c r="W21" s="478" t="s">
         <v>176</v>
       </c>
@@ -8732,14 +8739,14 @@
       <c r="AM21" s="480" t="s">
         <v>572</v>
       </c>
-      <c r="AN21" s="601"/>
+      <c r="AN21" s="604"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="606"/>
+      <c r="F22" s="585"/>
       <c r="G22" s="374" t="s">
         <v>507</v>
       </c>
-      <c r="O22" s="640"/>
+      <c r="O22" s="588"/>
       <c r="R22" s="486" t="s">
         <v>44</v>
       </c>
@@ -8747,7 +8754,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="577"/>
+      <c r="V22" s="622"/>
       <c r="W22" s="478" t="s">
         <v>176</v>
       </c>
@@ -8765,7 +8772,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="615" t="s">
+      <c r="AJ22" s="593" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="272"/>
@@ -8773,7 +8780,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="318"/>
-      <c r="AN22" s="601"/>
+      <c r="AN22" s="604"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="244" t="s">
@@ -8791,16 +8798,16 @@
       <c r="E23" s="238">
         <v>1</v>
       </c>
-      <c r="F23" s="606"/>
-      <c r="O23" s="640"/>
-      <c r="Q23" s="642" t="s">
+      <c r="F23" s="585"/>
+      <c r="O23" s="588"/>
+      <c r="Q23" s="590" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="472" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="577"/>
+      <c r="V23" s="622"/>
       <c r="W23" s="148"/>
       <c r="X23" s="481" t="s">
         <v>189</v>
@@ -8816,13 +8823,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="615"/>
+      <c r="AJ23" s="593"/>
       <c r="AK23" s="272"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="318"/>
-      <c r="AN23" s="601"/>
+      <c r="AN23" s="604"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="492" t="s">
@@ -8840,17 +8847,17 @@
       <c r="E24" s="488">
         <v>1</v>
       </c>
-      <c r="F24" s="606"/>
+      <c r="F24" s="585"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
-      <c r="O24" s="640"/>
-      <c r="Q24" s="643"/>
+      <c r="O24" s="588"/>
+      <c r="Q24" s="591"/>
       <c r="T24" s="17"/>
       <c r="U24" s="240" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="577"/>
+      <c r="V24" s="622"/>
       <c r="W24" s="148"/>
       <c r="X24" s="481" t="s">
         <v>186</v>
@@ -8874,11 +8881,11 @@
         <v>481</v>
       </c>
       <c r="AM24" s="318"/>
-      <c r="AN24" s="601"/>
+      <c r="AN24" s="604"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="606"/>
-      <c r="O25" s="640"/>
+      <c r="F25" s="585"/>
+      <c r="O25" s="588"/>
       <c r="P25" s="214" t="s">
         <v>285</v>
       </c>
@@ -8891,7 +8898,7 @@
       <c r="U25" s="452" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="578"/>
+      <c r="V25" s="623"/>
       <c r="W25" s="148"/>
       <c r="X25" s="481" t="s">
         <v>190</v>
@@ -8913,7 +8920,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="318"/>
-      <c r="AN25" s="601"/>
+      <c r="AN25" s="604"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="244" t="s">
@@ -8931,16 +8938,16 @@
       <c r="E26" s="424">
         <v>1</v>
       </c>
-      <c r="F26" s="606"/>
+      <c r="F26" s="585"/>
       <c r="G26" s="374" t="s">
         <v>505</v>
       </c>
-      <c r="O26" s="640"/>
-      <c r="P26" s="603" t="s">
+      <c r="O26" s="588"/>
+      <c r="P26" s="606" t="s">
         <v>549</v>
       </c>
-      <c r="Q26" s="604"/>
-      <c r="R26" s="636" t="s">
+      <c r="Q26" s="607"/>
+      <c r="R26" s="582" t="s">
         <v>561</v>
       </c>
       <c r="T26" s="183"/>
@@ -8979,7 +8986,7 @@
       <c r="AM26" s="494" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="601"/>
+      <c r="AN26" s="604"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8991,12 +8998,12 @@
       <c r="E27" s="281" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="638"/>
+      <c r="F27" s="586"/>
       <c r="G27" s="61" t="s">
         <v>571</v>
       </c>
-      <c r="O27" s="641"/>
-      <c r="R27" s="637"/>
+      <c r="O27" s="589"/>
+      <c r="R27" s="583"/>
       <c r="S27" s="473" t="s">
         <v>54</v>
       </c>
@@ -9026,32 +9033,26 @@
       <c r="AM27" s="427" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="602"/>
+      <c r="AN27" s="605"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -9068,22 +9069,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9093,8 +9100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P9" workbookViewId="0">
-      <selection activeCell="AM14" sqref="AM14"/>
+    <sheetView tabSelected="1" topLeftCell="P18" workbookViewId="0">
+      <selection activeCell="AM20" sqref="AM20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9181,16 +9188,16 @@
       <c r="Q1" s="142"/>
       <c r="R1" s="142"/>
       <c r="S1" s="6"/>
-      <c r="T1" s="562" t="s">
+      <c r="T1" s="572" t="s">
         <v>236</v>
       </c>
-      <c r="U1" s="660" t="s">
+      <c r="U1" s="649" t="s">
         <v>237</v>
       </c>
-      <c r="V1" s="662" t="s">
+      <c r="V1" s="651" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="663"/>
+      <c r="W1" s="652"/>
       <c r="X1" s="324">
         <f>68-(S8+W3+V3+Q3)</f>
         <v>0</v>
@@ -9206,42 +9213,42 @@
       <c r="AB1" s="320" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="664" t="s">
+      <c r="AC1" s="653" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="665"/>
-      <c r="AE1" s="666"/>
-      <c r="AF1" s="667" t="s">
+      <c r="AD1" s="654"/>
+      <c r="AE1" s="655"/>
+      <c r="AF1" s="656" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="668"/>
-      <c r="AH1" s="669"/>
-      <c r="AI1" s="656" t="s">
+      <c r="AG1" s="657"/>
+      <c r="AH1" s="658"/>
+      <c r="AI1" s="645" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="657"/>
-      <c r="AK1" s="658"/>
+      <c r="AJ1" s="646"/>
+      <c r="AK1" s="647"/>
       <c r="AN1" s="112"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="648">
+      <c r="J2" s="659">
         <f>SUM(J5:J30)</f>
         <v>2</v>
       </c>
-      <c r="K2" s="650">
+      <c r="K2" s="661">
         <f>SUM(K4:K29)</f>
-        <v>4</v>
-      </c>
-      <c r="L2" s="652">
+        <v>5</v>
+      </c>
+      <c r="L2" s="663">
         <f>SUM(L4:L29)</f>
         <v>7</v>
       </c>
-      <c r="M2" s="627">
+      <c r="M2" s="600">
         <f>SUM(K30:K37)* (-1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N2" s="285" t="s">
         <v>243</v>
@@ -9258,11 +9265,11 @@
       <c r="R2" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="S2" s="654" t="s">
+      <c r="S2" s="665" t="s">
         <v>239</v>
       </c>
-      <c r="T2" s="659"/>
-      <c r="U2" s="661"/>
+      <c r="T2" s="648"/>
+      <c r="U2" s="650"/>
       <c r="V2" s="61" t="s">
         <v>456</v>
       </c>
@@ -9322,10 +9329,10 @@
       </c>
     </row>
     <row r="3" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J3" s="649"/>
-      <c r="K3" s="651"/>
-      <c r="L3" s="653"/>
-      <c r="M3" s="628"/>
+      <c r="J3" s="660"/>
+      <c r="K3" s="662"/>
+      <c r="L3" s="664"/>
+      <c r="M3" s="601"/>
       <c r="N3" s="177">
         <f>(J2+K2)-W3</f>
         <v>0</v>
@@ -9339,10 +9346,10 @@
       </c>
       <c r="R3" s="159">
         <f>SUM(R4:R29)</f>
-        <v>43</v>
-      </c>
-      <c r="S3" s="655"/>
-      <c r="T3" s="563"/>
+        <v>42</v>
+      </c>
+      <c r="S3" s="666"/>
+      <c r="T3" s="573"/>
       <c r="U3" s="331">
         <f>R3+V3+W3+Q3</f>
         <v>68</v>
@@ -9353,7 +9360,7 @@
       </c>
       <c r="W3" s="187">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9365,7 +9372,7 @@
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
@@ -9397,7 +9404,7 @@
       </c>
       <c r="AH3" s="100">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AI3" s="100">
         <f t="shared" si="1"/>
@@ -9443,7 +9450,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="645" t="s">
+      <c r="M4" s="667" t="s">
         <v>200</v>
       </c>
       <c r="N4" s="20"/>
@@ -9526,7 +9533,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="646"/>
+      <c r="M5" s="668"/>
       <c r="N5" s="20"/>
       <c r="O5" s="2" t="s">
         <v>347</v>
@@ -9614,7 +9621,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="646"/>
+      <c r="M6" s="668"/>
       <c r="N6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9704,7 +9711,7 @@
         <f t="shared" ref="L7:L37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="M7" s="646"/>
+      <c r="M7" s="668"/>
       <c r="N7" s="20"/>
       <c r="O7" s="2" t="s">
         <v>342</v>
@@ -9808,7 +9815,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M8" s="646"/>
+      <c r="M8" s="668"/>
       <c r="N8" s="21" t="s">
         <v>238</v>
       </c>
@@ -9826,7 +9833,7 @@
       </c>
       <c r="S8" s="340">
         <f>R3</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T8" s="17"/>
       <c r="U8" s="348"/>
@@ -9894,7 +9901,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M9" s="646"/>
+      <c r="M9" s="668"/>
       <c r="N9" s="21" t="s">
         <v>342</v>
       </c>
@@ -9992,7 +9999,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M10" s="646"/>
+      <c r="M10" s="668"/>
       <c r="N10" s="20"/>
       <c r="O10" s="2" t="s">
         <v>347</v>
@@ -10071,7 +10078,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M11" s="646"/>
+      <c r="M11" s="668"/>
       <c r="N11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10133,7 +10140,7 @@
       <c r="AN11" s="112"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="591" t="s">
+      <c r="A12" s="636" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10142,7 +10149,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="642" t="s">
+      <c r="E12" s="590" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="277">
@@ -10162,7 +10169,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M12" s="646"/>
+      <c r="M12" s="668"/>
       <c r="N12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10236,14 +10243,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="593"/>
+      <c r="A13" s="638"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="643"/>
+      <c r="E13" s="591"/>
       <c r="F13" s="177">
         <v>0</v>
       </c>
@@ -10264,7 +10271,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M13" s="646"/>
+      <c r="M13" s="668"/>
       <c r="N13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10339,7 +10346,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M14" s="646"/>
+      <c r="M14" s="668"/>
       <c r="N14" s="20"/>
       <c r="O14" s="210" t="s">
         <v>346</v>
@@ -10407,7 +10414,7 @@
       <c r="AL14" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="AM14" s="723" t="s">
+      <c r="AM14" s="531" t="s">
         <v>592</v>
       </c>
       <c r="AN14" s="112" t="s">
@@ -10436,7 +10443,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M15" s="646"/>
+      <c r="M15" s="668"/>
       <c r="N15" s="20"/>
       <c r="O15" s="210" t="s">
         <v>346</v>
@@ -10521,7 +10528,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M16" s="646"/>
+      <c r="M16" s="668"/>
       <c r="N16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10617,7 +10624,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M17" s="646"/>
+      <c r="M17" s="668"/>
       <c r="N17" s="20"/>
       <c r="O17" s="2" t="s">
         <v>348</v>
@@ -10700,7 +10707,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M18" s="646"/>
+      <c r="M18" s="668"/>
       <c r="N18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10785,7 +10792,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M19" s="646"/>
+      <c r="M19" s="668"/>
       <c r="N19" s="20"/>
       <c r="O19" s="2" t="s">
         <v>341</v>
@@ -10874,23 +10881,23 @@
       </c>
       <c r="J20" s="362"/>
       <c r="K20" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="311">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M20" s="647"/>
+      <c r="M20" s="669"/>
       <c r="N20" s="537" t="s">
         <v>342</v>
       </c>
-      <c r="O20" s="644"/>
+      <c r="O20" s="592"/>
       <c r="P20" s="334" t="s">
         <v>86</v>
       </c>
       <c r="Q20" s="164"/>
       <c r="R20" s="157">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S20" s="338">
         <v>-3</v>
@@ -10900,7 +10907,7 @@
       <c r="V20" s="142"/>
       <c r="W20" s="190">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20" s="314"/>
       <c r="Y20" s="117">
@@ -10909,7 +10916,7 @@
       </c>
       <c r="Z20" s="308">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA20" s="308">
         <v>1</v>
@@ -10931,7 +10938,7 @@
         <v>1</v>
       </c>
       <c r="AH20" s="158">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI20" s="326">
         <f t="shared" si="7"/>
@@ -10951,7 +10958,9 @@
       <c r="AM20" s="19" t="s">
         <v>465</v>
       </c>
-      <c r="AN20" s="112"/>
+      <c r="AN20" s="24" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="21" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="21" t="s">
@@ -11129,7 +11138,7 @@
       <c r="AN22" s="112"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="598" t="s">
+      <c r="E23" s="643" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="185">
@@ -11215,7 +11224,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="599"/>
+      <c r="E24" s="644"/>
       <c r="F24" s="177"/>
       <c r="I24" s="430" t="s">
         <v>301</v>
@@ -11233,7 +11242,7 @@
       <c r="N24" s="537" t="s">
         <v>342</v>
       </c>
-      <c r="O24" s="644"/>
+      <c r="O24" s="592"/>
       <c r="P24" s="334" t="s">
         <v>254</v>
       </c>
@@ -12234,7 +12243,7 @@
       <c r="I37" s="434"/>
       <c r="J37" s="371"/>
       <c r="K37" s="263">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" s="311">
         <f t="shared" si="10"/>
@@ -12248,7 +12257,7 @@
         <v>1</v>
       </c>
       <c r="R37" s="202">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S37" s="232">
         <v>-1</v>
@@ -12258,7 +12267,7 @@
       <c r="V37" s="202"/>
       <c r="W37" s="24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X37" s="65"/>
       <c r="Y37" s="117">
@@ -12267,7 +12276,7 @@
       </c>
       <c r="Z37" s="64">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA37" s="64">
         <v>1</v>
@@ -12306,27 +12315,32 @@
       <c r="AL37" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="AN37" s="112"/>
+      <c r="AM37" s="19" t="s">
+        <v>594</v>
+      </c>
+      <c r="AN37" s="24" t="s">
+        <v>593</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="M4:M20"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="S2:S3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="M4:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12363,12 +12377,12 @@
       <c r="B1" s="537" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="644"/>
+      <c r="C1" s="592"/>
       <c r="D1" s="214"/>
       <c r="J1" s="537" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="644"/>
+      <c r="K1" s="592"/>
       <c r="L1" s="205" t="s">
         <v>337</v>
       </c>
@@ -12759,7 +12773,7 @@
       <c r="V1" s="537" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="644"/>
+      <c r="W1" s="592"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12778,7 +12792,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="690" t="s">
+      <c r="AD1" s="683" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12795,10 +12809,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="721" t="s">
+      <c r="F2" s="682" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="678" t="s">
+      <c r="G2" s="710" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -12826,10 +12840,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="662" t="s">
+      <c r="V2" s="651" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="663"/>
+      <c r="W2" s="652"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -12848,7 +12862,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="691"/>
+      <c r="AD2" s="684"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -12867,8 +12881,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="595"/>
-      <c r="G3" s="679"/>
+      <c r="F3" s="640"/>
+      <c r="G3" s="711"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -12879,13 +12893,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="688" t="s">
+      <c r="O3" s="720" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="709" t="s">
+      <c r="P3" s="702" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="710"/>
+      <c r="Q3" s="703"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -12895,15 +12909,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="691"/>
+      <c r="AD3" s="684"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="679"/>
+      <c r="G4" s="711"/>
       <c r="H4" s="6"/>
       <c r="L4" s="673" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="689"/>
+      <c r="O4" s="721"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -12917,8 +12931,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="538"/>
-      <c r="AA4" s="644"/>
-      <c r="AD4" s="691"/>
+      <c r="AA4" s="592"/>
+      <c r="AD4" s="684"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -12933,21 +12947,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="679"/>
+      <c r="G5" s="711"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="696" t="s">
+      <c r="K5" s="689" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="711"/>
+      <c r="L5" s="704"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="689"/>
+      <c r="O5" s="721"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -12963,11 +12977,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="699" t="s">
+      <c r="Y5" s="692" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="700"/>
-      <c r="AD5" s="691"/>
+      <c r="Z5" s="693"/>
+      <c r="AD5" s="684"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -12977,16 +12991,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="679"/>
+      <c r="G6" s="711"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="697"/>
-      <c r="L6" s="711"/>
-      <c r="O6" s="689"/>
+      <c r="K6" s="690"/>
+      <c r="L6" s="704"/>
+      <c r="O6" s="721"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -12996,20 +13010,20 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="691"/>
+      <c r="AD6" s="684"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="679"/>
+      <c r="G7" s="711"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="697"/>
-      <c r="L7" s="711"/>
+      <c r="K7" s="690"/>
+      <c r="L7" s="704"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="689"/>
+      <c r="O7" s="721"/>
       <c r="P7" s="73"/>
-      <c r="AD7" s="691"/>
+      <c r="AD7" s="684"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13022,7 +13036,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="679"/>
+      <c r="G8" s="711"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13032,41 +13046,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="697"/>
-      <c r="L8" s="711"/>
-      <c r="O8" s="689"/>
+      <c r="K8" s="690"/>
+      <c r="L8" s="704"/>
+      <c r="O8" s="721"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="693" t="s">
+      <c r="S8" s="686" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="694"/>
-      <c r="U8" s="694"/>
-      <c r="V8" s="694"/>
-      <c r="W8" s="694"/>
-      <c r="X8" s="694"/>
-      <c r="Y8" s="694"/>
-      <c r="Z8" s="694"/>
-      <c r="AA8" s="694"/>
-      <c r="AB8" s="694"/>
-      <c r="AC8" s="695"/>
-      <c r="AD8" s="691"/>
+      <c r="T8" s="687"/>
+      <c r="U8" s="687"/>
+      <c r="V8" s="687"/>
+      <c r="W8" s="687"/>
+      <c r="X8" s="687"/>
+      <c r="Y8" s="687"/>
+      <c r="Z8" s="687"/>
+      <c r="AA8" s="687"/>
+      <c r="AB8" s="687"/>
+      <c r="AC8" s="688"/>
+      <c r="AD8" s="684"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="715"/>
-      <c r="G9" s="679"/>
+      <c r="C9" s="676"/>
+      <c r="G9" s="711"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="697"/>
-      <c r="L9" s="682" t="s">
+      <c r="K9" s="690"/>
+      <c r="L9" s="714" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="683"/>
-      <c r="N9" s="684"/>
-      <c r="O9" s="689"/>
+      <c r="M9" s="715"/>
+      <c r="N9" s="716"/>
+      <c r="O9" s="721"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="691"/>
+      <c r="AD9" s="684"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="716"/>
+      <c r="C10" s="677"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13074,7 +13088,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="679"/>
+      <c r="G10" s="711"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13082,33 +13096,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="697"/>
-      <c r="M10" s="718" t="s">
+      <c r="K10" s="690"/>
+      <c r="M10" s="679" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="719"/>
-      <c r="O10" s="719"/>
-      <c r="P10" s="719"/>
-      <c r="Q10" s="719"/>
-      <c r="R10" s="719"/>
-      <c r="S10" s="719"/>
-      <c r="T10" s="719"/>
-      <c r="U10" s="719"/>
-      <c r="V10" s="719"/>
-      <c r="W10" s="719"/>
-      <c r="X10" s="719"/>
-      <c r="Y10" s="719"/>
-      <c r="Z10" s="719"/>
-      <c r="AA10" s="719"/>
-      <c r="AB10" s="719"/>
-      <c r="AC10" s="720"/>
-      <c r="AD10" s="691"/>
+      <c r="N10" s="680"/>
+      <c r="O10" s="680"/>
+      <c r="P10" s="680"/>
+      <c r="Q10" s="680"/>
+      <c r="R10" s="680"/>
+      <c r="S10" s="680"/>
+      <c r="T10" s="680"/>
+      <c r="U10" s="680"/>
+      <c r="V10" s="680"/>
+      <c r="W10" s="680"/>
+      <c r="X10" s="680"/>
+      <c r="Y10" s="680"/>
+      <c r="Z10" s="680"/>
+      <c r="AA10" s="680"/>
+      <c r="AB10" s="680"/>
+      <c r="AC10" s="681"/>
+      <c r="AD10" s="684"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="717"/>
-      <c r="G11" s="679"/>
+      <c r="C11" s="678"/>
+      <c r="G11" s="711"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="697"/>
+      <c r="K11" s="690"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13119,17 +13133,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="707" t="s">
+      <c r="Z11" s="700" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="708"/>
+      <c r="AA11" s="701"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="691"/>
+      <c r="AD11" s="684"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13142,7 +13156,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="679"/>
+      <c r="G12" s="711"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13150,8 +13164,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="697"/>
-      <c r="L12" s="712" t="s">
+      <c r="K12" s="690"/>
+      <c r="L12" s="705" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13182,25 +13196,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="701" t="s">
+      <c r="AA12" s="694" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="702"/>
+      <c r="AB12" s="695"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="691"/>
+      <c r="AD12" s="684"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="715"/>
-      <c r="G13" s="679"/>
-      <c r="K13" s="697"/>
-      <c r="L13" s="713"/>
+      <c r="C13" s="676"/>
+      <c r="G13" s="711"/>
+      <c r="K13" s="690"/>
+      <c r="L13" s="706"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="681" t="s">
+      <c r="Q13" s="713" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="604"/>
+      <c r="R13" s="607"/>
       <c r="S13" s="533"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13209,17 +13223,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="703"/>
-      <c r="AB13" s="704"/>
-      <c r="AD13" s="691"/>
+      <c r="AA13" s="696"/>
+      <c r="AB13" s="697"/>
+      <c r="AD13" s="684"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="717"/>
+      <c r="C14" s="678"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="679"/>
+      <c r="G14" s="711"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13227,8 +13241,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="697"/>
-      <c r="L14" s="713"/>
+      <c r="K14" s="690"/>
+      <c r="L14" s="706"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13249,9 +13263,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="703"/>
-      <c r="AB14" s="704"/>
-      <c r="AD14" s="691"/>
+      <c r="AA14" s="696"/>
+      <c r="AB14" s="697"/>
+      <c r="AD14" s="684"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13266,19 +13280,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="679"/>
+      <c r="G15" s="711"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="697"/>
-      <c r="L15" s="714"/>
-      <c r="Q15" s="681" t="s">
+      <c r="K15" s="690"/>
+      <c r="L15" s="707"/>
+      <c r="Q15" s="713" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="604"/>
+      <c r="R15" s="607"/>
       <c r="S15" s="533"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13287,14 +13301,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="703"/>
-      <c r="AB15" s="704"/>
-      <c r="AD15" s="691"/>
+      <c r="AA15" s="696"/>
+      <c r="AB15" s="697"/>
+      <c r="AD15" s="684"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="679"/>
-      <c r="K16" s="697"/>
+      <c r="G16" s="711"/>
+      <c r="K16" s="690"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13313,24 +13327,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="703"/>
-      <c r="AB16" s="704"/>
-      <c r="AD16" s="691"/>
+      <c r="AA16" s="696"/>
+      <c r="AB16" s="697"/>
+      <c r="AD16" s="684"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="676" t="s">
+      <c r="F17" s="708" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="679"/>
+      <c r="G17" s="711"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="697"/>
+      <c r="K17" s="690"/>
       <c r="S17" s="533"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13338,9 +13352,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="703"/>
-      <c r="AB17" s="704"/>
-      <c r="AD17" s="691"/>
+      <c r="AA17" s="696"/>
+      <c r="AB17" s="697"/>
+      <c r="AD17" s="684"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13350,15 +13364,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="677"/>
-      <c r="G18" s="679"/>
+      <c r="F18" s="709"/>
+      <c r="G18" s="711"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="697"/>
+      <c r="K18" s="690"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13369,39 +13383,42 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="705"/>
-      <c r="AB18" s="706"/>
-      <c r="AD18" s="691"/>
+      <c r="AA18" s="698"/>
+      <c r="AB18" s="699"/>
+      <c r="AD18" s="684"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="680"/>
-      <c r="K19" s="698"/>
+      <c r="G19" s="712"/>
+      <c r="K19" s="691"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="685" t="s">
+      <c r="R19" s="717" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="686"/>
-      <c r="T19" s="687"/>
+      <c r="S19" s="718"/>
+      <c r="T19" s="719"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="692"/>
+      <c r="AD19" s="685"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13413,14 +13430,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Boat Enabled - Zee N , Manorama , TBS News
Boat Enabled - Zee N
MatriX_TF_V - 4
MatriX_TF_CreditLoad - -3
</commit_message>
<xml_diff>
--- a/System_2.1.3.xlsx
+++ b/System_2.1.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3D366D-3E67-47A3-ADBC-C8F9DD032A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35ED1BCB-36B4-45D2-B3AC-89E8FC054F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="596">
   <si>
     <t>Zone</t>
   </si>
@@ -1824,6 +1824,9 @@
   </si>
   <si>
     <t>Boat Node</t>
+  </si>
+  <si>
+    <t>Credit Load</t>
   </si>
 </sst>
 </file>
@@ -3410,7 +3413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="723">
+  <cellXfs count="724">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4675,6 +4678,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4720,6 +4726,63 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4750,62 +4813,167 @@
     <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4831,12 +4999,6 @@
     <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4858,161 +5020,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5056,39 +5095,6 @@
     <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5107,25 +5113,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5203,51 +5230,28 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5593,10 +5597,10 @@
       <c r="I2" s="443" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="535" t="s">
+      <c r="J2" s="536" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="536"/>
+      <c r="K2" s="537"/>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5606,13 +5610,13 @@
       <c r="N2" s="386" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="537" t="s">
+      <c r="O2" s="538" t="s">
         <v>385</v>
       </c>
-      <c r="P2" s="538"/>
-      <c r="Q2" s="538"/>
-      <c r="R2" s="538"/>
-      <c r="S2" s="539" t="s">
+      <c r="P2" s="539"/>
+      <c r="Q2" s="539"/>
+      <c r="R2" s="539"/>
+      <c r="S2" s="540" t="s">
         <v>386</v>
       </c>
       <c r="U2" s="2" t="s">
@@ -5626,7 +5630,7 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="532"/>
+      <c r="D3" s="533"/>
       <c r="E3" s="374"/>
       <c r="F3" s="281" t="s">
         <v>69</v>
@@ -5651,7 +5655,7 @@
       </c>
       <c r="O3" s="6"/>
       <c r="R3" s="6"/>
-      <c r="S3" s="540"/>
+      <c r="S3" s="541"/>
     </row>
     <row r="4" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -5660,7 +5664,7 @@
       <c r="C4" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="D4" s="533"/>
+      <c r="D4" s="534"/>
       <c r="E4" s="61"/>
       <c r="F4" s="396" t="s">
         <v>42</v>
@@ -5677,7 +5681,7 @@
       </c>
       <c r="O4" s="6"/>
       <c r="R4" s="6"/>
-      <c r="S4" s="540"/>
+      <c r="S4" s="541"/>
     </row>
     <row r="5" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -5686,7 +5690,7 @@
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="534"/>
+      <c r="D5" s="535"/>
       <c r="F5" s="401" t="s">
         <v>42</v>
       </c>
@@ -5710,7 +5714,7 @@
       <c r="Q5" s="19">
         <v>5280</v>
       </c>
-      <c r="S5" s="540"/>
+      <c r="S5" s="541"/>
     </row>
     <row r="6" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -5742,7 +5746,7 @@
       </c>
       <c r="P6" s="16"/>
       <c r="Q6" s="6"/>
-      <c r="S6" s="540"/>
+      <c r="S6" s="541"/>
     </row>
     <row r="7" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="219" t="s">
@@ -5772,7 +5776,7 @@
       </c>
       <c r="P7" s="16"/>
       <c r="Q7" s="6"/>
-      <c r="S7" s="540"/>
+      <c r="S7" s="541"/>
     </row>
     <row r="8" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -5800,7 +5804,7 @@
       </c>
       <c r="P8" s="16"/>
       <c r="Q8" s="6"/>
-      <c r="S8" s="540"/>
+      <c r="S8" s="541"/>
     </row>
     <row r="9" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -5833,7 +5837,7 @@
       <c r="O9" s="256" t="s">
         <v>44</v>
       </c>
-      <c r="S9" s="540"/>
+      <c r="S9" s="541"/>
     </row>
     <row r="10" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -5868,7 +5872,7 @@
       <c r="Q10" s="64">
         <v>88</v>
       </c>
-      <c r="S10" s="540"/>
+      <c r="S10" s="541"/>
     </row>
     <row r="11" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -5902,7 +5906,7 @@
       </c>
       <c r="P11" s="16"/>
       <c r="Q11" s="142"/>
-      <c r="S11" s="540"/>
+      <c r="S11" s="541"/>
       <c r="T11" s="23"/>
     </row>
     <row r="12" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5929,7 +5933,7 @@
       </c>
       <c r="P12" s="16"/>
       <c r="Q12" s="142"/>
-      <c r="S12" s="540"/>
+      <c r="S12" s="541"/>
     </row>
     <row r="13" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="271" t="s">
@@ -5963,10 +5967,10 @@
       <c r="N13" s="404" t="s">
         <v>522</v>
       </c>
-      <c r="S13" s="540"/>
+      <c r="S13" s="541"/>
     </row>
     <row r="14" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S14" s="540"/>
+      <c r="S14" s="541"/>
     </row>
     <row r="15" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -5992,17 +5996,17 @@
       <c r="L15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="544">
+      <c r="M15" s="545">
         <v>45275</v>
       </c>
-      <c r="N15" s="532" t="s">
+      <c r="N15" s="533" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="256" t="s">
         <v>44</v>
       </c>
       <c r="R15" s="6"/>
-      <c r="S15" s="540"/>
+      <c r="S15" s="541"/>
     </row>
     <row r="16" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="514" t="s">
@@ -6028,9 +6032,9 @@
       <c r="L16" s="204" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="545"/>
-      <c r="N16" s="533"/>
-      <c r="S16" s="540"/>
+      <c r="M16" s="546"/>
+      <c r="N16" s="534"/>
+      <c r="S16" s="541"/>
     </row>
     <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -6058,15 +6062,15 @@
       <c r="L17" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="546"/>
-      <c r="N17" s="534"/>
+      <c r="M17" s="547"/>
+      <c r="N17" s="535"/>
       <c r="O17" s="256" t="s">
         <v>44</v>
       </c>
-      <c r="S17" s="540"/>
+      <c r="S17" s="541"/>
     </row>
     <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S18" s="540"/>
+      <c r="S18" s="541"/>
     </row>
     <row r="19" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -6094,13 +6098,13 @@
       <c r="L19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="544">
+      <c r="M19" s="545">
         <v>45275</v>
       </c>
       <c r="N19" s="442" t="s">
         <v>522</v>
       </c>
-      <c r="S19" s="540"/>
+      <c r="S19" s="541"/>
     </row>
     <row r="20" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="254" t="s">
@@ -6126,11 +6130,11 @@
       <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="545"/>
+      <c r="M20" s="546"/>
       <c r="N20" s="431" t="s">
         <v>26</v>
       </c>
-      <c r="S20" s="540"/>
+      <c r="S20" s="541"/>
     </row>
     <row r="21" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="254" t="s">
@@ -6156,15 +6160,15 @@
       <c r="L21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="545"/>
+      <c r="M21" s="546"/>
       <c r="N21" s="431" t="s">
         <v>18</v>
       </c>
-      <c r="P21" s="542" t="s">
+      <c r="P21" s="543" t="s">
         <v>226</v>
       </c>
-      <c r="Q21" s="543"/>
-      <c r="S21" s="540"/>
+      <c r="Q21" s="544"/>
+      <c r="S21" s="541"/>
     </row>
     <row r="22" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="288" t="s">
@@ -6190,11 +6194,11 @@
       <c r="L22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="545"/>
+      <c r="M22" s="546"/>
       <c r="N22" s="410" t="s">
         <v>26</v>
       </c>
-      <c r="S22" s="540"/>
+      <c r="S22" s="541"/>
     </row>
     <row r="23" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
@@ -6220,11 +6224,11 @@
       <c r="L23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="545"/>
+      <c r="M23" s="546"/>
       <c r="N23" s="61" t="s">
         <v>523</v>
       </c>
-      <c r="S23" s="540"/>
+      <c r="S23" s="541"/>
     </row>
     <row r="24" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
@@ -6250,7 +6254,7 @@
       <c r="L24" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="545"/>
+      <c r="M24" s="546"/>
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
@@ -6258,7 +6262,7 @@
         <v>44</v>
       </c>
       <c r="R24" s="16"/>
-      <c r="S24" s="540"/>
+      <c r="S24" s="541"/>
     </row>
     <row r="25" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
@@ -6284,11 +6288,11 @@
       <c r="L25" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="545"/>
+      <c r="M25" s="546"/>
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="S25" s="540"/>
+      <c r="S25" s="541"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
@@ -6314,11 +6318,11 @@
       <c r="L26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="545"/>
+      <c r="M26" s="546"/>
       <c r="N26" s="61" t="s">
         <v>524</v>
       </c>
-      <c r="S26" s="540"/>
+      <c r="S26" s="541"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="271" t="s">
@@ -6340,9 +6344,9 @@
       <c r="J27" s="439"/>
       <c r="K27" s="440"/>
       <c r="L27" s="441"/>
-      <c r="M27" s="545"/>
+      <c r="M27" s="546"/>
       <c r="N27" s="61"/>
-      <c r="S27" s="540"/>
+      <c r="S27" s="541"/>
     </row>
     <row r="28" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="271" t="s">
@@ -6370,12 +6374,12 @@
       <c r="L28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="546"/>
+      <c r="M28" s="547"/>
       <c r="N28" s="61" t="s">
         <v>524</v>
       </c>
       <c r="R28" s="16"/>
-      <c r="S28" s="541"/>
+      <c r="S28" s="542"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6396,8 +6400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView topLeftCell="M10" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6452,7 +6456,7 @@
       <c r="P1" s="450" t="s">
         <v>408</v>
       </c>
-      <c r="Q1" s="547" t="s">
+      <c r="Q1" s="567" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6461,34 +6465,37 @@
       <c r="S1" s="100" t="s">
         <v>81</v>
       </c>
+      <c r="T1" s="21" t="s">
+        <v>595</v>
+      </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="560">
+      <c r="A2" s="551">
         <f ca="1">TODAY()</f>
         <v>45277</v>
       </c>
-      <c r="B2" s="562" t="s">
+      <c r="B2" s="553" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="574" t="s">
+      <c r="C2" s="565" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="564" t="s">
+      <c r="D2" s="555" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="566" t="s">
+      <c r="E2" s="557" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="201" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="572" t="s">
+      <c r="G2" s="563" t="s">
         <v>381</v>
       </c>
       <c r="H2" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="554" t="s">
+      <c r="I2" s="574" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="448" t="s">
@@ -6512,7 +6519,7 @@
       <c r="P2" s="451">
         <v>40</v>
       </c>
-      <c r="Q2" s="548"/>
+      <c r="Q2" s="568"/>
       <c r="R2" s="21">
         <f>R7+R18</f>
         <v>8</v>
@@ -6521,18 +6528,22 @@
         <f>S7+S18</f>
         <v>5</v>
       </c>
+      <c r="T2" s="177">
+        <f>SUM(T4:T16)</f>
+        <v>-3</v>
+      </c>
       <c r="V2" s="520"/>
       <c r="X2" s="524"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="561"/>
-      <c r="B3" s="563"/>
-      <c r="C3" s="575"/>
-      <c r="D3" s="565"/>
-      <c r="E3" s="567"/>
-      <c r="G3" s="573"/>
+      <c r="A3" s="552"/>
+      <c r="B3" s="554"/>
+      <c r="C3" s="566"/>
+      <c r="D3" s="556"/>
+      <c r="E3" s="558"/>
+      <c r="G3" s="564"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="555"/>
+      <c r="I3" s="575"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6551,16 +6562,16 @@
         <v>390</v>
       </c>
       <c r="B4" s="257"/>
-      <c r="C4" s="568" t="s">
+      <c r="C4" s="559" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="555"/>
+      <c r="I4" s="575"/>
       <c r="R4" s="527" t="s">
         <v>585</v>
       </c>
-      <c r="T4" s="20">
+      <c r="T4" s="24">
         <f>IF((R7-SUM(V2:V10)&lt;0),R7-SUM(V2:V10),0)</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="V4" s="521"/>
       <c r="X4" s="525"/>
@@ -6572,7 +6583,7 @@
       <c r="B5" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="569"/>
+      <c r="C5" s="560"/>
       <c r="D5" s="235" t="s">
         <v>103</v>
       </c>
@@ -6582,13 +6593,13 @@
       <c r="F5" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="532" t="s">
+      <c r="G5" s="533" t="s">
         <v>276</v>
       </c>
       <c r="H5" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="555"/>
+      <c r="I5" s="575"/>
       <c r="J5" s="449" t="s">
         <v>273</v>
       </c>
@@ -6607,33 +6618,38 @@
       <c r="S5" s="527" t="s">
         <v>585</v>
       </c>
-      <c r="T5" s="20">
+      <c r="T5" s="24">
         <f>IF((S7-SUM(X2:X10))&lt;0,S7-SUM(X2:X10),0)</f>
         <v>0</v>
       </c>
-      <c r="V5" s="523"/>
+      <c r="U5" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="V5" s="523">
+        <v>1</v>
+      </c>
       <c r="W5" s="6"/>
       <c r="X5" s="523">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="557" t="s">
+      <c r="A6" s="548" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="570"/>
-      <c r="D6" s="571"/>
+      <c r="C6" s="561"/>
+      <c r="D6" s="562"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
-      <c r="G6" s="533"/>
-      <c r="I6" s="555"/>
+      <c r="G6" s="534"/>
+      <c r="I6" s="575"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="558"/>
+      <c r="A7" s="549"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -6643,8 +6659,8 @@
       <c r="D7" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="533"/>
-      <c r="I7" s="555"/>
+      <c r="G7" s="534"/>
+      <c r="I7" s="575"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -6682,7 +6698,7 @@
       </c>
     </row>
     <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="559"/>
+      <c r="A8" s="550"/>
       <c r="B8" s="222" t="s">
         <v>28</v>
       </c>
@@ -6690,13 +6706,13 @@
       <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="533"/>
-      <c r="I8" s="555"/>
+      <c r="G8" s="534"/>
+      <c r="I8" s="575"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="V8" s="525">
+      <c r="V8" s="24">
         <v>1</v>
       </c>
       <c r="W8" s="6"/>
@@ -6715,9 +6731,9 @@
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="533"/>
+      <c r="G9" s="534"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="555"/>
+      <c r="I9" s="575"/>
       <c r="M9" s="19" t="s">
         <v>548</v>
       </c>
@@ -6725,7 +6741,7 @@
       <c r="U9" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="V9" s="525">
+      <c r="V9" s="24">
         <v>1</v>
       </c>
       <c r="X9" s="521"/>
@@ -6741,10 +6757,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!S8</f>
-        <v>42</v>
-      </c>
-      <c r="G10" s="533"/>
-      <c r="I10" s="555"/>
+        <v>40</v>
+      </c>
+      <c r="G10" s="534"/>
+      <c r="I10" s="575"/>
       <c r="J10" s="24" t="s">
         <v>381</v>
       </c>
@@ -6755,14 +6771,19 @@
         <v>547</v>
       </c>
       <c r="N10" s="80"/>
-      <c r="V10" s="521"/>
+      <c r="U10" s="723" t="s">
+        <v>254</v>
+      </c>
+      <c r="V10" s="525">
+        <v>1</v>
+      </c>
       <c r="X10" s="521"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="532" t="s">
+      <c r="B11" s="533" t="s">
         <v>392</v>
       </c>
       <c r="C11" s="176" t="s">
@@ -6771,8 +6792,8 @@
       <c r="D11" s="229" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="533"/>
-      <c r="I11" s="555"/>
+      <c r="G11" s="534"/>
+      <c r="I11" s="575"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -6798,23 +6819,23 @@
       <c r="S11" s="24">
         <v>2</v>
       </c>
-      <c r="U11" s="549" t="s">
+      <c r="U11" s="569" t="s">
         <v>588</v>
       </c>
-      <c r="V11" s="550"/>
-      <c r="W11" s="550"/>
-      <c r="X11" s="551"/>
+      <c r="V11" s="570"/>
+      <c r="W11" s="570"/>
+      <c r="X11" s="571"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="240" t="s">
         <v>393</v>
       </c>
-      <c r="B12" s="534"/>
+      <c r="B12" s="535"/>
       <c r="E12" s="242">
         <v>3</v>
       </c>
-      <c r="G12" s="533"/>
-      <c r="I12" s="555"/>
+      <c r="G12" s="534"/>
+      <c r="I12" s="575"/>
       <c r="J12" s="24" t="s">
         <v>539</v>
       </c>
@@ -6842,12 +6863,12 @@
       <c r="B13" s="227" t="s">
         <v>330</v>
       </c>
-      <c r="C13" s="532" t="s">
+      <c r="C13" s="533" t="s">
         <v>195</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="G13" s="533"/>
-      <c r="I13" s="555"/>
+      <c r="G13" s="534"/>
+      <c r="I13" s="575"/>
       <c r="J13" s="108" t="s">
         <v>577</v>
       </c>
@@ -6874,7 +6895,7 @@
       <c r="B14" s="178" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="534"/>
+      <c r="C14" s="535"/>
       <c r="D14" s="214" t="s">
         <v>154</v>
       </c>
@@ -6884,11 +6905,11 @@
       <c r="F14" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="G14" s="534"/>
+      <c r="G14" s="535"/>
       <c r="H14" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="555"/>
+      <c r="I14" s="575"/>
       <c r="U14" s="6"/>
       <c r="V14" s="112"/>
       <c r="W14" s="6"/>
@@ -6906,7 +6927,7 @@
       <c r="H15" s="289">
         <v>0</v>
       </c>
-      <c r="I15" s="555"/>
+      <c r="I15" s="575"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -6924,7 +6945,7 @@
       </c>
       <c r="T15" s="24">
         <f>IF((R18-SUM(V18:V23))&lt;0,R18-SUM(V18:V23),0)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="U15" s="6"/>
       <c r="V15" s="112"/>
@@ -6937,7 +6958,7 @@
       <c r="D16" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="I16" s="555"/>
+      <c r="I16" s="575"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -6971,7 +6992,7 @@
       <c r="G17" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I17" s="555"/>
+      <c r="I17" s="575"/>
       <c r="L17" s="2" t="s">
         <v>444</v>
       </c>
@@ -6983,13 +7004,13 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="555"/>
+      <c r="I18" s="575"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="552" t="s">
+      <c r="O18" s="572" t="s">
         <v>540</v>
       </c>
-      <c r="P18" s="553"/>
+      <c r="P18" s="573"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7015,7 +7036,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="555"/>
+      <c r="I19" s="575"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
@@ -7047,7 +7068,7 @@
       <c r="G20" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I20" s="555"/>
+      <c r="I20" s="575"/>
       <c r="K20" s="19" t="s">
         <v>440</v>
       </c>
@@ -7072,7 +7093,7 @@
       <c r="Z20" s="6"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="555"/>
+      <c r="I21" s="575"/>
       <c r="M21" s="227" t="s">
         <v>422</v>
       </c>
@@ -7106,7 +7127,7 @@
       <c r="G22" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="I22" s="555"/>
+      <c r="I22" s="575"/>
       <c r="U22" s="6" t="s">
         <v>589</v>
       </c>
@@ -7130,17 +7151,17 @@
       <c r="E23" s="301" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="555"/>
+      <c r="I23" s="575"/>
       <c r="U23" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V23" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="555"/>
+      <c r="I24" s="575"/>
       <c r="U24" s="379"/>
       <c r="V24" s="526">
         <v>-1</v>
@@ -7168,7 +7189,7 @@
       <c r="H25" s="201" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="555"/>
+      <c r="I25" s="575"/>
       <c r="J25" s="449" t="s">
         <v>274</v>
       </c>
@@ -7182,7 +7203,12 @@
         <v>1</v>
       </c>
       <c r="U25" s="35"/>
-      <c r="W25" s="19"/>
+      <c r="V25" s="100">
+        <v>8</v>
+      </c>
+      <c r="W25" s="19" t="s">
+        <v>486</v>
+      </c>
       <c r="X25" s="530" t="s">
         <v>44</v>
       </c>
@@ -7208,7 +7234,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="555"/>
+      <c r="I26" s="575"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7243,7 +7269,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="555"/>
+      <c r="I27" s="575"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7270,7 +7296,7 @@
       <c r="E28" s="226">
         <v>2</v>
       </c>
-      <c r="I28" s="555"/>
+      <c r="I28" s="575"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7292,7 +7318,7 @@
       <c r="H29" s="201" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="556"/>
+      <c r="I29" s="576"/>
       <c r="J29" s="358"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7330,12 +7356,17 @@
       <c r="W30" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="X30" s="722">
+      <c r="X30" s="532">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
     <mergeCell ref="A2:A3"/>
@@ -7347,11 +7378,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7427,7 +7453,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="572" t="s">
+      <c r="I1" s="563" t="s">
         <v>378</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -7463,7 +7489,7 @@
       <c r="X1" s="482" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="618" t="s">
+      <c r="Y1" s="619" t="s">
         <v>555</v>
       </c>
       <c r="Z1" s="458">
@@ -7488,7 +7514,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="454"/>
-      <c r="AN1" s="603"/>
+      <c r="AN1" s="601"/>
       <c r="AO1" s="375" t="s">
         <v>487</v>
       </c>
@@ -7497,23 +7523,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="627">
+      <c r="A2" s="583">
         <f ca="1">TODAY()</f>
         <v>45277</v>
       </c>
-      <c r="B2" s="629" t="s">
+      <c r="B2" s="585" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="574" t="s">
+      <c r="C2" s="565" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="631" t="s">
+      <c r="D2" s="587" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="576" t="s">
+      <c r="E2" s="631" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="584" t="s">
+      <c r="F2" s="606" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="445" t="s">
@@ -7522,15 +7548,15 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="573"/>
+      <c r="I2" s="564"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="578" t="s">
+      <c r="K2" s="633" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="579"/>
-      <c r="M2" s="584" t="s">
+      <c r="L2" s="634"/>
+      <c r="M2" s="606" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
@@ -7542,11 +7568,11 @@
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="574" t="s">
+      <c r="Q2" s="565" t="s">
         <v>144</v>
       </c>
-      <c r="R2" s="532"/>
-      <c r="S2" s="597" t="s">
+      <c r="R2" s="533"/>
+      <c r="S2" s="623" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7556,7 +7582,7 @@
       <c r="X2" s="483" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="619"/>
+      <c r="Y2" s="620"/>
       <c r="Z2" s="459">
         <v>1</v>
       </c>
@@ -7579,15 +7605,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="480"/>
-      <c r="AN2" s="604"/>
+      <c r="AN2" s="602"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="628"/>
-      <c r="B3" s="630"/>
-      <c r="C3" s="575"/>
-      <c r="D3" s="632"/>
-      <c r="E3" s="577"/>
-      <c r="F3" s="585"/>
+      <c r="A3" s="584"/>
+      <c r="B3" s="586"/>
+      <c r="C3" s="566"/>
+      <c r="D3" s="588"/>
+      <c r="E3" s="632"/>
+      <c r="F3" s="607"/>
       <c r="G3" s="446" t="s">
         <v>28</v>
       </c>
@@ -7606,7 +7632,7 @@
       <c r="L3" s="211" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="585"/>
+      <c r="M3" s="607"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
@@ -7614,9 +7640,9 @@
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="575"/>
-      <c r="R3" s="534"/>
-      <c r="S3" s="599"/>
+      <c r="Q3" s="566"/>
+      <c r="R3" s="535"/>
+      <c r="S3" s="624"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7624,7 +7650,7 @@
       <c r="X3" s="483" t="s">
         <v>158</v>
       </c>
-      <c r="Y3" s="619"/>
+      <c r="Y3" s="620"/>
       <c r="Z3" s="460">
         <v>1</v>
       </c>
@@ -7633,7 +7659,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="594" t="s">
+      <c r="AD3" s="622" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="272"/>
@@ -7645,16 +7671,16 @@
       <c r="AK3" s="272"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="480"/>
-      <c r="AN3" s="604"/>
+      <c r="AN3" s="602"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="251" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="643" t="s">
+      <c r="B4" s="599" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="574" t="s">
+      <c r="C4" s="565" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="384" t="s">
@@ -7663,7 +7689,7 @@
       <c r="E4" s="422">
         <v>1</v>
       </c>
-      <c r="F4" s="585"/>
+      <c r="F4" s="607"/>
       <c r="G4" s="427" t="s">
         <v>203</v>
       </c>
@@ -7680,7 +7706,7 @@
         <v>151</v>
       </c>
       <c r="L4" s="214"/>
-      <c r="M4" s="585"/>
+      <c r="M4" s="607"/>
       <c r="N4" s="179" t="s">
         <v>70</v>
       </c>
@@ -7706,12 +7732,12 @@
       <c r="X4" s="483" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="619"/>
+      <c r="Y4" s="620"/>
       <c r="Z4" s="461"/>
       <c r="AA4" s="325"/>
       <c r="AB4" s="219"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="594"/>
+      <c r="AD4" s="622"/>
       <c r="AE4" s="272"/>
       <c r="AF4" s="272"/>
       <c r="AG4" s="16"/>
@@ -7721,33 +7747,33 @@
       <c r="AK4" s="272"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="480"/>
-      <c r="AN4" s="604"/>
+      <c r="AN4" s="602"/>
       <c r="AO4" s="375" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="572" t="s">
+      <c r="A5" s="563" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="644"/>
-      <c r="C5" s="575"/>
+      <c r="B5" s="600"/>
+      <c r="C5" s="566"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="423">
         <v>1</v>
       </c>
-      <c r="F5" s="585"/>
-      <c r="G5" s="635" t="s">
+      <c r="F5" s="607"/>
+      <c r="G5" s="591" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="635"/>
-      <c r="I5" s="635"/>
-      <c r="J5" s="635"/>
-      <c r="K5" s="635"/>
-      <c r="L5" s="636"/>
-      <c r="M5" s="585"/>
+      <c r="H5" s="591"/>
+      <c r="I5" s="591"/>
+      <c r="J5" s="591"/>
+      <c r="K5" s="591"/>
+      <c r="L5" s="592"/>
+      <c r="M5" s="607"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
@@ -7759,7 +7785,7 @@
       <c r="X5" s="483" t="s">
         <v>160</v>
       </c>
-      <c r="Y5" s="619"/>
+      <c r="Y5" s="620"/>
       <c r="Z5" s="461">
         <v>1</v>
       </c>
@@ -7782,23 +7808,23 @@
       <c r="AK5" s="272"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="480"/>
-      <c r="AN5" s="604"/>
+      <c r="AN5" s="602"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="573"/>
-      <c r="B6" s="641" t="s">
+      <c r="A6" s="564"/>
+      <c r="B6" s="597" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="570"/>
-      <c r="D6" s="571"/>
-      <c r="F6" s="585"/>
-      <c r="G6" s="637"/>
-      <c r="H6" s="637"/>
-      <c r="I6" s="637"/>
-      <c r="J6" s="637"/>
-      <c r="K6" s="637"/>
-      <c r="L6" s="638"/>
-      <c r="M6" s="585"/>
+      <c r="C6" s="561"/>
+      <c r="D6" s="562"/>
+      <c r="F6" s="607"/>
+      <c r="G6" s="593"/>
+      <c r="H6" s="593"/>
+      <c r="I6" s="593"/>
+      <c r="J6" s="593"/>
+      <c r="K6" s="593"/>
+      <c r="L6" s="594"/>
+      <c r="M6" s="607"/>
       <c r="O6" s="611"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
@@ -7809,7 +7835,7 @@
       <c r="X6" s="483" t="s">
         <v>161</v>
       </c>
-      <c r="Y6" s="619"/>
+      <c r="Y6" s="620"/>
       <c r="Z6" s="459">
         <v>1</v>
       </c>
@@ -7823,16 +7849,16 @@
       <c r="AF6" s="272"/>
       <c r="AG6" s="272"/>
       <c r="AH6" s="272"/>
-      <c r="AI6" s="593"/>
+      <c r="AI6" s="616"/>
       <c r="AJ6" s="493" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="593" t="s">
+      <c r="AK6" s="616" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="272"/>
       <c r="AM6" s="480"/>
-      <c r="AN6" s="604"/>
+      <c r="AN6" s="602"/>
       <c r="AO6" s="375" t="s">
         <v>488</v>
       </c>
@@ -7841,7 +7867,7 @@
       <c r="A7" s="245" t="s">
         <v>552</v>
       </c>
-      <c r="B7" s="642"/>
+      <c r="B7" s="598"/>
       <c r="C7" s="212" t="s">
         <v>383</v>
       </c>
@@ -7851,7 +7877,7 @@
       <c r="E7" s="281">
         <v>3</v>
       </c>
-      <c r="F7" s="585"/>
+      <c r="F7" s="607"/>
       <c r="G7" s="447">
         <v>0</v>
       </c>
@@ -7864,13 +7890,13 @@
       <c r="J7" s="30">
         <v>0</v>
       </c>
-      <c r="K7" s="532">
+      <c r="K7" s="533">
         <v>1</v>
       </c>
       <c r="L7" s="222">
         <v>0</v>
       </c>
-      <c r="M7" s="585"/>
+      <c r="M7" s="607"/>
       <c r="O7" s="611"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
@@ -7885,7 +7911,7 @@
       <c r="X7" s="483" t="s">
         <v>162</v>
       </c>
-      <c r="Y7" s="619"/>
+      <c r="Y7" s="620"/>
       <c r="Z7" s="459">
         <v>1</v>
       </c>
@@ -7895,18 +7921,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="272"/>
       <c r="AF7" s="272"/>
-      <c r="AG7" s="594" t="s">
+      <c r="AG7" s="622" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="272"/>
-      <c r="AI7" s="593"/>
+      <c r="AI7" s="616"/>
       <c r="AJ7" s="272"/>
-      <c r="AK7" s="593"/>
+      <c r="AK7" s="616"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="480"/>
-      <c r="AN7" s="604"/>
+      <c r="AN7" s="602"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -7923,23 +7949,23 @@
         <f>SUM(G7:N9)</f>
         <v>16</v>
       </c>
-      <c r="F8" s="585"/>
-      <c r="G8" s="636">
-        <v>0</v>
-      </c>
-      <c r="H8" s="633" t="s">
+      <c r="F8" s="607"/>
+      <c r="G8" s="592">
+        <v>0</v>
+      </c>
+      <c r="H8" s="589" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="532">
-        <v>0</v>
-      </c>
-      <c r="J8" s="633" t="s">
+      <c r="I8" s="533">
+        <v>0</v>
+      </c>
+      <c r="J8" s="589" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="639"/>
-      <c r="L8" s="595"/>
+      <c r="K8" s="595"/>
+      <c r="L8" s="625"/>
       <c r="M8" s="608"/>
-      <c r="N8" s="600">
+      <c r="N8" s="628">
         <f>N5+N11</f>
         <v>15</v>
       </c>
@@ -7953,7 +7979,7 @@
       <c r="X8" s="483" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="619"/>
+      <c r="Y8" s="620"/>
       <c r="Z8" s="461"/>
       <c r="AA8" s="325"/>
       <c r="AB8" s="219"/>
@@ -7961,14 +7987,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="272"/>
       <c r="AF8" s="272"/>
-      <c r="AG8" s="594"/>
+      <c r="AG8" s="622"/>
       <c r="AH8" s="272"/>
-      <c r="AI8" s="593"/>
+      <c r="AI8" s="616"/>
       <c r="AJ8" s="272"/>
       <c r="AK8" s="272"/>
       <c r="AL8" s="272"/>
       <c r="AM8" s="480"/>
-      <c r="AN8" s="604"/>
+      <c r="AN8" s="602"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="245" t="s">
@@ -7983,17 +8009,17 @@
       <c r="D9" s="385" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="585"/>
-      <c r="G9" s="638"/>
-      <c r="H9" s="634"/>
-      <c r="I9" s="534"/>
-      <c r="J9" s="634"/>
-      <c r="K9" s="640"/>
-      <c r="L9" s="596"/>
+      <c r="F9" s="607"/>
+      <c r="G9" s="594"/>
+      <c r="H9" s="590"/>
+      <c r="I9" s="535"/>
+      <c r="J9" s="590"/>
+      <c r="K9" s="596"/>
+      <c r="L9" s="626"/>
       <c r="M9" s="609"/>
-      <c r="N9" s="601"/>
+      <c r="N9" s="629"/>
       <c r="O9" s="612"/>
-      <c r="S9" s="597" t="s">
+      <c r="S9" s="623" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8005,7 +8031,7 @@
       <c r="X9" s="483" t="s">
         <v>164</v>
       </c>
-      <c r="Y9" s="619"/>
+      <c r="Y9" s="620"/>
       <c r="Z9" s="462"/>
       <c r="AA9" s="325"/>
       <c r="AB9" s="219"/>
@@ -8015,16 +8041,16 @@
       </c>
       <c r="AE9" s="272"/>
       <c r="AF9" s="272"/>
-      <c r="AG9" s="594"/>
+      <c r="AG9" s="622"/>
       <c r="AH9" s="272"/>
-      <c r="AI9" s="593"/>
+      <c r="AI9" s="616"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="593" t="s">
+      <c r="AK9" s="616" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="272"/>
       <c r="AM9" s="480"/>
-      <c r="AN9" s="604"/>
+      <c r="AN9" s="602"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -8039,13 +8065,13 @@
       <c r="D10" s="142"/>
       <c r="E10" s="250">
         <f>Boat!S8</f>
-        <v>42</v>
-      </c>
-      <c r="F10" s="585"/>
+        <v>40</v>
+      </c>
+      <c r="F10" s="607"/>
       <c r="N10" s="470" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="587" t="s">
+      <c r="O10" s="640" t="s">
         <v>103</v>
       </c>
       <c r="P10" s="613" t="s">
@@ -8054,7 +8080,7 @@
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="598"/>
+      <c r="S10" s="627"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8066,7 +8092,7 @@
       <c r="X10" s="483" t="s">
         <v>165</v>
       </c>
-      <c r="Y10" s="619"/>
+      <c r="Y10" s="620"/>
       <c r="Z10" s="461">
         <v>0</v>
       </c>
@@ -8084,16 +8110,16 @@
       <c r="AF10" s="251" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="594"/>
+      <c r="AG10" s="622"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="593"/>
+      <c r="AI10" s="616"/>
       <c r="AJ10" s="272"/>
-      <c r="AK10" s="593"/>
+      <c r="AK10" s="616"/>
       <c r="AL10" s="272"/>
       <c r="AM10" s="494" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="604"/>
+      <c r="AN10" s="602"/>
       <c r="AO10" s="214" t="s">
         <v>95</v>
       </c>
@@ -8102,7 +8128,7 @@
       <c r="A11" s="236" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="532" t="s">
+      <c r="B11" s="533" t="s">
         <v>288</v>
       </c>
       <c r="C11" s="509" t="s">
@@ -8111,18 +8137,18 @@
       <c r="D11" s="175" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="585"/>
+      <c r="F11" s="607"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="588"/>
+      <c r="O11" s="641"/>
       <c r="P11" s="614"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="598"/>
+      <c r="S11" s="627"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8132,7 +8158,7 @@
       <c r="X11" s="483" t="s">
         <v>166</v>
       </c>
-      <c r="Y11" s="619"/>
+      <c r="Y11" s="620"/>
       <c r="Z11" s="461"/>
       <c r="AA11" s="325">
         <v>1</v>
@@ -8146,14 +8172,14 @@
       <c r="AF11" s="272" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="594"/>
+      <c r="AG11" s="622"/>
       <c r="AH11" s="272"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="272"/>
       <c r="AK11" s="272"/>
       <c r="AL11" s="272"/>
       <c r="AM11" s="480"/>
-      <c r="AN11" s="604"/>
+      <c r="AN11" s="602"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -8162,7 +8188,7 @@
       <c r="A12" s="240" t="s">
         <v>393</v>
       </c>
-      <c r="B12" s="534"/>
+      <c r="B12" s="535"/>
       <c r="C12" s="510" t="s">
         <v>394</v>
       </c>
@@ -8172,25 +8198,25 @@
       <c r="E12" s="237">
         <v>3</v>
       </c>
-      <c r="F12" s="585"/>
+      <c r="F12" s="607"/>
       <c r="G12" s="374" t="s">
         <v>411</v>
       </c>
-      <c r="H12" s="537" t="s">
+      <c r="H12" s="538" t="s">
         <v>447</v>
       </c>
-      <c r="I12" s="538"/>
-      <c r="J12" s="538"/>
-      <c r="K12" s="592"/>
+      <c r="I12" s="539"/>
+      <c r="J12" s="539"/>
+      <c r="K12" s="645"/>
       <c r="L12" s="213"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
-      <c r="O12" s="588"/>
+      <c r="O12" s="641"/>
       <c r="P12" s="614"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="599"/>
+      <c r="S12" s="624"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8200,7 +8226,7 @@
       <c r="X12" s="483" t="s">
         <v>167</v>
       </c>
-      <c r="Y12" s="619"/>
+      <c r="Y12" s="620"/>
       <c r="Z12" s="459">
         <v>1</v>
       </c>
@@ -8211,16 +8237,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="602" t="s">
+      <c r="AD12" s="630" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="493" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="594" t="s">
+      <c r="AF12" s="622" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="594"/>
+      <c r="AG12" s="622"/>
       <c r="AH12" s="251" t="s">
         <v>264</v>
       </c>
@@ -8230,10 +8256,10 @@
       <c r="AJ12" s="272"/>
       <c r="AK12" s="272"/>
       <c r="AL12" s="272"/>
-      <c r="AM12" s="616" t="s">
+      <c r="AM12" s="617" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="604"/>
+      <c r="AN12" s="602"/>
       <c r="AO12" s="375" t="s">
         <v>97</v>
       </c>
@@ -8245,16 +8271,16 @@
       <c r="E13" s="500">
         <v>-3</v>
       </c>
-      <c r="F13" s="585"/>
-      <c r="G13" s="538" t="s">
+      <c r="F13" s="607"/>
+      <c r="G13" s="539" t="s">
         <v>448</v>
       </c>
-      <c r="H13" s="538"/>
-      <c r="I13" s="538"/>
-      <c r="J13" s="592"/>
+      <c r="H13" s="539"/>
+      <c r="I13" s="539"/>
+      <c r="J13" s="645"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="588"/>
+      <c r="O13" s="641"/>
       <c r="P13" s="615"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
@@ -8265,7 +8291,7 @@
       <c r="X13" s="483" t="s">
         <v>168</v>
       </c>
-      <c r="Y13" s="619"/>
+      <c r="Y13" s="620"/>
       <c r="Z13" s="459">
         <v>1</v>
       </c>
@@ -8276,8 +8302,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="602"/>
-      <c r="AF13" s="594"/>
+      <c r="AD13" s="630"/>
+      <c r="AF13" s="622"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="251" t="s">
         <v>314</v>
@@ -8288,8 +8314,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="272"/>
       <c r="AL13" s="272"/>
-      <c r="AM13" s="616"/>
-      <c r="AN13" s="604"/>
+      <c r="AM13" s="617"/>
+      <c r="AN13" s="602"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="502"/>
@@ -8297,18 +8323,18 @@
       <c r="C14" s="511"/>
       <c r="D14" s="504"/>
       <c r="E14" s="505"/>
-      <c r="F14" s="585"/>
-      <c r="G14" s="538" t="s">
+      <c r="F14" s="607"/>
+      <c r="G14" s="539" t="s">
         <v>447</v>
       </c>
-      <c r="H14" s="538"/>
-      <c r="I14" s="538"/>
-      <c r="J14" s="592"/>
+      <c r="H14" s="539"/>
+      <c r="I14" s="539"/>
+      <c r="J14" s="645"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="588"/>
+      <c r="O14" s="641"/>
       <c r="Q14" s="61" t="s">
         <v>559</v>
       </c>
@@ -8322,34 +8348,34 @@
       <c r="X14" s="483" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="619"/>
+      <c r="Y14" s="620"/>
       <c r="Z14" s="459">
         <v>1</v>
       </c>
       <c r="AA14" s="325"/>
       <c r="AB14" s="219"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="602"/>
+      <c r="AD14" s="630"/>
       <c r="AE14" s="272"/>
-      <c r="AF14" s="594"/>
+      <c r="AF14" s="622"/>
       <c r="AG14" s="272"/>
       <c r="AH14" s="272"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="272"/>
       <c r="AK14" s="272"/>
       <c r="AL14" s="272"/>
-      <c r="AM14" s="616"/>
-      <c r="AN14" s="604"/>
+      <c r="AM14" s="617"/>
+      <c r="AN14" s="602"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="501" t="s">
         <v>525</v>
       </c>
-      <c r="C15" s="532" t="s">
+      <c r="C15" s="533" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="585"/>
-      <c r="O15" s="588"/>
+      <c r="F15" s="607"/>
+      <c r="O15" s="641"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8362,7 +8388,7 @@
       <c r="X15" s="483" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="619"/>
+      <c r="Y15" s="620"/>
       <c r="Z15" s="461">
         <v>1</v>
       </c>
@@ -8371,8 +8397,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="602"/>
-      <c r="AF15" s="594"/>
+      <c r="AD15" s="630"/>
+      <c r="AF15" s="622"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="251" t="s">
         <v>466</v>
@@ -8385,8 +8411,8 @@
       </c>
       <c r="AK15" s="272"/>
       <c r="AL15" s="272"/>
-      <c r="AM15" s="616"/>
-      <c r="AN15" s="604"/>
+      <c r="AM15" s="617"/>
+      <c r="AN15" s="602"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8401,20 +8427,20 @@
       <c r="B16" s="21" t="s">
         <v>417</v>
       </c>
-      <c r="C16" s="534"/>
+      <c r="C16" s="535"/>
       <c r="D16" s="61" t="s">
         <v>511</v>
       </c>
       <c r="E16" s="237">
         <v>1</v>
       </c>
-      <c r="F16" s="585"/>
+      <c r="F16" s="607"/>
       <c r="G16" s="374" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="588"/>
+      <c r="O16" s="641"/>
       <c r="R16" s="487" t="s">
         <v>185</v>
       </c>
@@ -8425,7 +8451,7 @@
       <c r="X16" s="483" t="s">
         <v>171</v>
       </c>
-      <c r="Y16" s="619"/>
+      <c r="Y16" s="620"/>
       <c r="Z16" s="459">
         <v>1</v>
       </c>
@@ -8446,18 +8472,18 @@
       <c r="AM16" s="480" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="604"/>
+      <c r="AN16" s="602"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="585"/>
+      <c r="F17" s="607"/>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="588"/>
+      <c r="O17" s="641"/>
       <c r="Q17" s="21" t="s">
         <v>557</v>
       </c>
@@ -8477,7 +8503,7 @@
       <c r="X17" s="483" t="s">
         <v>172</v>
       </c>
-      <c r="Y17" s="619"/>
+      <c r="Y17" s="620"/>
       <c r="Z17" s="461"/>
       <c r="AA17" s="325"/>
       <c r="AB17" s="219"/>
@@ -8502,7 +8528,7 @@
       <c r="AK17" s="272"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="480"/>
-      <c r="AN17" s="604"/>
+      <c r="AN17" s="602"/>
       <c r="AO17" s="214" t="s">
         <v>516</v>
       </c>
@@ -8526,21 +8552,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="585"/>
+      <c r="F18" s="607"/>
       <c r="G18" s="374" t="s">
         <v>554</v>
       </c>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="588"/>
+      <c r="O18" s="641"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="580" t="s">
+      <c r="R18" s="635" t="s">
         <v>562</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="624" t="s">
+      <c r="U18" s="580" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8550,7 +8576,7 @@
       <c r="X18" s="483" t="s">
         <v>173</v>
       </c>
-      <c r="Y18" s="619"/>
+      <c r="Y18" s="620"/>
       <c r="Z18" s="461">
         <v>1</v>
       </c>
@@ -8561,37 +8587,37 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="272"/>
-      <c r="AF18" s="593" t="s">
+      <c r="AF18" s="616" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="272"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="617" t="s">
+      <c r="AJ18" s="618" t="s">
         <v>322</v>
       </c>
       <c r="AK18" s="272"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="480"/>
-      <c r="AN18" s="604"/>
+      <c r="AN18" s="602"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="585"/>
-      <c r="O19" s="588"/>
-      <c r="R19" s="581"/>
+      <c r="F19" s="607"/>
+      <c r="O19" s="641"/>
+      <c r="R19" s="636"/>
       <c r="S19" s="30" t="s">
         <v>560</v>
       </c>
-      <c r="U19" s="625"/>
+      <c r="U19" s="581"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="483" t="s">
         <v>174</v>
       </c>
-      <c r="Y19" s="619"/>
+      <c r="Y19" s="620"/>
       <c r="Z19" s="459">
         <v>1</v>
       </c>
@@ -8600,17 +8626,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="272"/>
-      <c r="AF19" s="593"/>
+      <c r="AF19" s="616"/>
       <c r="AG19" s="272"/>
       <c r="AH19" s="272"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="617"/>
+      <c r="AJ19" s="618"/>
       <c r="AK19" s="512" t="s">
         <v>256</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="480"/>
-      <c r="AN19" s="604"/>
+      <c r="AN19" s="602"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8631,23 +8657,23 @@
       <c r="E20" s="489">
         <v>-1</v>
       </c>
-      <c r="F20" s="585"/>
+      <c r="F20" s="607"/>
       <c r="G20" s="374" t="s">
         <v>509</v>
       </c>
-      <c r="O20" s="588"/>
-      <c r="Q20" s="590" t="s">
+      <c r="O20" s="641"/>
+      <c r="Q20" s="643" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="456" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="626"/>
+      <c r="U20" s="582"/>
       <c r="W20" s="457"/>
       <c r="X20" s="484" t="s">
         <v>175</v>
       </c>
-      <c r="Y20" s="619"/>
+      <c r="Y20" s="620"/>
       <c r="Z20" s="463">
         <v>1</v>
       </c>
@@ -8672,7 +8698,7 @@
       <c r="AM20" s="427" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="604"/>
+      <c r="AN20" s="602"/>
       <c r="AO20" s="375" t="s">
         <v>478</v>
       </c>
@@ -8696,19 +8722,19 @@
       <c r="E21" s="281">
         <v>1</v>
       </c>
-      <c r="F21" s="585"/>
-      <c r="O21" s="588"/>
-      <c r="Q21" s="591"/>
+      <c r="F21" s="607"/>
+      <c r="O21" s="641"/>
+      <c r="Q21" s="644"/>
       <c r="T21" s="474"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="621"/>
+      <c r="V21" s="577"/>
       <c r="W21" s="478" t="s">
         <v>176</v>
       </c>
       <c r="X21" s="481" t="s">
         <v>187</v>
       </c>
-      <c r="Y21" s="619"/>
+      <c r="Y21" s="620"/>
       <c r="Z21" s="497">
         <v>3</v>
       </c>
@@ -8739,14 +8765,14 @@
       <c r="AM21" s="480" t="s">
         <v>572</v>
       </c>
-      <c r="AN21" s="604"/>
+      <c r="AN21" s="602"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="585"/>
+      <c r="F22" s="607"/>
       <c r="G22" s="374" t="s">
         <v>507</v>
       </c>
-      <c r="O22" s="588"/>
+      <c r="O22" s="641"/>
       <c r="R22" s="486" t="s">
         <v>44</v>
       </c>
@@ -8754,14 +8780,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="622"/>
+      <c r="V22" s="578"/>
       <c r="W22" s="478" t="s">
         <v>176</v>
       </c>
       <c r="X22" s="481" t="s">
         <v>188</v>
       </c>
-      <c r="Y22" s="619"/>
+      <c r="Y22" s="620"/>
       <c r="Z22" s="467"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="467"/>
@@ -8772,7 +8798,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="593" t="s">
+      <c r="AJ22" s="616" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="272"/>
@@ -8780,7 +8806,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="318"/>
-      <c r="AN22" s="604"/>
+      <c r="AN22" s="602"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="244" t="s">
@@ -8798,21 +8824,21 @@
       <c r="E23" s="238">
         <v>1</v>
       </c>
-      <c r="F23" s="585"/>
-      <c r="O23" s="588"/>
-      <c r="Q23" s="590" t="s">
+      <c r="F23" s="607"/>
+      <c r="O23" s="641"/>
+      <c r="Q23" s="643" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="472" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="622"/>
+      <c r="V23" s="578"/>
       <c r="W23" s="148"/>
       <c r="X23" s="481" t="s">
         <v>189</v>
       </c>
-      <c r="Y23" s="619"/>
+      <c r="Y23" s="620"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="467"/>
@@ -8823,13 +8849,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="593"/>
+      <c r="AJ23" s="616"/>
       <c r="AK23" s="272"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="318"/>
-      <c r="AN23" s="604"/>
+      <c r="AN23" s="602"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="492" t="s">
@@ -8847,22 +8873,22 @@
       <c r="E24" s="488">
         <v>1</v>
       </c>
-      <c r="F24" s="585"/>
+      <c r="F24" s="607"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
-      <c r="O24" s="588"/>
-      <c r="Q24" s="591"/>
+      <c r="O24" s="641"/>
+      <c r="Q24" s="644"/>
       <c r="T24" s="17"/>
       <c r="U24" s="240" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="622"/>
+      <c r="V24" s="578"/>
       <c r="W24" s="148"/>
       <c r="X24" s="481" t="s">
         <v>186</v>
       </c>
-      <c r="Y24" s="619"/>
+      <c r="Y24" s="620"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="467"/>
@@ -8881,11 +8907,11 @@
         <v>481</v>
       </c>
       <c r="AM24" s="318"/>
-      <c r="AN24" s="604"/>
+      <c r="AN24" s="602"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="585"/>
-      <c r="O25" s="588"/>
+      <c r="F25" s="607"/>
+      <c r="O25" s="641"/>
       <c r="P25" s="214" t="s">
         <v>285</v>
       </c>
@@ -8898,12 +8924,12 @@
       <c r="U25" s="452" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="623"/>
+      <c r="V25" s="579"/>
       <c r="W25" s="148"/>
       <c r="X25" s="481" t="s">
         <v>190</v>
       </c>
-      <c r="Y25" s="619"/>
+      <c r="Y25" s="620"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="467"/>
@@ -8920,7 +8946,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="318"/>
-      <c r="AN25" s="604"/>
+      <c r="AN25" s="602"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="244" t="s">
@@ -8938,16 +8964,16 @@
       <c r="E26" s="424">
         <v>1</v>
       </c>
-      <c r="F26" s="585"/>
+      <c r="F26" s="607"/>
       <c r="G26" s="374" t="s">
         <v>505</v>
       </c>
-      <c r="O26" s="588"/>
-      <c r="P26" s="606" t="s">
+      <c r="O26" s="641"/>
+      <c r="P26" s="604" t="s">
         <v>549</v>
       </c>
-      <c r="Q26" s="607"/>
-      <c r="R26" s="582" t="s">
+      <c r="Q26" s="605"/>
+      <c r="R26" s="637" t="s">
         <v>561</v>
       </c>
       <c r="T26" s="183"/>
@@ -8959,7 +8985,7 @@
       <c r="X26" s="481" t="s">
         <v>182</v>
       </c>
-      <c r="Y26" s="619"/>
+      <c r="Y26" s="620"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="467"/>
@@ -8986,7 +9012,7 @@
       <c r="AM26" s="494" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="604"/>
+      <c r="AN26" s="602"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8998,12 +9024,12 @@
       <c r="E27" s="281" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="586"/>
+      <c r="F27" s="639"/>
       <c r="G27" s="61" t="s">
         <v>571</v>
       </c>
-      <c r="O27" s="589"/>
-      <c r="R27" s="583"/>
+      <c r="O27" s="642"/>
+      <c r="R27" s="638"/>
       <c r="S27" s="473" t="s">
         <v>54</v>
       </c>
@@ -9016,7 +9042,7 @@
       <c r="X27" s="481" t="s">
         <v>556</v>
       </c>
-      <c r="Y27" s="620"/>
+      <c r="Y27" s="621"/>
       <c r="Z27" s="163"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="468"/>
@@ -9033,10 +9059,48 @@
       <c r="AM27" s="427" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="605"/>
+      <c r="AN27" s="603"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -9053,44 +9117,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9100,8 +9126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P18" workbookViewId="0">
-      <selection activeCell="AM20" sqref="AM20"/>
+    <sheetView topLeftCell="P9" workbookViewId="0">
+      <selection activeCell="AL27" sqref="AL27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9188,16 +9214,16 @@
       <c r="Q1" s="142"/>
       <c r="R1" s="142"/>
       <c r="S1" s="6"/>
-      <c r="T1" s="572" t="s">
+      <c r="T1" s="563" t="s">
         <v>236</v>
       </c>
-      <c r="U1" s="649" t="s">
+      <c r="U1" s="661" t="s">
         <v>237</v>
       </c>
-      <c r="V1" s="651" t="s">
+      <c r="V1" s="663" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="652"/>
+      <c r="W1" s="664"/>
       <c r="X1" s="324">
         <f>68-(S8+W3+V3+Q3)</f>
         <v>0</v>
@@ -9213,42 +9239,42 @@
       <c r="AB1" s="320" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="653" t="s">
+      <c r="AC1" s="665" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="654"/>
-      <c r="AE1" s="655"/>
-      <c r="AF1" s="656" t="s">
+      <c r="AD1" s="666"/>
+      <c r="AE1" s="667"/>
+      <c r="AF1" s="668" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="657"/>
-      <c r="AH1" s="658"/>
-      <c r="AI1" s="645" t="s">
+      <c r="AG1" s="669"/>
+      <c r="AH1" s="670"/>
+      <c r="AI1" s="657" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="646"/>
-      <c r="AK1" s="647"/>
+      <c r="AJ1" s="658"/>
+      <c r="AK1" s="659"/>
       <c r="AN1" s="112"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="659">
+      <c r="J2" s="649">
         <f>SUM(J5:J30)</f>
         <v>2</v>
       </c>
-      <c r="K2" s="661">
+      <c r="K2" s="651">
         <f>SUM(K4:K29)</f>
-        <v>5</v>
-      </c>
-      <c r="L2" s="663">
+        <v>7</v>
+      </c>
+      <c r="L2" s="653">
         <f>SUM(L4:L29)</f>
         <v>7</v>
       </c>
-      <c r="M2" s="600">
+      <c r="M2" s="628">
         <f>SUM(K30:K37)* (-1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2" s="285" t="s">
         <v>243</v>
@@ -9265,11 +9291,11 @@
       <c r="R2" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="S2" s="665" t="s">
+      <c r="S2" s="655" t="s">
         <v>239</v>
       </c>
-      <c r="T2" s="648"/>
-      <c r="U2" s="650"/>
+      <c r="T2" s="660"/>
+      <c r="U2" s="662"/>
       <c r="V2" s="61" t="s">
         <v>456</v>
       </c>
@@ -9329,10 +9355,10 @@
       </c>
     </row>
     <row r="3" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J3" s="660"/>
-      <c r="K3" s="662"/>
-      <c r="L3" s="664"/>
-      <c r="M3" s="601"/>
+      <c r="J3" s="650"/>
+      <c r="K3" s="652"/>
+      <c r="L3" s="654"/>
+      <c r="M3" s="629"/>
       <c r="N3" s="177">
         <f>(J2+K2)-W3</f>
         <v>0</v>
@@ -9346,10 +9372,10 @@
       </c>
       <c r="R3" s="159">
         <f>SUM(R4:R29)</f>
-        <v>42</v>
-      </c>
-      <c r="S3" s="666"/>
-      <c r="T3" s="573"/>
+        <v>40</v>
+      </c>
+      <c r="S3" s="656"/>
+      <c r="T3" s="564"/>
       <c r="U3" s="331">
         <f>R3+V3+W3+Q3</f>
         <v>68</v>
@@ -9360,7 +9386,7 @@
       </c>
       <c r="W3" s="187">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9372,7 +9398,7 @@
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
@@ -9450,7 +9476,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="667" t="s">
+      <c r="M4" s="646" t="s">
         <v>200</v>
       </c>
       <c r="N4" s="20"/>
@@ -9533,7 +9559,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="668"/>
+      <c r="M5" s="647"/>
       <c r="N5" s="20"/>
       <c r="O5" s="2" t="s">
         <v>347</v>
@@ -9621,7 +9647,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="668"/>
+      <c r="M6" s="647"/>
       <c r="N6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9711,7 +9737,7 @@
         <f t="shared" ref="L7:L37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="M7" s="668"/>
+      <c r="M7" s="647"/>
       <c r="N7" s="20"/>
       <c r="O7" s="2" t="s">
         <v>342</v>
@@ -9815,7 +9841,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M8" s="668"/>
+      <c r="M8" s="647"/>
       <c r="N8" s="21" t="s">
         <v>238</v>
       </c>
@@ -9833,7 +9859,7 @@
       </c>
       <c r="S8" s="340">
         <f>R3</f>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="T8" s="17"/>
       <c r="U8" s="348"/>
@@ -9901,7 +9927,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M9" s="668"/>
+      <c r="M9" s="647"/>
       <c r="N9" s="21" t="s">
         <v>342</v>
       </c>
@@ -9993,13 +10019,13 @@
       </c>
       <c r="J10" s="363"/>
       <c r="K10" s="107">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="311">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M10" s="668"/>
+      <c r="M10" s="647"/>
       <c r="N10" s="20"/>
       <c r="O10" s="2" t="s">
         <v>347</v>
@@ -10011,7 +10037,7 @@
         <v>1</v>
       </c>
       <c r="R10" s="157">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" s="338">
         <v>-2</v>
@@ -10021,7 +10047,7 @@
       <c r="V10" s="346"/>
       <c r="W10" s="190">
         <f>SUM(J10:K10)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X10" s="314"/>
       <c r="Y10" s="117">
@@ -10030,7 +10056,7 @@
       </c>
       <c r="Z10" s="308">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA10" s="308">
         <v>1</v>
@@ -10062,9 +10088,13 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="AL10" s="6"/>
+      <c r="AL10" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="AM10" s="231"/>
-      <c r="AN10" s="80"/>
+      <c r="AN10" s="80" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="11" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I11" s="430" t="s">
@@ -10078,7 +10108,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M11" s="668"/>
+      <c r="M11" s="647"/>
       <c r="N11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10140,7 +10170,7 @@
       <c r="AN11" s="112"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="636" t="s">
+      <c r="A12" s="592" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10149,7 +10179,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="590" t="s">
+      <c r="E12" s="643" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="277">
@@ -10169,7 +10199,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M12" s="668"/>
+      <c r="M12" s="647"/>
       <c r="N12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10243,14 +10273,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="638"/>
+      <c r="A13" s="594"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="591"/>
+      <c r="E13" s="644"/>
       <c r="F13" s="177">
         <v>0</v>
       </c>
@@ -10271,7 +10301,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M13" s="668"/>
+      <c r="M13" s="647"/>
       <c r="N13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10346,7 +10376,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M14" s="668"/>
+      <c r="M14" s="647"/>
       <c r="N14" s="20"/>
       <c r="O14" s="210" t="s">
         <v>346</v>
@@ -10443,7 +10473,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M15" s="668"/>
+      <c r="M15" s="647"/>
       <c r="N15" s="20"/>
       <c r="O15" s="210" t="s">
         <v>346</v>
@@ -10528,7 +10558,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M16" s="668"/>
+      <c r="M16" s="647"/>
       <c r="N16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10624,7 +10654,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M17" s="668"/>
+      <c r="M17" s="647"/>
       <c r="N17" s="20"/>
       <c r="O17" s="2" t="s">
         <v>348</v>
@@ -10707,7 +10737,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M18" s="668"/>
+      <c r="M18" s="647"/>
       <c r="N18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10792,7 +10822,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M19" s="668"/>
+      <c r="M19" s="647"/>
       <c r="N19" s="20"/>
       <c r="O19" s="2" t="s">
         <v>341</v>
@@ -10887,11 +10917,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M20" s="669"/>
-      <c r="N20" s="537" t="s">
+      <c r="M20" s="648"/>
+      <c r="N20" s="538" t="s">
         <v>342</v>
       </c>
-      <c r="O20" s="592"/>
+      <c r="O20" s="645"/>
       <c r="P20" s="334" t="s">
         <v>86</v>
       </c>
@@ -11138,7 +11168,7 @@
       <c r="AN22" s="112"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="643" t="s">
+      <c r="E23" s="599" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="185">
@@ -11224,7 +11254,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="644"/>
+      <c r="E24" s="600"/>
       <c r="F24" s="177"/>
       <c r="I24" s="430" t="s">
         <v>301</v>
@@ -11233,16 +11263,16 @@
         <v>0</v>
       </c>
       <c r="K24" s="107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="311">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="N24" s="537" t="s">
+      <c r="N24" s="538" t="s">
         <v>342</v>
       </c>
-      <c r="O24" s="592"/>
+      <c r="O24" s="645"/>
       <c r="P24" s="334" t="s">
         <v>254</v>
       </c>
@@ -11250,7 +11280,7 @@
         <v>2</v>
       </c>
       <c r="R24" s="157">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S24" s="338">
         <v>-2</v>
@@ -11262,7 +11292,7 @@
       <c r="V24" s="345"/>
       <c r="W24" s="190">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X24" s="314"/>
       <c r="Y24" s="117">
@@ -11271,7 +11301,7 @@
       </c>
       <c r="Z24" s="308">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA24" s="308">
         <v>1</v>
@@ -12176,7 +12206,7 @@
       </c>
       <c r="J36" s="370"/>
       <c r="K36" s="264">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" s="311">
         <f t="shared" si="10"/>
@@ -12190,7 +12220,7 @@
         <v>1</v>
       </c>
       <c r="R36" s="268">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S36" s="18">
         <v>-1</v>
@@ -12200,7 +12230,7 @@
       <c r="V36" s="64"/>
       <c r="W36" s="190">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X36" s="65"/>
       <c r="Y36" s="117">
@@ -12209,7 +12239,7 @@
       </c>
       <c r="Z36" s="64">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA36" s="64"/>
       <c r="AB36" s="319">
@@ -12236,7 +12266,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AL36" s="6"/>
+      <c r="AL36" s="6" t="s">
+        <v>313</v>
+      </c>
       <c r="AN36" s="112"/>
     </row>
     <row r="37" spans="3:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12324,23 +12356,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="S2:S3"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="N20:O20"/>
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="N24:O24"/>
     <mergeCell ref="M4:M20"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12374,15 +12406,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="537" t="s">
+      <c r="B1" s="538" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="592"/>
+      <c r="C1" s="645"/>
       <c r="D1" s="214"/>
-      <c r="J1" s="537" t="s">
+      <c r="J1" s="538" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="592"/>
+      <c r="K1" s="645"/>
       <c r="L1" s="205" t="s">
         <v>337</v>
       </c>
@@ -12420,13 +12452,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="206"/>
-      <c r="M2" s="670"/>
+      <c r="M2" s="671"/>
       <c r="N2" s="154">
         <v>2</v>
       </c>
       <c r="O2" s="155"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="673" t="s">
+      <c r="Q2" s="674" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="19">
@@ -12449,13 +12481,13 @@
       <c r="K3" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="M3" s="671"/>
+      <c r="M3" s="672"/>
       <c r="N3" s="17">
         <v>1</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="674"/>
+      <c r="Q3" s="675"/>
       <c r="R3" s="231"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12474,13 +12506,13 @@
       <c r="K4" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="M4" s="671"/>
+      <c r="M4" s="672"/>
       <c r="N4" s="17"/>
       <c r="O4" s="15">
         <v>1</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="674"/>
+      <c r="Q4" s="675"/>
       <c r="R4" s="231"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12500,13 +12532,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="206"/>
-      <c r="M5" s="671"/>
+      <c r="M5" s="672"/>
       <c r="N5" s="17">
         <v>1</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="674"/>
+      <c r="Q5" s="675"/>
       <c r="R5" s="19">
         <v>-1</v>
       </c>
@@ -12527,13 +12559,13 @@
       <c r="K6" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="M6" s="671"/>
+      <c r="M6" s="672"/>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="674"/>
+      <c r="Q6" s="675"/>
       <c r="R6" s="231"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12553,13 +12585,13 @@
         <v>334</v>
       </c>
       <c r="L7" s="208"/>
-      <c r="M7" s="671"/>
+      <c r="M7" s="672"/>
       <c r="N7" s="17">
         <v>1</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="674"/>
+      <c r="Q7" s="675"/>
       <c r="R7" s="19">
         <v>-1</v>
       </c>
@@ -12580,13 +12612,13 @@
       <c r="K8" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="M8" s="671"/>
+      <c r="M8" s="672"/>
       <c r="N8" s="17">
         <v>1</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="674"/>
+      <c r="Q8" s="675"/>
       <c r="R8" s="231"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12606,13 +12638,13 @@
         <v>336</v>
       </c>
       <c r="L9" s="186"/>
-      <c r="M9" s="672"/>
+      <c r="M9" s="673"/>
       <c r="N9" s="163"/>
       <c r="O9" s="18"/>
       <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="675"/>
+      <c r="Q9" s="676"/>
       <c r="R9" s="232"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -12770,10 +12802,10 @@
         <f ca="1">TODAY()</f>
         <v>45277</v>
       </c>
-      <c r="V1" s="537" t="s">
+      <c r="V1" s="538" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="592"/>
+      <c r="W1" s="645"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12792,7 +12824,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="683" t="s">
+      <c r="AD1" s="691" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12809,10 +12841,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="682" t="s">
+      <c r="F2" s="722" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="710" t="s">
+      <c r="G2" s="679" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -12840,10 +12872,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="651" t="s">
+      <c r="V2" s="663" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="652"/>
+      <c r="W2" s="664"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -12862,7 +12894,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="684"/>
+      <c r="AD2" s="692"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -12881,8 +12913,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="640"/>
-      <c r="G3" s="711"/>
+      <c r="F3" s="596"/>
+      <c r="G3" s="680"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -12893,13 +12925,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="720" t="s">
+      <c r="O3" s="689" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="702" t="s">
+      <c r="P3" s="710" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="703"/>
+      <c r="Q3" s="711"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -12909,15 +12941,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="684"/>
+      <c r="AD3" s="692"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="711"/>
+      <c r="G4" s="680"/>
       <c r="H4" s="6"/>
-      <c r="L4" s="673" t="s">
+      <c r="L4" s="674" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="721"/>
+      <c r="O4" s="690"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -12927,12 +12959,12 @@
       <c r="X4" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="537" t="s">
+      <c r="Y4" s="538" t="s">
         <v>195</v>
       </c>
-      <c r="Z4" s="538"/>
-      <c r="AA4" s="592"/>
-      <c r="AD4" s="684"/>
+      <c r="Z4" s="539"/>
+      <c r="AA4" s="645"/>
+      <c r="AD4" s="692"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -12947,21 +12979,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="711"/>
+      <c r="G5" s="680"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="689" t="s">
+      <c r="K5" s="697" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="704"/>
+      <c r="L5" s="712"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="721"/>
+      <c r="O5" s="690"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -12977,11 +13009,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="692" t="s">
+      <c r="Y5" s="700" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="693"/>
-      <c r="AD5" s="684"/>
+      <c r="Z5" s="701"/>
+      <c r="AD5" s="692"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -12991,16 +13023,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="711"/>
+      <c r="G6" s="680"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="690"/>
-      <c r="L6" s="704"/>
-      <c r="O6" s="721"/>
+      <c r="K6" s="698"/>
+      <c r="L6" s="712"/>
+      <c r="O6" s="690"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13010,20 +13042,20 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="684"/>
+      <c r="AD6" s="692"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="711"/>
+      <c r="G7" s="680"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="690"/>
-      <c r="L7" s="704"/>
+      <c r="K7" s="698"/>
+      <c r="L7" s="712"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="721"/>
+      <c r="O7" s="690"/>
       <c r="P7" s="73"/>
-      <c r="AD7" s="684"/>
+      <c r="AD7" s="692"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13036,7 +13068,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="711"/>
+      <c r="G8" s="680"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13046,41 +13078,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="690"/>
-      <c r="L8" s="704"/>
-      <c r="O8" s="721"/>
+      <c r="K8" s="698"/>
+      <c r="L8" s="712"/>
+      <c r="O8" s="690"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="686" t="s">
+      <c r="S8" s="694" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="687"/>
-      <c r="U8" s="687"/>
-      <c r="V8" s="687"/>
-      <c r="W8" s="687"/>
-      <c r="X8" s="687"/>
-      <c r="Y8" s="687"/>
-      <c r="Z8" s="687"/>
-      <c r="AA8" s="687"/>
-      <c r="AB8" s="687"/>
-      <c r="AC8" s="688"/>
-      <c r="AD8" s="684"/>
+      <c r="T8" s="695"/>
+      <c r="U8" s="695"/>
+      <c r="V8" s="695"/>
+      <c r="W8" s="695"/>
+      <c r="X8" s="695"/>
+      <c r="Y8" s="695"/>
+      <c r="Z8" s="695"/>
+      <c r="AA8" s="695"/>
+      <c r="AB8" s="695"/>
+      <c r="AC8" s="696"/>
+      <c r="AD8" s="692"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="676"/>
-      <c r="G9" s="711"/>
+      <c r="C9" s="716"/>
+      <c r="G9" s="680"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="690"/>
-      <c r="L9" s="714" t="s">
+      <c r="K9" s="698"/>
+      <c r="L9" s="683" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="715"/>
-      <c r="N9" s="716"/>
-      <c r="O9" s="721"/>
+      <c r="M9" s="684"/>
+      <c r="N9" s="685"/>
+      <c r="O9" s="690"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="684"/>
+      <c r="AD9" s="692"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="677"/>
+      <c r="C10" s="717"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13088,7 +13120,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="711"/>
+      <c r="G10" s="680"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13096,33 +13128,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="690"/>
-      <c r="M10" s="679" t="s">
+      <c r="K10" s="698"/>
+      <c r="M10" s="719" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="680"/>
-      <c r="O10" s="680"/>
-      <c r="P10" s="680"/>
-      <c r="Q10" s="680"/>
-      <c r="R10" s="680"/>
-      <c r="S10" s="680"/>
-      <c r="T10" s="680"/>
-      <c r="U10" s="680"/>
-      <c r="V10" s="680"/>
-      <c r="W10" s="680"/>
-      <c r="X10" s="680"/>
-      <c r="Y10" s="680"/>
-      <c r="Z10" s="680"/>
-      <c r="AA10" s="680"/>
-      <c r="AB10" s="680"/>
-      <c r="AC10" s="681"/>
-      <c r="AD10" s="684"/>
+      <c r="N10" s="720"/>
+      <c r="O10" s="720"/>
+      <c r="P10" s="720"/>
+      <c r="Q10" s="720"/>
+      <c r="R10" s="720"/>
+      <c r="S10" s="720"/>
+      <c r="T10" s="720"/>
+      <c r="U10" s="720"/>
+      <c r="V10" s="720"/>
+      <c r="W10" s="720"/>
+      <c r="X10" s="720"/>
+      <c r="Y10" s="720"/>
+      <c r="Z10" s="720"/>
+      <c r="AA10" s="720"/>
+      <c r="AB10" s="720"/>
+      <c r="AC10" s="721"/>
+      <c r="AD10" s="692"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="678"/>
-      <c r="G11" s="711"/>
+      <c r="C11" s="718"/>
+      <c r="G11" s="680"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="690"/>
+      <c r="K11" s="698"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13133,17 +13165,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="700" t="s">
+      <c r="Z11" s="708" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="701"/>
+      <c r="AA11" s="709"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="684"/>
+      <c r="AD11" s="692"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13156,7 +13188,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="711"/>
+      <c r="G12" s="680"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13164,8 +13196,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="690"/>
-      <c r="L12" s="705" t="s">
+      <c r="K12" s="698"/>
+      <c r="L12" s="713" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13180,7 +13212,7 @@
       <c r="Q12" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="532" t="s">
+      <c r="S12" s="533" t="s">
         <v>107</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -13196,26 +13228,26 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="694" t="s">
+      <c r="AA12" s="702" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="695"/>
+      <c r="AB12" s="703"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="684"/>
+      <c r="AD12" s="692"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="676"/>
-      <c r="G13" s="711"/>
-      <c r="K13" s="690"/>
-      <c r="L13" s="706"/>
+      <c r="C13" s="716"/>
+      <c r="G13" s="680"/>
+      <c r="K13" s="698"/>
+      <c r="L13" s="714"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="713" t="s">
+      <c r="Q13" s="682" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="607"/>
-      <c r="S13" s="533"/>
+      <c r="R13" s="605"/>
+      <c r="S13" s="534"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
         <v>132</v>
@@ -13223,17 +13255,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="696"/>
-      <c r="AB13" s="697"/>
-      <c r="AD13" s="684"/>
+      <c r="AA13" s="704"/>
+      <c r="AB13" s="705"/>
+      <c r="AD13" s="692"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="678"/>
+      <c r="C14" s="718"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="711"/>
+      <c r="G14" s="680"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13241,8 +13273,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="690"/>
-      <c r="L14" s="706"/>
+      <c r="K14" s="698"/>
+      <c r="L14" s="714"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13252,7 +13284,7 @@
       <c r="R14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="533"/>
+      <c r="S14" s="534"/>
       <c r="T14" s="77" t="s">
         <v>130</v>
       </c>
@@ -13263,9 +13295,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="696"/>
-      <c r="AB14" s="697"/>
-      <c r="AD14" s="684"/>
+      <c r="AA14" s="704"/>
+      <c r="AB14" s="705"/>
+      <c r="AD14" s="692"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13280,20 +13312,20 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="711"/>
+      <c r="G15" s="680"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="690"/>
-      <c r="L15" s="707"/>
-      <c r="Q15" s="713" t="s">
+      <c r="K15" s="698"/>
+      <c r="L15" s="715"/>
+      <c r="Q15" s="682" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="607"/>
-      <c r="S15" s="533"/>
+      <c r="R15" s="605"/>
+      <c r="S15" s="534"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
         <v>44</v>
@@ -13301,14 +13333,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="696"/>
-      <c r="AB15" s="697"/>
-      <c r="AD15" s="684"/>
+      <c r="AA15" s="704"/>
+      <c r="AB15" s="705"/>
+      <c r="AD15" s="692"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="711"/>
-      <c r="K16" s="690"/>
+      <c r="G16" s="680"/>
+      <c r="K16" s="698"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13316,7 +13348,7 @@
       <c r="R16" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="533"/>
+      <c r="S16" s="534"/>
       <c r="T16" s="76" t="s">
         <v>129</v>
       </c>
@@ -13327,34 +13359,34 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="696"/>
-      <c r="AB16" s="697"/>
-      <c r="AD16" s="684"/>
+      <c r="AA16" s="704"/>
+      <c r="AB16" s="705"/>
+      <c r="AD16" s="692"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="708" t="s">
+      <c r="F17" s="677" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="711"/>
+      <c r="G17" s="680"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="690"/>
-      <c r="S17" s="533"/>
+      <c r="K17" s="698"/>
+      <c r="S17" s="534"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="696"/>
-      <c r="AB17" s="697"/>
-      <c r="AD17" s="684"/>
+      <c r="AA17" s="704"/>
+      <c r="AB17" s="705"/>
+      <c r="AD17" s="692"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13364,61 +13396,58 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="709"/>
-      <c r="G18" s="711"/>
+      <c r="F18" s="678"/>
+      <c r="G18" s="680"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="690"/>
+      <c r="K18" s="698"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="S18" s="533"/>
+      <c r="S18" s="534"/>
       <c r="U18" s="76" t="s">
         <v>133</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="698"/>
-      <c r="AB18" s="699"/>
-      <c r="AD18" s="684"/>
+      <c r="AA18" s="706"/>
+      <c r="AB18" s="707"/>
+      <c r="AD18" s="692"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="712"/>
-      <c r="K19" s="691"/>
+      <c r="G19" s="681"/>
+      <c r="K19" s="699"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="717" t="s">
+      <c r="R19" s="686" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="718"/>
-      <c r="T19" s="719"/>
+      <c r="S19" s="687"/>
+      <c r="T19" s="688"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="685"/>
+      <c r="AD19" s="693"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13430,11 +13459,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>